<commit_message>
updated for 2015 - 2019, ignored error 429...
</commit_message>
<xml_diff>
--- a/data_cleaning.xlsx
+++ b/data_cleaning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B178"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>URL</t>
+          <t>URLs</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -448,2130 +448,1464 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/bungalow-oei-tiong-ham-park-fetched-14-mil-profit</t>
+          <t>https://www.edgeprop.sg/property-news/freehold-properties-balestier-and-east-coast-sale</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">A former executive director of Kim Eng Holdings could be the seller of a detached house in Good-Class Bungalow (GCB) area Oei Tiong Ham Park, which fetched a profit of $14 million recently. The deal was among the new caveats uploaded by the URA on June 10 and 14. The bungalow, which sits on a 11,722 sq ft site, was first purchased in June 2006 at $4.9 million ($418 psf on a land area) and resold for $19 million ($1,621 psf) on June 6 this year. This translates to an annualised gain of 14%. The buyer is understood to be a partner of a renowned law firm Allen &amp; Gledhill. This marked the second most profitable deal in 2016. In February, a bungalow on Peirce Road, was sold for a $14.5 million profit.  A bungalow at Oei Tiong Ham Park was recently sold for a profit of $14 million  </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/buying-opportunities-balmoral-area</t>
+          <t>https://www.edgeprop.sg/property-news/gcb-dalvey-estate-sale-auction-30-mil</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Last December, listed property developer Hiap Hoe Ltd announced that its controlling shareholder Hiap Hoe Holdings, the investment firm of the Teo family, acquired all the shares in Hiap Hoe SuperBowl JV Pte Ltd which ownsTreasure on Balmoral, its 48-unit freeholdcondominiumblock. The sale worked out to $185 million or $1,789 psf for the development. This has had an impact on prices of neighbouring new condominiums launched in the Balmoral area, leading to transactions drying up for much of the first six months of the year. For example, next door to Treasure on Balmoral isThree Balmoral, a 40-unit freehold boutique condominium project by Tong Eng Group. The 12-storey project contains only one-bedroom-plus study units with sizes starting from 614 sq ft and three-bedroom units above 1,500 sq ft. Sales of Three Balmoral started in Oct 2011, and only seven of 20 units launched have been sold to date, according to URA data. The latest recorded sale was on June 15, for a 1,539 sq ft three-bedroom unit on the eighth floor that was sold for $3.4 million ($2,209 psf), according to URA Realis. The price psf is the lowest seen in the project to date as the earlier recorded transactions from Oct 2011 to April 2013 ranged from $2,388 psf to $2,608 psf, observes Ssamuel Eyo, managing director of Singapore Christies Homes. Hiap Hoe Ltd, which is a public listed company, was pressured to sell under the conditions of the Qualifying Certificate (QC) which requires all foreign companies (which includes listed companies) to sell all the units in their residential developments within two years of completion to avoid paying a penalty for any unsold units. The privately held Tong Eng Group on the other hand is not subject to the QC, and is therefore in no hurry to sell off the units. The group also has the holding power to ride through the current period of slow sales, adds Eyo. Located on the opposite side of the road from Three Balmoral is another freehold condominium by Tong Eng Group. CalledGoodwood Grand, the freehold project contains a condominium block of 65 units and eight stratabungalows. The project was launched for sale in December 2013. Of 31 units released, 26 units have been sold, with the latest transaction recorded in May at a median price of $2,563 psf, according to URA data. Likewise, Goodwood Grands price level is also being affected by another listed group, GuocoLand, which has been selling the remaining units at its 210-unitGoodwood Residencelocated off Bukit Timah Road. The project was completed in 2013, and the developer has sold 27 units, with three-bedroom units sized from 1,948 sq ft to 2,142 sq ft sold at prices ranging from $2,181 psf to $2,614 psf; and four-bedroom units from 2,454 sq ft to 2,928 sq ft offloaded at prices of $2,413 psf to $2,678 psf, based on caveats lodged with URA Realis from January to June 2015 to date. The price psf range of Goodwood Residence which is trading at $2,400 psf to $2,600 psf serves as a rough ballpark pricing for many of the newer developments with larger unit layouts of three- and four-bedroom types, notes Aldric Tan, senior associate director of CBRE Realty Associates. CBREs Tan attributes the lack of transactions for both Three Balmoral and Goodwood Grand to the absence of a proper showflat on site as construction of both projects are already well underway. Without a proper showflat, buyers cant visualise the unit layout and orientation, he explains. And people are more reluctant to commit to a purchase without seeing an actual showflat. If there are serious buyers, Tong Eng is willing to negotiate with them on pricing on a case-by-case basis and willing to offer discounts from 3% to 5%, notes CBREs Tan. On the opposite side of Balmoral Road diagonally opposite Goodwood Grand isBelmond Green, a 211-unit freehold condominium developed by CapitaLand and completed in 2004. The latest resale was for a 1,335 sq ft three-bedroom unit on the ninth floor that changed hands for $2.35 million ($1,723 psf), according to a caveat lodged on June 8. The unit last changed hands in 2006 for $1.3 million ($996 psf), hence the seller saw the price of the unit appreciate almost two fold in under a decade. According to CBREs Tan, Belmond Greens resale prices are affected by the recent transaction prices atHallmark Residences, a recently completed project located behind it on Ewe Boon Road. At Hallmark Residences, a 75-unit high-end condominium by MCL Land, the two latest transactions were for two ground floor units that were sold for $3.13 million ($1,773 psf) and $2.92 million ($1,739 psf). The lower price psf could be due to the private enclosed space of the ground floor units or the developer willing to shave off the price to clear the last few units, suggests Tan. As of end May, there were only three unsold units at Hallmark Residences, based on URA data. Meanwhile the lower price psf of Belmond Green - where four units had changed hands this year at prices ranging from $1,635 psf to $1,723 psf - may be proving attractive to buyers shopping in the resale market, notes Bruce Lye, managing partner of SRI5000, a division of SLP Realty. Belmond Green is not as old as some of the other developments in the area, for examplePalm Spring,Crystal TowerandEwe Boon Regentwhich were built in the 1970s to 1990s. So Belmond Green appears relatively new in comparison, he adds. On an a quantum basis, units at Belmond Green look more affordable compared to those of Hallmark Residences which are larger in size and have a higher price psf given that the project is new.  This article appeared in the City &amp; Country of Issue 683 (June 29) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/buying-vietnam%E2%80%99s-sizzling-market</t>
+          <t>https://www.edgeprop.sg/property-news/glimpse-eden-swire-properties%E2%80%99-first-ultra-luxury-condo-singapore</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Singaporean businessman and property investor Alvin Ong relocated with his family to Ho Chi Minh City in Vietnam in 2012. Ong, who is married to a Vietnamese citizen and a father of four, says, Its a slower pace of life. The same cannot be said of Vietnams property market, though. It has been sizzling since the government relaxed its foreign ownership rules in July 2015. There has been a lot of interest from overseas investors, especially those from Singapore, notes Ong. The appetite for Vietnamese projects was evident at CapitaLands and Keppel Lands weekend launches of their Ho Chi Minh City (HCMC) projects in Singapore in late-2015. Keppel Land sold more than 50 units in the second phase of the 719-unit The Estella over one weekend in late October. The following weekend, CapitaLand sold over 100 units in Singapore when it showcased two projects, the 1,152-unit Vista Verde and the 750-unit The Vista. Meanwhile, Singaporean serial entrepreneur and property investor Adam Khoo of the eponymous Adam Khoo Learning Centre reportedly scooped up 100 apartments at Diamond Lotus Lake View project in Tan Phu District, HCMC in December 2015. The 100 apartments Khoo purchased are equivalent to 10 floors in the project of more than 700 units, developed by Vietnamese developer Phuc Khang Corp. Prices at Diamond Lotus Lake View are said to start from VND678 million ($41,656 ) a unit. For that price, one cannot buy even an HDB flat in Singapore, nor the Certificate of Entitlement on a new car  only a four-year-old Ducati or a used Honda Civic. Source: Bloomberg With a young and entrepreneurial population driving consumer spending and GDP growth, Vietnam has one
-of the most vibrant economies in the region Very attractive yields And it is such price comparisons that are luring Singaporeans to invest in Vietnam. For $1 million, you can buy five to six high-end condos in Ho Chi Minh City, or up to 10 units in a mid-tier condo, says Ong. He and his wife have amassed a portfolio of more than five properties in Vietnam, primarily in Hanoi and HCMC. We buy condos in the city centre, or within 2km to 3km of the CBD, he adds. Prices have also escalated over the past three years. Ong bought a high-end condo for US$1,600 psm in HCMC in 2013. A month ago, a new high-end condo development located across the road was launched at US$2,500 psm. If I were to sell my unit today, I think I can easily fetch US$2,000 psm, says Ong. Currently, gross yields are at about 6% to 7%, which is considered very attractive for investors from Singapore and Taiwan, as yield is low in their home markets, observes Neil MacGregor, managing director of Savills Vietnam. Hence, these investors tend to focus on smaller units priced between US$150,000 and US$250,000, which can be easily leased out, and achieve higher yields, he says. Investments by Singaporean investors may not be as much as that by the mainland Chinese, but they are the leading investors in real estate in Vietnam to date, notes Marc Townsend of CBRE. Set to reap demographic dividend One of Vietnams biggest assets is its population of 95.2 million, of which more than half are aged between 15 and 39. They form the majority of the workforce. With a young and entrepreneurial population driving consumer spending and GDP growth, Vietnam has one of the most vibrant economies in the region, says Savills MacGregor, who has lived there since 2000. Vietnam is set to reap the benefits of this demographic dividend for the next 10 to 15 years, MacGregor notes. The rapidly growing middle class and the young population have also fuelled strong demand for affordable housing, with the sweet spot in the price range of US$40,000 to US$120,000, he adds. Recognising the demand, major real estate companies, especially local firms, have shifted their focus to low- to mid-tier residential developments. With a booming economy, Vietnam is attracting foreign investors who see untapped opportunities in a range of different sectors, says MacGregor. Boom in hospitality The hospitality sector is also entering a boom period, with strong demand for both city-centre hotels as well as resorts, says MacGregor. According to the General Statistics Office, Vietnam recorded 10.1 million international visitor arrivals in 2016, up 26% from a year ago. In 1Q2017, international visitors reached 3.2 million, a 29% increase over the same period last year, according to financial and investment advisory services firm AsiaInvest Group. The increase was said to be driven by visitors from other Asian countries, notably mainland Chinese, who accounted for almost 30% of the total number of arrivals. This was followed by visitors from South Korea, Japan, the US and Russia. Danang has seen particularly strong growth in recent years as tourism has boomed, supported by rapid growth in the number of direct flights from other cities across Asia, says MacGregor. With Danang hosting the Asia-Pacific Economic Cooperation (Apec) Summit this year, the profile of the city is likely to be raised. Nha Trang/Cam Ranh and Phu Quoc are the next destinations that will benefit from tourism growth, with the number of direct flights set to increase rapidly over the next three to five years, says MacGregor. In Haiphong, northern Vietnams busiest port, the economy is being driven by growth in manufacturing and logistics. MacGregor: Vietnam is set to reap the benefits of this demographic dividend for the next 10 to 15 years Manufacturing-led economy The manufacturing sector is fuelling household income and promises a sustained trade surplus in Vietnam, according to AsiaInvest. While GDP growth in 1Q2017 was estimated at 5.1%, according to the General Statistics Office, FocusEconomics panellists have forecast economic growth of 6.4% for Vietnam for the whole of 2017, and the same level of growth in 2018. The Nikkei manufacturing Purchasing Managers Index hit a 22-month high of 54.6 points in March. This resulted in 1Q2017 PMI data being the strongest quarter that we have seen since the survey began in early 2011, says IHS Markit economist Andrew Harker. This was coupled with a near-record increase in employment stemming from companies optimism that workload will continue to expand in the near term, he adds. It is even more remarkable considering that the Trans-Pacific Partnership, of which Vietnam was supposed to be a major beneficiary, has since been put on ice after the US pulled out. Instead, Vietnams economy has been bolstered by its other regional alliances, including the Asean Economic Community; Free Trade Agreements with the EU, Russia, South Korea, Chile; and the upcoming Regional Comprehensive Economic Partnership. In 1Q2017, Vietnam registered foreign direct investment of US$7.7 billion, up 77.6% y-o-y. About 85% of the FDI went to the manufacturing sector, and 4.4%, to real estate. The 4.4% FDI in real estate totalled US$343.7 million, representing a 34.4% increase from a year ago, according to the Ministry of Planning and Investment. The property sector, therefore, ranked second in terms of FDI inflows between January and March this year. The biggest FDI contributor to Vietnam in 1Q2017 was South Korea (US$3.75 billion), with Singapore in second place (US$911 million), followed by China (US$824 million), Taiwan (US$644 million) and Japan (US$452 million). Growth in retail Another sector that is booming is retail. During the first two months of 2017, Vietnams retail sales and service turnover grew 8.7% compared with the same period last year, says JLL in its Vietnam property market report on March 28. While supply of prime shopping centres in HCMC remained flat in 1Q2017, convenience stores  operated by domestic and foreign retailers  continued to expand citywide, JLL adds. Supply reached 199,350 sq m in total, and the overall occupancy rate rose to 92.2%. Likewise, in the capital city of Hanoi, total supply of prime shopping centres and retail space remained unchanged as no new projects were completed in 1Q2017. However, convenience stores saw rapid growth in the city, with supply reaching 47,500 sq m in total. A large volume of quality supply in retail space is projected to be completed over the next two years, says JLL. The retail market in Hanoi and HCMC is likely to see more local and foreign retailers expanding their footprint in good locations, according to the property consultancy. Record office occupancy There is also strong demand for quality office buildings in HCMC. The occupancy rate of Grade-A office space hit a record 95.6% in 1Q2017, while that for Grade-B office space stood at 91.8%, according to JLL. Total stock of Grade-A office space in HCMC was 192,179 sq m  just 23% of Grade-B stock (831,948 sq m) and 24.5% of Grade-C stock (785,037 sq m). In 1Q2017, average net rents in the Grade-A and Grade-B space in HCMC rose 0.4% q-o-q to US$38.7 and US$22 psm per month respectively, says JLL. Net absorption in Grade-A and Grade-B projects totalled 490 sq m and 41,087 sq m, respectively, with demand driven primarily by the financial services and IT sectors. Average rents of office space in non-CBD office projects rose at a faster clip  up 0.9% q-o-q in 1Q2017  with demand driven by newcomers in District 7, District 10 and Tan Binh District, says JLL. Office rents in HCMC are expected to continue their upward trend as supply will remain unchanged until 2H2017, notes JLL. The new office developments  Deutsches Haus and Saigon Centre Phase II  are scheduled to be completed in 3Q2017. Office supply is expected to soar only in 2019, as high-quality projects are expected to come on stream then, and mostly in the suburban areas, JLL says. In Hanoi, more than 130,000 sq m of Grade-B office space from five projects is expected to come on stream this year. However, there is no new supply of Grade-A office space this year. Two huge Grade-A office projects scheduled for completion in 2018/19 will add a total of 240,000 sq m of space to the market, says JLL. Demand for new and modern office space with a reasonable rent is expected to increase over the next quarters. Infrastructure boom Both Hanoi and HCMC have ambitious transport infrastructure programmes, according to Savills Vietnam Research. HCMC is expected to invest more than US$20 billion in infrastructure, including five planned elevated roads stretching 71km and five new metro lines of 106km. Similarly, Hanoi has eight metro lines of 260km and six elevated roads in the pipeline. The first metro line, scheduled to be fully operational by 2020, is expected to shift development focus. Living further from the city will become more appealing and cost-effective and shift the focus of investors away from the centre, says Savills in its report on urban transport. Properties near transit hubs can have significant capital appreciation: 10% in China and Thailand, and 32% in Hong Kong. The same pattern will arise in Vietnam. Building infrastructure has become critical as more people are buying cars in Vietnam, owing to decreased import duties within Asean and increased incomes. In the past five years, car sales grew 35% per annum and are expected to triple by 2025, according to Savills. Massive urbanisation is also taking place. Construction is happening everywhere  not just in HCMC, but Hanoi, Danang and across many other cities in Vietnam, according to CBRE. Acquiring land is a challenge As there is a limited amount of government land for public auction, the big local Vietnamese developers are turning to farmers to purchase big land parcels, notes CBREs Townsend. They are developing large townships that are likely to benefit from future infrastructure development, he adds. As the rules concerning buying government land are opaque, the biggest challenge for foreign developers is finding a greenfield site that is free and has a clean ownership title, says Savills MacGregor. Some developers may face issues such as having to buy a site from multiple shareholders. Others may have to deal with clearance and compensation of existing households on the site, which can be time-consuming, he notes. The Vietnam Association of Realtors recorded 18,340 transactions of land plots, residential and resort properties in 1Q2017, according to the breaking news on Vietnam on April 21. The figure is said to reflect both a q-o-q and y-o-y decline. The difficulty in securing land sites could have also led to a fall in the number of new apartments launched. In 1Q2017, 5,200 new apartments were available for sale in HCMC, a 47% contraction q-o-q. At the same time, total volume of transactions in 1Q2017 was 8,800 units, down 13% q-o-q. Savills forecasts that supply from 2Q2017 to 2019 will reach 62,200 in HCMC, with Districts 2 and 7 contributing the most  21% each. Source: VN REA NREA is also the bridge between enterprises and government authorities, and between Vietnam enterprises and the international business community, says Nguyen. VNREA members have played an important role in Vietnams booming property market, he adds. Foreign ownership concerns The biggest concern among individual foreign buyers of apartments is the withdrawal of their funds when they sell their property in the future, and also whether the 50-year lease is renewable, says MacGregor. Another major concern that surfaced recently is the issue of ownership certificates (or pink book) to foreigners.Tuoi Tre NewsandThe Straits Timesreported last month that the municipal land registration office in HCMC has stopped issuing ownership certificates to foreigners. Currently, foreign purchasers of CapitaLands projects, including Mulberry Lane in Hanoi, have received ownership certificates, says the developer. Thus, it is a matter of waiting for clear procedural guidelines from the upper level authorities, says CapitaLand in an email response to queries. The issue has not dented demand in Vietnams housing market, though. Nguyen Tran Nam, chairman of the Vietnam National Real Estate Association (VNREA) and former deputy minister of construction, expects more new launches in 2Q2017 and foresees higher sales volume than in the first quarter. VNREA is a non-profit organisation with 4,500 members across the country, many of whom are involved in the real estate sector  from developers and property consultants to investors and analysts. As an official representative of the real estate community, VNREA is also the bridge between enterprises and government authorities, and between Vietnam enterprises and the international business community, says Nguyen. VNREA members have played an important role in Vietnams booming property market, he adds. Meanwhile, Vietnam is seeing more millionaires who have made their money from trading property, says Savills MacGregor. It has happened all over the world. But the fact that Vietnam is still at a very early stage of development, it is possible to make a lot of money in a short space of time during the boom times. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/capitaland-announces-plans-560-mil-new-funan-mall</t>
+          <t>https://www.edgeprop.sg/property-news/global-citizen-global-investor</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CapitaLand Mall Trust has announced plans for a new $560 million mall to be called Funan, which will be built on the site of the former Funan DigitaLife Mall. CMT held the ground-breaking ceremony for Funan on Sept 7. Funan will have a total gross floor area (GFA) of 887,000 sq ft. Over half of the GFA, or 500,000 sq ft, will be in the six-storey retail component, which comprises four levels above ground and two basement levels. Funan will integrate online-to-offline (O2O) shopping experiences by offering the CBDs first drive-through click-and-collect and hands-free shopping service. Shoppers can choose to either pick up their purchases at Funans concierge when they are done, or have their shopping bags delivered to their homes. CapitaLands Funan Mall certainly sets a very high standard by embracing technology and lifestyle trends, says Christine Li, director of research at Cushman &amp; Wakefield. The landlord is thinking out of the box to reinvent itself in order to combat the trend of retailers moving from offline to online, she adds. In addition, three towers will sit above the retail component. They include two six-storey Grade A office towers from the fifth to 10th storey with a GFA of 266,000 sq ft. Another will be a nine-storey residential tower with 279 co-living serviced residences, from the fourth to 12th storey, with a GFA of 121,000 sq ft.  Artist's impression of Funan Source: CapitaLand Mall Trust</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/capri-fraser-sold-frasers-centrepoint-2034-mil</t>
+          <t>https://www.edgeprop.sg/property-news/good-value-city-fringe-living</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>The Capri by Fraser, a 313-room hotel-cum-serviced apartment development located within the Changi City integrated development, was sold to a unit of Frasers Centrepoint Ltd (FCL) for $203.4 million. The price translates into about $650,000 per room. The land on which The Capri by Fraser is situated has a lease term of 54 years left. The 12-storey property was sold by Ascendas Frasers Pte Ltd, a 50:50 joint venture between Ascendas Land and Frasers Centrepoint. The joint-venture partners had purchased the 4.7ha site for $150.8 million, or $119 psf per plot ratio (psf ppr) for the development of a mixed-use project in 2008. The Capri by Fraser is part of the integrated project, which includes a shopping mall and office block. The purchase price translates into a yield of 6%, says Donald Han, managing director of Chesterton Singapore. This article appeared in the City &amp; Country of Issue 669 (Mar 23) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/cascading-effect-highline-residences</t>
+          <t>https://www.edgeprop.sg/property-news/government-raises-development-charge-rates-non-landed-residential-sector</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Keppel Land held the preview of its 500-unitHighline Residenceson Kim Tian Road inTiong Bahrulast September. The preview saw 149 (93%) of 160 units released sold, according to URA data, with transaction prices ranging from US$1,627 psf to US$2,245 psf or at an average of about US$1,900 psf. Following the preview of the project, the showflat has since been closed. There are no plans to re-launch the project as yet, according to a source. Whether Keppel Land will adjust the selling prices of the 500-unit, 99-year leaseholdcondoon Kim Tian Road remains to be seen. After all, the developer paid a record US$550.8 million ($1,163 psf per plot ratio) for the site in April 2013. Property consultants like Nicholas Mak, executive director of research &amp; consultancy had estimated then that the breakeven cost for the project would be around US$1,700 psf to US$1,800 psf. Therefore Highline Residences selling prices are not expected to be lower than the average price of US$1,900 psf, according to a property agent. Whether it will be higher than the average of $1,900 psf achieved to date remains to be seen Highline Residences will therefore maintain the benchmark pricing for the Tiong Bahru area despite the current downbeat market conditions, says Tim Ong of ERA Realty. This could explain why there have been very few transactions in the Tiong Bahru area in the first six months of 2015 as some sellers of private condo units hold on to their asking prices. Some home sellers continue to have inflated price expectations, notes SLPs Mak. However, he cautions that this might not be the best strategy as homebuyers and tenants searching for a city fringe location within close proximity to an MRT station have many choices. In the current market, both buyers and tenants are price sensitive. Homebuyers also continue to face tighter loan restrictions and uncertainty about what lies ahead in terms of the property measures and loan limits being relaxed, among other factors, he adds. Despite Tiong Bahrus bohemian lifestyle offerings, the neighbourhood is facing stiff competition from other up-and-coming city fringe locations like Dakota, Lavender andPotong Pasir, observes Mak. This is reflected in the recent resale of a unit at the 99-year leasehold condoMeraprimelocated at Jalan Bukit Ho Swee. The 213-unit development by MCL Land was launched in 2004 at an average price of US$600 psf. The project completed in 2006, is located behind Tiong Bahru Plaza and a short walk to theTiong Bahru MRT station. The recent transaction was for the resale of am 18th floor 1,173 sq ft three-bedroom unit that changed hands for US$1.67 million (US$1,423 psf) in early June. The unit last changed hands in 2010 for US$1.55 million (US$1,321 psf). Even rents have come off in the Tiong Bahru area. A three-bedroom unit of that size could command monthly rental rates of US$5,800 back at the peak in 2012. Today, rental rates of such units are hovering around the US$5,000 mark, notes ERAs Ong. AtTwin Regency, a 234-unit freehold private condo by UOL Group and completed in 2007, there were two resales this year  one in February and the other in May, according to caveats lodged with URA Realis. The unit in February that had changed hands was a 1,776 sq ft four-bedroom unit on the 22nd level of one of the 36-storey towers. It was sold for US$2.3 million (US$1,295 psf). It was last purchased in 2007 for US$1.9 million (US$1,070 psf) when the project was newly completed.  The most recent transaction at Twin Regency was the sale of a 2,121 sq ft penthouse that changed hands for US$2.95 million (US$1,391 psf).  The former was a 2,121 sq ft penthouse that changed hands for US$2.95 million (US$1,391 psf). The unit was first purchased for US$1.51 million (US$712 psf) in 2006, hence the owner still saw a capital gain of 95.3% in nearly a decade. Meanwhile atCentral Green Condo, located adjacent to Twin Regency, a unit on the 14th floor of one of the three residential blocks was sold for US$1.59 million (US$1,233 psf). The 1,292 sq ft three-bedroom unit was last purchased for 2002 for US$760,000 (US$588 psf), hence the seller saw the value of his property double over the last 13 years. Central Green is a 412-unit, 99-year leasehold condo developed by Wing Tai Holdings and completed in 1995.   This article appeared in the City &amp; Country of Issue 682 (June 22) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/cbre%E2%80%99s-martin-samworth-transcending-space</t>
+          <t>https://www.edgeprop.sg/property-news/ground-floor-strata-fb-space-grand-building-selling-18-mil</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Beyond physical space, real estate advisers have to help create environments that draw people in  whether it is for a shopping centre, office, hotel or restaurant. You can walk into a restaurant or bar and think, Im not sure I want to be here because it has no vibe, or you can walk into one thats buzzing and then struggle to get out, saysMartin Samworth, group president and CEO of advisory services for EMEA (Europe, Middle East and Africa) and Asia Pacific at CBRE. Were trying to create ones where people want to be in; that creates value in a holistic sense.  Samworth: Clients dont see borders and boundaries; they only see investment opportunities (Credit: Albert Chua/EdgeProp Singapore)  Having been in the real estate business for 36 years, Samworth continues to find it stimulating. What I really enjoy about it is the fact that it draws on so many aspects of life and economics, he says. Samworth, who is based in London, was in Singapore last month for the official launch of CBREs new 32,000 sq ft headquarters at Paya Lebar Quarter (PLQ). Designed to showcase its vision of next-generation workplaces,CBREs premises at PLQfeature the property consultancys proprietary technology, such as Floored, to visualise and edit floor plans in 3D; Workplace 360, an approach to creating a variety of space settings that caters to different working needs; and a new mobile app, Host, which offers access to office amenities and services. Host is the glue around the business to help make things more efficient and help people save time so that they are more productive, he says.  Reference point Deploying technology and design, the workplace at PLQ is a reference point for CBREs corporate clients, whether it is for creating wellness components, design, fit-out or project management. Our corporate clients are increasingly looking to reorganise their different teams or departments when their leases are up for renewal, explains Samworth. They want to know how they can create greater collaborative spaces; or new social spaces for hospitality, food and beverage offerings. All these things are becoming increasingly important in attracting and retaining key talent in the workplace. CBRE also intends to progressively roll out the Host app and the new co-working brand, Hana, says Samworth.  The workspace area at CBRE's new headquarters at Paya Lebar Quarter (Credit: CBRE)  Launched in late 2018 and operating as a wholly-owned subsidiary of CBRE, Hana was created to help building owners develop and operate integrated scaleable, flexible workspaces. The first Hana co-working space opened in the middle of this year in the US, across three floors and more than 500,000 sq ft of Grade-A office space at the PwC Tower in Park District in Dallas, Texas. The fit-out and operating costs, as well as revenue, are shared between Hana and the buildings developers and co-owners, Metropolitan Life Insurance Co and Trammel Crow, a commercial real estate developer which is a subsidiary of CBRE. This partnership model will be replicated across multiple locations in 25 markets over the next three to four years, according to Hana in a release in February. The second Hana co-working space is scheduled to open later this year at Park Place in Irvine, California.  Read more: A Quick Guide to Singapore Co-Working Spaces And Their RatesCBRE Singapore Plans Innovation Centre of Excellence at Paya Lebar Quarter CampusERA and CBRE join forces to increase sales force to 6,500  Beyond borders After a global reorganisation last year, CBREs revenue and earnings were split along three business lines: advisory services, global workplace solutions and real estate investments. It was also then that Samworth was promoted to group president and CEO of advisory services for EMEA and Asia Pacific. The change took effect from Jan 1, 2019.  Art mural showcasing CBRE's proprietary mobile app, Host which offers access to office amenities and services (Credit: CBRE)  Samworth oversees the divisional presidents of Continental Europe, India, Southeast Asia, the Middle East &amp; Africa, North Asia, Pacific and the UK. One of the reasons why were expanding my responsibility into the Asia-Pacific and EMEA is to make sure that the two regions are absolutely connected, says Samworth. So, for major corporates that were already working for in EMEA, we can extend the relationship into Asia-Pacific. Weve already done that for a number of companies. He adds: We also see the flow of investment capital from Asia going the other way  from both local and international corporate clients. Asian outbound real estate investment had declined 36% y-o-y to US$53.8 billion ($73.2 billion) last year, butSingapore investorscontributed about 40% or US$21.6 billion. Singapore was the largest source of Asian capital in global real estate investments in 2018, said Yvonne Siew, CBRE executive director of global capital markets, Asia Pacific, in a statement in March. The top three countries for Singapore-based investors last year were: the US (US$6.4 billion), China (US$4.3 billion), and the UK (US$3.1 billion). The top three sectors they invested in were: industrial and logistics (US$7.7 billion), office (US$6.9 billion), and residential/multi-family (US$1.5 billion). The trend of Singapore investors exporting capital abroad is expected to continue in 2019, notes Siew. Clients dont see borders and boundaries; they only see investment opportunities, adds Samworth. Increasingly, corporate clients want just one service provider who can deliver the many different facets for their real estate issues. That is why CBRE has continued to broaden its offerings in facilities management and project management, with specialisation around retail, logistics, workplace environments, wellness or energy solutions, he says.  Singapore was the largest source of Asian capital in global real estate investments in 2018, according to CBRE (Credit: Albert Chua/EdgeProp Singapore)  Outsourcing, growth of GWS Advisory services business is still the biggest contributor to CBREs fee revenue, having generated US$7.56 billion in FY2018 and US$1.6 billion in 1Q2019. The next biggest fee generator is global workplace solutions (GWS), which clocked US$2.74 billion and US$692 million in FY2018 and 1Q2019 respectively. CBRE had acquired the GWS business from Johnson Controls in 2015 for US$1.48 billion, and it has become one of the fastest-growing revenue and earnings contributors for the past two years. GWS was also the biggest source of fee revenue in 1Q2019 at 28%, followed by advisory leasing services (26%), according to CBRE. Of the US$692 million in fees generated in 1Q2019, the US contributed US$302 million, with another US$319 million from EMEA and US$70 million from the Asia-Pacific. The outsourcing business is at an embryonic stage in a number of the markets, but its quite mature now in the US and in parts of Europe, notes Samworth. In many parts of the world, our key clients are still exploring how they can use our range of services and professional staff to deliver better services and at more efficient costs  whether its from a property management or facility management point of view. Thats going to be a trend that continues. Listed on the New York Stock Exchange, CBRE has a market capitalisation of US$17.57 billion as at July 9. It is considered the worlds biggest commercial real estate advisory firm in terms of revenue, which stood at US$21.34 billion as at FY2018. Among the US 500 largest public companies, CBREs ranking rose to 146th in 2019 from 207th last year. The real estate advisory business has become increasingly sophisticated, notes Samworth. We employ people from banking, and we have a lot of people in property management business who have an accounting background, understand the procurement business, the physical attributes of hotels, office buildings and shopping centres, he continues. Increasingly, were also creating environments that are fulfilling for our clients. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/cdl-unveils-republic-plaza-after-70-mil-makeover</t>
+          <t>https://www.edgeprop.sg/property-news/ground-floor-unit-bukit-timah-shopping-centre-going-58-mil</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SINGAPORE (EDGEPROP) - City Developments Ltd (CDL) has unveiled its newly revampedRepublic Plaza(RP) after an extensive $70 million asset enhancement initiative (AEI) that started in April 2018. While RP had previously undergone several enhancements, this is its first major facelift since the building was completed in 1996. RP comprises a 66-storey Grade-A office building with retail podium and a 23-storey annex block. It has a total gross floor area of approximately 1.1 million sq ft and total net lettable area of 780,000 sq ft. The RP revamp is the second AEI that CDL has undertaken as part of its growth, enhancement, transformation (G-E-T) strategy. Last year, CDL completed a $30 million AEI for Le Grove Serviced Residences, reconfiguring the original 97-unit property into 173 serviced apartments for lease. Republic Plazas AEI includes a major makeover of its main lobby, arrival frontage, individual lift lobbies as well as lift modernisation (Photos: Samuel Isaac Chua/EdgeProp Singapore) The revamp of RP reflects our focus on rejuvenating our existing assets to unlock value and strengthen our recurring income stream, says Sherman Kwek, group CEO of CDL. Post AEI, we have seen positive rental reversions at RP and achieved strong committed occupancy of over 90%, with the retail space fully leased.  More retail and F&amp;B options RPs AEI includes a major makeover of its main lobby, arrival frontage, individual lift lobbies, as well as lift modernisation. In addition, the Grade-A office buildings retail podium was expanded by another 3,400 sq ft of lettable space. This was done by partially converting its car-park area. CDL also reworked RPs public area layouts to improve pedestrian traffic, and technical specifications were upgraded to cater for more F&amp;B offerings. Following the revamp, RP now has 24,100 sq ft of retail space across three levels where close to 40 F&amp;B and retail outlets are located. Over 80% of the retail tenants are new to RP, while returning tenants include TWG Tea, Ptisserie Glac, The Herbal Bar and Bose. CDL has reworked RPs public area layouts to improve pedestrian traffic Dining options include familiar names like Din Tai Fung, Starbucks, Caf Amazon, MOS Burger, Cedele and Dimbulah. Meanwhile, there are several new-to-market concepts like Heybo, Shin Donburi, BIGDADDY and SUKHUMVIT 100. The new retail enclave also has customisable grab-and-go concepts like SIMPLEburger Inc, MOJO and Wok Hey.  CityNexus  smart building app Apart from boosting its retail offerings, CDL has created CityNexus, a smart building app that enhances the user experience of tenants. With the app, tenants can access valueadded services such as building access, meeting room booking, air-con extension requests and building feedback submissions. The app also allows tenants to provide their guests with direct turnstile entry and book dedicated VIP parking lots. CityNexus includes an order-pay-collect function that enables office tenants to preorder their meals from RPs F&amp;B outlets and notifies them when the pick-up is ready. CDL has also collaborated with United Overseas Bank to provide F&amp;B tenants with financial and digital solutions that complement the preorder function. This helps tenants to streamline their transaction workflow, improve operational efficiency and gain real-time insights into their finances. RPs several new-to-market concepts like Shin Donburi Kwek reveals plans to add more services on the CityNexus platform. Currently available exclusively to RP, the app will potentially be rolled out across other CDL office buildings in Singapore and overseas, he says.  Beyond commercial space In conjunction with the launch of the revamped RP, a Founders Gallery was unveiled to honour the late Kwek Hong Png, founder of the Hong Leong Group, CDLs parent company. Located at the main entrance of RP, the gallery encapsulates his achievements and philanthropic contributions and pays tribute to one of Singapores pioneer business leaders. Continuing his legacy of entrepreneurship, RP is providing a platform to support aspiring social innovators. This also complements CDLs commitment to sustainability. A unit at RPs basement has been converted into an incubator and co-working space for start-ups and social enterprises, called Incubator4SDGs. This initiative is in partnership with the Singapore Centre for Social Enterprise, the United Nations Development Programme and Social Collider. Sherman Kwek, group CEO of CDL, unveils the Founders Gallery at RP Elsewhere, RP has Singapores largest ultrahigh-definition (UHD) LED wall in an office building. At 1,800 sq ft, the digital wall comprises 622 UHD LED panels and serves as a digital canvas for CDL to transform RPs lobby into a gallery with varying sensory experiences throughout the day. Through the AEI, RP has been transformed into a modern and vibrant destination in the Central Business District, renewing its standing as one of Singapores most iconic Grade-A office landmarks, says Kwek. For price trends, recent transactions, other project info, check out theRepublic Plazaproject research page Read also: AWARDS: Kwek on CDLs journey of renewal and transformationThree pairs of shophouses in Tanjong Pagar for sale at $57.82 milCommercial building at North Bridge Road for sale</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/cdl%E2%80%99s-forest-woods-and-gramercy-park-steal-show</t>
+          <t>https://www.edgeprop.sg/property-news/habitap-one-app-rule-them-all</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Singapores leading listed property group, City Developments (CDL), has launched just one residential project this year, the 519-unit Forest Woods. Yet, it was one of the bestselling private condominium projects in 2016. At its launch during the weekend of Oct 8 and 9, Forest Woods saw 337 units (65%) sold by balloting at an average price of $1,400 psf. As at mid-December, the tally was 380 units (73%). Located on Lorong Lew Lian, Forest Woods is a five-minute walk to the nex shopping mall, which is integrated with the Serangoon MRT interchange station and the Serangoon bus interchange.  The crowd on balloting day at Forest Woods, during which 337 units were snapped up  Forest Woods was CDLs top-selling project in October, with 337 out of 519 units sold over its launch weekend of Oct 8 and 9  However, it is not just in the suburbs that CDL has seen units move. There has also been buying activity at Gramercy Park on Grange Road, its 174-unit luxury condo project. Gramercy Park  future capital upside When Gramercy Park obtained its Temporary Occupation Permit (TOP) in 2Q2016, the project was soft launched with an initial release of 40 units in May. The units, priced at an average of $2,600 psf, were quickly snapped up, mainly by Singaporeans. To date, 45 of the 50 units released have been sold. There are some foreign buyers as well, given Gramercy Parks freehold tenure and prime district 10 address. CDL has also marketed the project overseas, in Malaysia, Indonesia, Hong Kong and China (in Beijing and Shanghai).  View of the Gramercy Park grounds from one of the towers. CDL has sold 45 of the 50 units launched, at an average price of $2,600 psf.  The buyers recognise that $2,600 psf for a prime freehold project on Grange Road represents great value, says Samuel Eyo, managing director of Singapore Christies International Real Estate. In the past, projects launched in the area crossed $3,000 psf. So buyers of Gramercy Park today can expect to see future capital upside. Units at the project range from 1,184 sq ft for a two-bedder to 7,287 sq ft for a five-bedroom penthouse. It was designed by NBBJ of New York, the same architect behind CDLs other landmark development, the 1,111-unit The Sail @ Marina Bay. Nouvel 18  CDLs third PPS Unlike Gramercy Park, Nouvel 18, another CDL luxury condo project, had a more unconventional exit. It was divested via a Profit Participation Securities platform in October, marking CDLs third and latest PPS. The divestment involved the sale of CDLs entire stake in Summervale Properties, the entity that owns Nouvel 18, for $977.6 million. CDL sold its entire investment in Summervale Properties, the owner of Nouvel 18 for $977.6 million, through its third PPS platform  Based on the saleable area of 351,000 sq ft, the deal valued the 156-unit freehold project at $2,750 psf. The sale allows CDL to avoid paying hefty extension charges under the governments Qualifying Certificate conditions, which would have kicked in last month. Nouvel 18 is a redevelopment of the former Anderson 18. The 112,098 sq ft freehold site was purchased for $477.7 million, or $1,650 psf per plot ratio, in 2007 under a 50:50 joint venture (JV) between CDL and Wing Tai. The twin 36-storey solid black towers were designed by renowned Pritzker Prize-winning French architect Jean Nouvel, who also designed Wing Tais other luxury condo, Le Nouvel Ardmore, next door. The PPS has been widely anticipated after CDL bought Wing Tais 50% stake in Nouvel 18 for $411 million in July, which valued the property at $2,342 psf. Although CDL has divested the asset, its wholly-owned subsidiary, Trentwell Management, has been appointed the asset manager and marketing agent of Nouvel 18. It will manage, lease, market and sell the units in the development. For now, asset enhancement works are underway, and units will be offered for lease in 1Q2017. CDLs first PPS, launched two years ago, was a $1.5 billion partnership with US investment bank Blackstones Tactile Opportunities Fund and CIMB Banks Labuan Offshore Branch. The PPS invests in the cash flow of the assets within CDLs Quayside Collection, namely the W Singapore Hotel, The Residences at W Singapore and the Quayside Isle retail strip. The second PPS was launched in 2015, and it was a $1.1 billion joint investment with Alpha Investment Partners in a portfolio of three of CDLs office assets, namely Central Mall (office tower), Manulife Centre, and 7 &amp; 9 Tampines Grande. New beginning at South Beach, The Venue At South Beach, CDLs mixed-use development in a JV with Malaysias IOI Properties, the JW Marriott Hotel Singapore South Beach officially opened on Dec 15. The 634-room luxury hotel was initially branded The South Beach. Besides the JW Marriott Hotel, South Beach also contains luxury residences above the hotel, which is yet to be launched, as well as retail outlets and a Grade-A office tower, which is fully leased. The South Beach is linked to Suntec City via an overhead pedestrian bridge, and to the Esplanade MRT station underground. Next year will see the completion of CDLs The Venue Residences and Shoppes in the second quarter. Loca ted a short distance from the Potong Pasir MRT Station, The Venue contains 266 residential units and a retail po dium with 28 strata shops for sale. The residential units range from a 495 sq ft one-bedder to a 2,142 sq ft four-bedroom penthouse and the commercial units are from 301 to 1,302 sq ft.  At The Venue Residences, 70% of the 266 units have been sold, while 60% of the 28 units at The Venue Shoppes have been taken up  To date, 70% of the residential units at The Venue have been taken up at an average price of $1,400 psf, while 60% of the strata commercial units have been sold, with the average price hovering at $5,400 psf. Buying demand was slow and selective this year and the cautious sentiment may extend into 2017, says CDLs spokesman. Nevertheless, projects with strong locational attributes can be expected to out perform the rest of the market.  This article appeared in The Edge Property Pullout, Issue 760 (Dec 26, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/centrepoint-gets-50-million-makeover</t>
+          <t>https://www.edgeprop.sg/property-news/hefty-loss-incurred-despite-19-year-holding-period</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">SINGAPORE (Mar 19): Frasers Centrepoint Malls has announced plans for The Centrepoint shopping centre to undergo a $50 million asset enhancement initiative (AEI), as part of the group's ongoing efforts to boost the shopping experience for the mall's customers. The programme is scheduled to start in May this year, and will see major renovation works to the ground and basement levels and an integration of floor plates between the main building and basement annexes. Frasers Centrepoint Commercial CEO Christopher Tang said the asset enhancement of The Centrepoint was part of an on going strategic initiative aimed at refreshing the malls under the group's portfolio. "We are pleased to announced the AEI and are confident the overall exercise will inject greater vibrancy into the mall. The Centrepoint is one of the most iconic malls of Orchard Road...since it opened its doors in 1983, the mall has undergone several makeovers ," he said in a statement filed with SGX this evening. According to the statement, the Orchard Road entrance will see a major revamp with a wider street frontage and greater shop visibility. The mall will remain open and continue to trade during the renovation. The AEI is scheduled for completion in the second half of 2016. Fraser Centrepoint Ltd closed 2.5 cents higher at $1.75. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/centrium-square-retail-units-sold-bulk-deal</t>
+          <t>https://www.edgeprop.sg/property-news/high-park-residences-hits-right-note-buyers</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>At least 32 retail units at Centrium Square with a total strata area of 16,738 sq ft could have been sold through a bulk purchase for $70.1 million, based on caveats published by the URA. The project, which was the former Serangoon Plaza, is being developed by Feature Development, which is an associate of Tong Eng Group. The buyer is believed to be Canali Logistics Pte Ltd which also purchased Hotel Grand Chancellor at Belilios Road in Little India in 2014. The first storey retail units were sold at an average price of $6,015 psf while those on level two fetched an average price of $3,932 psf. Centrium Square is a freehold development located next to the 24-hour department store Mustafa Centre. It is also within a short walking distance from Farrer Park MRT station, just two stops from Dhoby Ghaut MRT station on the Orchard Road shopping belt. The area is touted to be the next medical hub with the recent opening of Farrer Park Hospital which is part of an integrated complex comprising Farrer Park Medical Centre housing specialist clinics and One Farrer Hotel and Spa. Separately, RB Capital is developing Farrer Square, a mixed-use project comprising medical suites and 300-room Park Hotel Farrer Park. It was reported that three floors of the medical suites were also sold in a bulk deal in 2014 to HSC Healthcare which is headquartered in Kuala Lumpur. Centrium Square has two levels of retail units, 39 medical suites on level six to eight and 143 offices from level nine to 19. It was reported that Tong Eng had initially planned to retain and manage the two floors of retail units. Meanwhile, the medical units will be sold on a per floor basis. Based on URA caveats, at least 20 office units have been sold at between $2,353 and $2,624 psf, or $2,514 psf on average. They range from 570 sq ft to 1,012 sq ft in size. In 2014, Canali Logistics acquired the 328-room Hotel Grand Chancellor from Hotel Grand Central Limited for $248 million. The price works out to around $756,000 per room.  Centrium Square is a freehold development comprising two levels of retail units, 39 medical suites and 143 offices. It is within a short walk from Farrer Park MRT station</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/changi-ranked-top-logistic-micro-market-singapore-colliers</t>
+          <t>https://www.edgeprop.sg/property-news/high-park-residences-rises-amid-uncertainty</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SINGAPORE (EDGEPROP) - Changi has come out on top as the most desirable location in Singapore for logistics players, owing to its proximity to Changi Airport. The mature industrial area is ahead of other industrial zones in Tuas and the cluster around Boon Lay/Jurong West, according to a report by Colliers International. In Changi, available stock in the industrial area is limited and warehouse unit sizes are typically smaller than those in the West region. Total warehouse space in Changi amounts to about 3.7 million sq ft, compared to other areas such as the cluster at Jurong East/Clementi which has a total warehouse stock of 30 million sq ft. However, there is strong demand for industrial space in Changi from light industries, logistics and third-party logistics operators requiring air transportation. The latter two business segments are the top industrial space occupiers, accounting for about 44% of occupied warehouse space in Singapore. As a result, the vacancy rate in Changi is the lowest among the major logistics locations in Singapore at close to 2.7%, compared to the cluster at Tampines/Paya Lebar at 15.2% or Tuas at 10.5%. Singapore has been the location of choice for e-commerce players to establish their footprint when entering the region. The emergence of e-commerce in recent years has had a positive spillover to the 3PL and logistics sector in Singapore, says Tricia Song, head of research for Singapore at Colliers International. Other warehouse occupiers in Singapore include the manufacturing sector which takes up 30% of warehouse space; distributors (10%); food, chemicals and pharmaceuticals (6%); oil, marine and energy companies (5%); and IT and technology (5%). According to the report, regional trade and the growth in e-commerce is likely to translate into stronger warehouse demand in the long term, but greater efficiencies in inventory forecasting and stock management may moderate the need for drastic warehouse expansion. Overall warehouse rents in Singapore have been sliding for more than five years, and the latest JTC rental index showed that in 2Q2019 the index had declined by 19.4% from its peak in 4Q2013. The warehouse rental index fell 0.2% q-o-q in 2Q2019, and declined by 0.2% y-o-y. Logistics rents are expected to remain weak in the near term, and with a more benign warehouse supply pipeline, occupancies and rents could improve from 2022 onwards, says Song. It is timely for tenants to review their lease and space requirements, and explore options. They can consider locating further away from the city centre to enjoy rental savings or opt for customised and build-to-suit warehouse facilities which would offer greater rental certainty, says Dominic Peters, senior director of industrial services at Colliers. Read also: Investment sales jump 49% q-o-q to $6.7 bil in 2Q2019CBD revitalisation and integrated resort investment to drive up local commercial property investmentLogistics building Space@Tampines on the market from $170 mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/chinoiserie-chic-we-beg-differ</t>
+          <t>https://www.edgeprop.sg/property-news/high-specification-industrial-building-paya-lebar-sale</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Contemporary Asian design does not have to scream chinoiserie, as proven by a penthouse show unit at Leedon Residence designed by Creative Mind Design. Ian Lee, lead designer of the project, describes it as the new Asian luxury, where luxury is quiet, contemplative and, as paradoxical as it sounds, modest. Born to Malaysian-Chinese parents but raised in the UK, Lee admits to being more familiar with Western values and culture than his Asian roots. Nevertheless, he subconsciously draws from Asian influences in his design process, marrying them with his Westernised tastes. Hence, you are not likely to find heavily lacquered timber, fretwork screens or dogmatic minimalism in his design. Instead, you will find balance, restraint and serenity, which are highly valued in Asian societies. Throughout the interior spaces, dualities in form, texture and colour are skilfully balanced. Clean lines bring out the patterned surfaces of natural stone and timber, while the hardness of these materials is softened with flowing drapes. The space is amply filled with cushions and plush throws and rugs. Dark millwork forms a reticent backdrop for furniture mostly in light grey and beige tones.  Balancing contemporary and classic In the living area, a full-height shelving unit with a hidden TV compartment has sliding doors clad in faux shagreen. Shagreen is a highly sought-after decorative material dating back to the Chinese Han Dynasty and has graced the sword hilts of the Japanese samurai and the trinkets of French aristocrats alike. Commonly sourced from East Asia, it is traditionally found in the homes of the very rich around the world and deemed an exotic and precious material by those in the know. A sense of balance is also apparent in the furniture selection. Anchoring the space is a modern, classic L-shaped sofa, paired with a rectilinear coffee table. There is stability in the stance of the table, yet a sense of lightness as it seems to hover just above the soft carpet. Balancing out the conservative silhouettes of the sofa and coffee table is a very hip and unexpected form of an armchair with its pillowy upholstery  the Husk by Patricia Urquiola  and a wireframe end table, both of which exude playfulness and freshness.  Balance out conservative silhouettes with unexpected forms such as the playful Husk armchair by Patricia Urquiola  The courtyard concept The penthouse unit comes with a sky garden, which has two main spaces  a lounge area and an outdoor dining area. The sky garden does not pretend to be a traditional Asian courtyard, but it serves to contain family- oriented activities. A bright red Kub low table by Japanese design studio Nendo gives the lounge area an upbeat vibe.  Spacious sanctuary Timber blinds over a glass screen separate the bedroom from the master bathroom, a spare and clutter-free space that has a freestanding tub to complete the experience of a private Zen-like sanctuary.  A free-standing tub makes the bath appear spacious and clutter-free, creating a private Zen-like sanctuary  Luxury with restraint In the dining area, a bespoke marble table is arguably the showpiece of the apartment. Composed of Italian marble with timber accents, this three-metre table may not be Asian in appearance, but it is so in essence. It was designed to be a gathering place, drawing families together for a meal in traditional Asian style. It is luxurious without being ostentatious, as its designer, Charlton Ho of Creative Mind Design, explains. Bullnose detailing, as well as the choice of white Carrara marble, make this potentially clunky table appear elegantly sleek. We also made sure the proportions are generous enough to seat the whole family comfortably. He explains that timber laminate strips were incorporated to complement the dark millwork in the rest of the apartment. For the dining chairs, Lee selected the iconic mid-century Platner Arm Chairs in ivory. With their graceful wire structure and comfortable upholstery, they are a picture of elegance or, in other words, restrained luxury.  Bullnose detailing and thechoice of white Carrara marblemake this potentially chunkytable appear sleek and modest  Serenity in style The quiet luxury of the common areas carries over into the bedrooms. Fuss-free fabrics in a neutral palette create a calming, restful mood, with punches of statement Thai silk pillows from Jim Thompson to break the monotony, as described by Lee. In the master bedroom, he opted for dark timber strips that form a feature wall behind the headboard. To accessorise the space, he chose objects that are subtle but have character, such as exotic bedside table lamps with shagreen-clad stands sourced from Thailand.  Instead of wallpaper, how about a feature wall made of dark timber laminate strips to add depth to the space and enhance the calming ambience  Grace Chen is a communications writer/designer for Creative Mind Design, an award-wining interior design studio that crafts meaningful and relevant interior spaces, bringing fresh and compelling expe riences for all to enjoy. Visit www.cmd.sg for more information.  This article appeared in The Edge Property Pullout, Issue 727 (May 9, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/city-developments-only-singapore-property-group-listed-gender-equality-index-two-years-running</t>
+          <t>https://www.edgeprop.sg/property-news/hilltops-unit-sold-2397-psf</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Singapore property giant City Developments Ltd (CDL) has been selected for the 2019 Bloomberg Gender-Equality Index (GEI). It was selected in recognition of its commitment to transparency in gender reporting and advancing gender diversity in the workplace. In a traditionally male-dominated industry, CDL is honoured to be listed on the GEI for the second consecutive year, says Sherman Kwek, CDL group CEO. Our diversity across genders, age groups, cultures and geographies has given us a strong strategic advantage and we will continue to support the professional development of all employees within our Group.  CDL Group CEO Sherman Kwek (centre) and group general manager Chia Ngiang Hong (fifth from left) with women department heads. Women employees form 70% of CDLs workforce and 47% of its department heads (Credit: CDL)  GEI is tracked by investors and uses a standardised reporting framework for public companies to disclose information on how they promote equality across different areas based on company statistics, policies, community engagement as well as products and services. Women employees form 70% of CDLs workforce and 47% of its department heads. In 2018, the number of women department heads in CDL increased by 60% compared to 2017. CDL established an internal Diversity and Inclusion Task Force in 2017, complementing its CDLs Women4Green network, a first in Singapore, which inspires and empowers women to create a financially, environmentally and socially sustainable future. CDL also adopted a formal Board Diversity Policy in 2017. To date, two, or about 30%, of the seven directors on the CDL board are women. This surpasses the Diversity Action Committee (DAC) Singapores recommended target of having a 20% woman representation on the boards of Singapore-listed companies by 2020. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/close-31-units-sold-1953</t>
+          <t>https://www.edgeprop.sg/property-news/house-fortune</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A mixed-use development named 1953 by developer Oxley Holdings, was launched over the weekend of Mar 9-10. The boutique development located on the corner of Balestier Road and Tessesohn Road, contains 72 units, of which 58 are apartments and 14 are strata commercial units. The freehold development contains a conserved two-storey shophouse integrated with a new six-storey block. The appointed design architect for the project is Park + Associates, with Ecoplan as the landscape architect. Meanwhile, 2nd Edition is the projects interior designer.  Crowd on Sat Mar 9, first day of launch at 1953 sales gallery (Credit: Oxley Holdings)  The project was launched via placement of units, says Eugene Lim, Oxley Holdings marketing and sales director. The turnout and sales have been very encouraging, he adds. Feedback was buyers like the architecture and the product. Its a rare opportunity for buyers to own a freehold development with a conservation element. According to Oxley, 22 units  19 residential and three commercial - were snapped up as at 6pm on Sunday, Mar 10. The residential units fetched an average price of $1,875 psf while the commercial units were sold for an average of $3,185 psf. Residential apartments range from two-bedroom-plus-study units of 614 sq ft to four-bedroom units of 1,399 sq ft. Retail units are from 700 to 786 sq ft. The number of units sold translates to about 31% of the total number of units in 1953. This makes 1953 the best-selling, boutique development in 2019 so far, says Oxleys Lim. The pricing of the units proved to be attractive given that its a freehold development in a city-fringe location, says Ismail Gafoor, CEO of PropNex Realty. Most of the city-fringe projects that are freehold today are priced above $2,300 psf and even some 99-year leasehold projects in the city fringe are around $2,000 psf." Adds Gafoor: "The sales rate at 1953 shows that even though buyers may be price-sensitive, if they perceive that a project presents good value, they will still make a purchase."</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/close-city-yet-surrounded-greenery</t>
+          <t>https://www.edgeprop.sg/property-news/house-tour-jerome-and-sarahs-charming-home-industrial-style-mezzanine</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>For shipping manager Chong Yoke Chye and his three adult sons, all of whom are avid joggers,The Interlaceprovides the ideal base from which to explore the surrounding green belt.  It was love at first sight when Chong Yoke Chye, 58, and his family of four eyed the ample sporting facilities and lush landscaped grounds ofThe Interlace, a condominium along Depot Road. I go jogging a lot, and so do my kids, says the father of three boys aged 25 to 31. The 1-kilometre jogging track, which skirts the borders of the sprawling 8-hectare site and connects its various courtyards and gardens, was therefore the most attractive feature. 50m lap pool at the Water Park Courtyard and the state-of-the-art gym were a close second. The Chong family, who toured the development almost immediately after it was completed and handed over to residents in late 2013, was keen on The Interlaces other recreational facilities, such as the BBQ promenade, karaoke rooms and theatrettes. Yoke Chyes sons were also particularly fond of the Spa Valley Courtyard, which houses the massage pool, spa pool lagoon, Jacuzzi and Waterfall Grotto. The Spa Valley Courtyard is just one of eight themed courtyards interspersed throughout the property.  It was love at first sight when Chong Yoke Chye and his sons toured the ample sporting facilities and lush landscaped grounds ofThe Interlace  GENEROUS UNITS So the decision to settle down in a three-bedroom unit was made very quickly. That the units were generously proportioned was a plus  considering how small the units in newer condominiums in the downtown core tend to be  but not a main consideration. The units here are all pretty big but because my children are grown up, we thought we would get one that was just the right size for us, says Yoke Chye, a shipping manager who is planning to retire soon. His sons Shao Ming, 31 and Shao Soon, 28, are both engineers, while Shao Siong, 25, is a recent graduate looking for employment in the banking/finance sector. The Chongs were among the first to buy their home soon after the projects Temporary Occupation Permit in 2013. They chose a 1,260 sq ft three-bedder. One of the main characteristics of the development that attracted them was the spacious layout of the units  with most units ranging in size from 1,873 sq ft for a three-bedder to 6,308 sq ft for a luxurious penthouse with private roof terrace. Many of the units come with private enclosed spaces or even private roof terraces.  Youngest son and recent graduate Shao Siong in his bedroom-cum-study  Second son Shao Soon in the family room of the spacious three-bedroom unit  A VERTICAL VILLAGE Of course, the most distinctive feature ofThe Interlacehas to be its unique architecture, designed by world renowned architect OMA/Ole Scheeren, and developed by a consortium led by CapitaLand. Thirty-one apartment blocks, each six storeys in height, are stacked in a hexagonal configuration and laid out around the eight courtyards. The interlocking blocks create a series of stepped volumes, some partly resting, others partly floating, like a vertical village. The sum effect is one of an interlaced structure  from which the development gets its name  that weaves individual apartments into the fabric of an inclusive community. Because of this design, the developments 1,040 units come in various configurations and facings. I wanted something thats very quiet and peaceful, says Yoke Chye. Of the apartment he picked, he says: This, to me, is a perfect unit. You can see the AYE but youre not so close to it that you can hear the traffic. And the height (on the ninth floor) is just right. The family moved into their new home atThe Interlacefive weeks after they received their keys and did a simple renovation. Among the more interesting fittings that Yoke Chye chose are pendant lights that resemble The Interlaces stepped architecture. We bought the unit without knowing much about the architect. But after that, I did some research and learned that the architect designed a lot of well-known buildings, he says, referring to the China Central Television (CCTV) Headquarters in Beijing, the MahaNakhon in Bangkok, as well as the Prada Epicenters in New York and Los Angeles. The Interlaceis famous in its own right, too, having won multiple awards, such as Best Architecture at the 2010 Asia Pacific Property Awards and World Building of the Year at the 2015 World Architecture Festival, affectionately dubbed The Architectural Oscars.  What the Chong family likes is the spaciousness of the 8-hectare site atThe Interlace, with its lush tropical foliage  GREENERY EVERYWHERE Thanks to the way the apartment blocks are stacked, the number of horizontal surfaces supporting roof gardens and landscaped terraces could be maximised. These extend the outdoor space on multiple levels, providing views above the tree line to the surrounding courtyards, the Central Business District and the Straits of Singapore beyond. In total, these provide green areas that equate to 112% of the development site area. Theres greenery everywhere, says Yoke Chye. I also appreciate the spaciousness of the property. I dont think you can find a condominium of this size thats so close to the city. The 8-hectare site, with its towers abundant in lush tropical foliage, reinforces the idea of a vertical village embedded in nature.  LOCATION, LOCATION Besides the proximity to the city, Yoke Chye  who has been a city dweller all his life  also appreciates The Interlaces immediate vicinity, especially since it is nestled within a green belt. The location is superb, he says. Within 20 minutes of walking, youll hit Kent Ridge Park, HortPark, Labrador Nature Reserve and Mount Faber Park. On weekends, when he has more leisure time, Yoke Chye will take the free shuttle bus fromThe Interlaceto VivoCity. From there, he will take the Marang trail to Mount Faber Park, jog all the way to Kent Ridge Park, and then take the train from Kent Ridge MRT station home. Its a total distance of 9.3 km, with two treetop walks and scenic trails along the way, he adds. When the avid jogger is pressed for time, he will work out at the gym and run five laps around the 1km track. I start running at 10.30pm and the jogging track is very well-lit. Its really like running in a park, says Yoke Chye. His sons go for runs on their own as well, and occasionally get together with the neighbours for bouts of street soccer. And when it comes to family bonding time, the Chongs love nothing better than to enjoy one anothers company over BBQ at one of the barbeque pavilions.  More than 100 units snapped in just one week! 15% discount for selected units. With a downpayment from as low as $250k*, move into your dream home immediately and save on loan interest payments for 12 months! The CapitaLand Stay Then Pay programme is applicable for selected units only. *Based on the selling price of a $2.5M unit (excluding any stamp duties payable) Visit our sales office at 216 Depot Road #03-70. Open daily from 11am to 6pm. 6273 0340 / theinterlace.com.sg</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/co-investing-development-opportunities-uk</t>
+          <t>https://www.edgeprop.sg/property-news/how-do-mrt-stations-affect-property-prices-and-rent</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>An inevitable outcome of greater government intervention in the form of higher taxes and tighter regulations is more creative alternative investment schemes targeted at cash-rich investors. The primary target? Singaporeans. Owing to the series of property cooling measures in both Singapore and the UK, launches of London projects have lost some of their lustre. In 2009, there were 30 exhibitions with sales of 100 million. By 2011, there were 80 exhibitions with total sales of 450 million. At the height of the market in 2012, there were 100 UK property exhibitions in town, with sales of 650 million. By 2014, the number of exhibitions had slowed to 70, and last year, it whittled down to 50, according to data compiled by CBRE. The projection is that the figure could be even lower this year. In good times, developers budgets for overseas project launches are typically in the seven-figure range. In 2012, I was involved in the marketing of a London project across five cities in Asia, including Singapore, says a veteran in overseas property marketing. The developer spent about 1 million. An overseas property launch with all the bells and whistles  five-star hotel venue with wine and canapes; smartly suited representatives from the developer flown in for the occasion; marketing materials, including advertisements  can amount to $200,000 for just one weekend. Some niche players who have focused on marketing London projects to overseas buyers in Asia have since repositioned themselves as property developers and are offering Singapore investors co-investment opportunities.  Thinking out of the boxThe off-plan sales exhibitions have taken a hit, says London-based Naoufal Dhimi, co-founder and director of Saffron Homes, who was in Singapore last week. So, we have to think out of the box and [come up with] ways to move the business forward. Our investors and clients always tell us that deep down, they want to be developers. And, it can be a success ful strategy. Another co-founder of Saffron Homes is Monty Nawaz, who set up Saffron International as a London broker with an office in Singapore in 2005. Saffron was established in London in 1997 and specialises in lettings and identifying resale or undervalued investment opportunities in London for overseas clients. Saffron Homes was launched as a property investment and development arm with opportunities exclusively for investors in Asia, says Nawaz. We look out for undervalued or overlooked projects, and structure tax- efficient investment schemes for Asian investors to co-invest in. A third co-founder is Singaporean architect Patrick Ng, who has practised in London for the past 15 years, previously with award-winning London architectural firms Tate Hindle and Sheppard Robson.  Niche developer Saffron Homes founders (from left): Ng, Dhimi and Nawaz  Club dealsSome of the projects in London offered by Saffron Homes to Singaporean investors are in the form of club deals, with a minimum entry of 200,000 ($384,908). One example is a 10,000 sq ft commercial site at Leyton High Road, currently an investment hotspot in the London borough of Waltham Forest. The site was secured by Saffron for 1.6 million; it can be torn down and redeveloped into a residential scheme. In February, the group obtained planning permission for the development of a three storey building with retail space on the first level and nine apartments on the upper levels. Construction is expected to cost 1.2 million. Upon completion, the total gross development value of the project is estimated to be 4 million. Saffron is not new to the area. In June 2014, it acquired the Oliver Twist Pub, which already had planning permission to renovate internally and add another floor for conversion into nine apartments. The acquisition price was 900,000, and another 650,0000 was spent on renovations. Saffron gutted the property and rebuilt it as planned. By February 2015, all nine apartments were sold, for a total of 2.7 million. Another example of redevelopment with change-of-use opportunity is a 10,000 sq ft freehold site on Coopers Lane. Currently, there is a vacant metal pipe workshop on the site, but planning approval has been secured for it to be redeveloped into a gated residence with six townhouses, Ng says. In the prestigious Knightsbridge area, Saffron Homes recently completed the acquisition of two freehold houses at Draycott Place, located just 800m from Harrods. The acquisition was made with equity participation from a Middle Eastern bank. The vendors have already obtained planning approval and Saffron just needs to take care of the additions and alterations to the interior of the building. Plans are underway to turn the property into 10 apartments with sizes starting from 1,600 sq ft, says Ng. The level of quality and finishing of the apartments are expected to be comparable to those at the ultra luxury One Hyde Park. There is space to add two studio apartments. Given the projects prestigious location, the market price of the apartments is in the range of 3,500 to 4,000 psf. That translates to asking prices of 6 million to 25 million per unit. If we were to put it on the market today, the apartments will sell out in a very short time as there are a lot of people who would love to live in [them], says Dhimi.  Draycott Place at Knightsbridge, which Saffron Homes acquired with equityparticipation by a Middle Eastern bank, where planning approval has beenobtained for 10 apartments and 12 underground parking  When additions and alterations are completed, the project at Draycott Place will have the quality finishing of One Hyde Park   Boutique projectsSaffron Homes intends to stick to its niche of boutique developments. We dont want to go into large-scale developments with a few hundred units, says Nawaz. Many of the investors weve been talking to are those we have [established a] relationship with over the years, and they understand the London market. While some of Saffrons offshore structures and special-purpose vehicles are based in the British Virgin Islands (BVI) or Guernsey, Dhimi does not see any cause for concern, even in the wake of greater scrutinity in such offshore vehicles following the recent Panama Papers leak. Nawaz adds that the only tax that investors in the investment vehicles will be subjected to is a 20% corporate tax. Interest in these schemes has been equally strong among investors in both Singapore and Malaysia. We dont offer these opportunities as agents on behalf of developers, he adds. We offer them as a development opportunity in a joint venture (JV) with Saffron Homes. According to Norman Ho, partner in law firm Rodyk &amp; Davidsons real estate practice, such offshore companies are often used by parties to minimise tax liabilities. But being tax efficient does not equate to tax avoidance, he says. And it cannot be assumed that an offshore vehicle is used for improper purposes.  Marketing agency turned developerLike Saffron, another property group that is changing its strategy is Strawberry Star Group, founded in 2006 by its chairman, Santhosh Gowda, and set up in London in 2007. Strawberry Stars maiden investment was in Berkeley Homes Chelsea Bridge Wharf, where it invested 18 million. That was our first acquisition, says Gowda. We underwrote the project and sold the units to individual investors. In 2012, Strawberry Star undertook the development of Sky Gardens in Vauxhall, Nine Elms. The project has over 200 units and was developed in partnership with Frasers Property UK, the UK property arm of Singapore listed property group Frasers Centrepoint Ltd. It will be completed this year.  The 999-year leasehold Sky Gardens contains 204one- and two-bedroom apartments and is scheduledto be completed by end-2016 or early 2017 Source: Strawberry Star  Hoola, a 360-unit residential development developedby Strawberry Star in partnership with HUB,is located at the Royal Victoria Dock in London  Another project is Hoola, which Strawberry Star acquired from UK developers Hub in 2014. Located at Londons Royal Victoria Dock, the 360-unit development with a mix of studios and one- to three-bedroom apartments is scheduled for completion this year. Last year, Strawberry Star also invested in the 1 billion Asian Business Port (ABP) project in Royal Albert Dock in East London, jointly with Chinese developer Advanced Business Park. Strawberry Star invested 34 million in the first phase of the project, and is expected to invest up to 98 million in total, making ABP its biggest investment to date.  Gowda: Were confident that we can now deliverprojects like mainstream developers, and we wantto reach out to people in Asia and the Middle Eastto join hands with us  Scaling upTo date, Strawberry Star Group has aggregate investments totalling 500 million and a develop ment pipeline of more than 1,000 units, says Gowda. Over the last five years, it has also formed its own development, sales and market ing as well as leasing teams. Were confident that we can now deliver projects like mainstream developers, and we want to reach out to people in Asia and the Middle East to join hands with us, he adds. Besides a presence in London, Strawberry Star now has an office in Hong Kong and Singapore. Gowda had set up his family office and holding company KSD Holdings in Singapore in 2006. Prior to that, he spent 10 years in the Middle East, marketing projects to nonresident Indians working there who wanted to invest in property back home. The group has a division called Strawberry Star Capital, which focuses on identifying investment opportunities and raising funds to secure the investments. In January, Straw berry Star launched its first property investment fund after securing 25 million. The firm also announced that it has secured a commitment of another 50 million from co-investors in the Middle East, Asia and the US. Were looking at deploying the fund in a couple of investments, adds Gowda.  New starStrawberry Star also announced the appointment of Doris Tan as regional director from the start of 2016. Tan, an international property veteran of more than 30 years, was heading the international residential property team in JLL before this. She had joined JLL after her firm, DST International, which she founded in 1998, was acquired by JLL five years ago. A lot of smaller developers from Singapore are keen to enter the London market but they dont know how to get started, says Tan. Now, we can help them [look] for the right site, raise capital, develop the project, and then sell the units downstream, as well as manage them on behalf of investors after the sale. Tan will be overseeing Strawberry Stars operations in both Singapore and Hong Kong. According to Gowda, the primary objective of opening offices in Singapore and Hong Kong is to raise more equity for our investments in London. Typically, Strawberry Star will look at develop ment projects of 150 to 250 units. Tan says the minimum investment by investors in Straw berry Stars projects is 5 million to 10 million. The profile of the investor is very important, she says. Were not targeting the man in the street. First, the investors must have experience investing in London. If they prefer to be passive investorst but are prepared to provide funding, they can enjoy the returns.  Tan: Were not targeting the man in the street. Theinvestors must have experience investing in London.If they do not but are prepared to provide funding,they can enjoy the returns.  Joint venturesThe group is also looking at forming JVs with UK government councils to build homes for the local communities, primarily in Zones 3 and 4 in London. According to Gowda, while prices of prime Central London have peaked, there is still a housing shortage in the Greater London area. In a JV with the councils, we dont have to pay for the land upfront, but we will provide funding for the construction, he adds. Thats where investors from Singapore can invest with Strawberry Star. Thats where the demand for housing is. Tan says she will continue to tap her network of overseas developers and bring projects to Singapore. On April 14, Strawberry Star showcased a project from Berlin. The project offers a mix of one- to two-bedroom units priced from 250,000 ($381,753) to 500,000. Tan adds that up to 70% bank financing will be provided. While the heady days of strong sales every weekend at overseas property exhibitions may be over, Saffrons Nawaz sees the rise of new opportunities. It was a good ride while it lasted, he says. But the strategy of selling projects off-plan at overseas property exhibitions was always going to be short-lived. As for us, were the developers and were offering investors the opportunity to invest alongside us.  This article appeared in the City &amp; Country, Issue 724 (April 18, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/commercial-building-north-bridge-road-sale</t>
+          <t>https://www.edgeprop.sg/property-news/how-has-singapore%E2%80%99s-first-dbss-project-fared-against-resale-hdbs</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SINGAPORE (EDGEPROP) - A commercial building at 333 North Bridge Road is up for sale by tender with an indicative guide price in the region of $80 million. The 999-year leasehold, nine-storey commercial building has a site area of about 4,684 sq ft and a total gross floor area (GFA) of 29,049 sq ft. Additional GFA of 3,218 sq ft may be built, with no development charge payable. Located on a corner plot with dual frontage along North Bridge Road and Cashin Street, the building has views of the Raffles Hotel right across it. The property is zoned commercial under the 2014 Master Plan, with a plot ratio of 5.2 and building height of up to 16 storeys. No additional buyer's stamp duty or seller's stamp duty will be imposed, and both locals and foreigners are eligible for purchase. Keen interest is expected from companies seeking to own a corporate office with a strong presence in the city centre, as well as investors looking to invest in a prime commercial asset in a good location, says Swee Shou Fern, executive director of investment advisory of Edmund Tie, the sole marketing agent for the sale. The property is served by four MRT stations located within a 500-metre radius, with the Raffles Place financial district and the Orchard Road shopping belt just an MRT stop away. The astute developer may also consider redeveloping the property to maximise the gross floor area and explore a strata sale of the new development. Given its central location, the property is also ideal as a private members club or an embassy, subject to authorities approval, adds Swee. The tender exercise will close on Nov 5, at 3pm. For price trends, recent transactions, other project info, check out theNorth Bridge Roadresearch page Read also: DC rates up 1.7% for commercial, down 0.3% for non-landed residential useEu Yan Sang Building in Chinatown going for $62.5 milMixed-use building in Kallang up for collective sale at $160 mil Check out the latest listings nearNorth Bridge RoadandMRT Stations</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/commercial-component-wilkie-edge-sale</t>
+          <t>https://www.edgeprop.sg/property-news/how-rents-fared-hdb-flats</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The commercial component at Wilkie Edge has been put up for sale by expression of interest (EOI). Wilkie Edge is located within the Bras Basah-Bugis district. Completed in 2008, Wilkie Edge is designed by the award-winning architect, WOHA Architects, and was awarded the BCA Green Mark Gold Award in 2012. The 99-year leasehold property is a 12-storey integrated mixed-use development, comprising retail, office, 154-unit serviced residences and 215 carparks lot. The commercial component for sale comprises a two-level retail podium, six floors of prime grade quality office space and two basement carpark. It has a gross floor area of approximately 215,000 sq ft and net lettable area of approximately 154,000 sq ft. As at end-October, its occupancy rate was close to 100%. Cushman &amp; Wakefield is the appointed sole marketing agent and the EOI closes on Jan 19.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/commercial-development-site-queenstown-200-mil</t>
+          <t>https://www.edgeprop.sg/property-news/impact-mrt-property-prices</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A 99-year leasehold site at the corner of Commonwealth Avenue and Margaret Drive is on the market for $200 mil. The sites tenure started on January 1 1975, and the 32,305 sq ft vacant plot used to be the site of the former Queenstown Cinema. Cushman &amp; Wakefield (C&amp;W) is the marketing agent for the sale. Located 300m to the Queenstown MRT station, the site has been granted Written Permission to be developed into a six-storey commercial building comprising shops, restaurants, community institutions, and a cineplex with basement car parking lots. The approved gross floor area (GFA) is 96,914 sq ft, and no development charge is payable. The current asking price translates to $2,063 psf over the approved GFA. (Picture: Cushman &amp; Wakefield) The immediate neighbourhood of the subject site is undergoing massive rejuvenation with multiple new condominium developments such as Stirling Residences, Margaret Ville, Commonwealth Towers and Queens Peak, as well as new public housing projects including SkyOasis @ Dawson, Skyresidence @ Dawson, Skyville @ Dawson and Skypac @ Dawson, says Shaun Poh, executive director of capital markets at C&amp;W. The site for sale is the only commercial site available on the market in the area, and when completed, it would cater to more than 17,000 households around the new and existing residential developments in the area, he adds. The tender closes on Jan 8 2019.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/commercial-site-paya-lebar-central-sold</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-building-tai-seng-sale-23-mil</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A 99-year commercial site at Paya Lebar Road/Sims Avenue closed its tender on 31st March 2015 with a total of 6 bids received. The land parcel was awarded on 1st April 2015 to its highest bidder, Roma Central Pte Ltd, Milano Central Pte Ltd and Verona Central Pte Ltd, at a tendered sale price of $1,671,688,888 or $942.55 psf ppr. All 3 entities are related to Australian developer Lend Lease, the developer of the third biggest retail shopping mall in Singapore, JEM. It has been reported that 30% of the joint venture will be owned by Land Lease whereas the remaining 70% will be owned by Land Leases investor partners. Comprising of 4 plots, 2 land parcels and an underground area and an airspace, the maximum gross floor area (GFA) of the site is 164,794 sqm of which the maximum area for retail usage is capped at 39,000 sqm and at least 90,000 sqm of the gross floor area must be for office use. A maximum of 440 residential units (including Serviced Apartment) are allowed in the development. Strata subdivision for the commercial component is capped at 5 lots for office GFA and 3 lots for the remaining GFA such as retail, F&amp;B etc. This is the second of the 3 parcels that will be pivoting the development of Paya Lebar Commercial Hub as part of the governments decentralization strategy to develop commercial hubs at the city fringes. The first land parcel, currently occupied by Paya Lebar Square, was sold under the Government Land Sales (GLS) Programme in April 2011 to a joint venture company comprising Guthrie (PLC) Pte Ltd, Siong Feng Development Ltd and Sun Venture Commercial Pte Ltd. at a tendered price of $585,586,000 or $872.15 psf ppr. The Paya Lebar Square comprises 556 office units and 159 retail stalls. The office units were launched for sale in December 2011 and has sold 97% as of April-2014. Based on URA data, the average launch price is $1,777.7 psf. The retail component is retained by the developer and is reportedly 82% leased as of April 2014.      Land Parcel</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/commonwealth-towers-principal-garden-benefit-launch-queens-peak</t>
+          <t>https://www.edgeprop.sg/property-news/inside-48-mil-copper-house</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Queens Peak has been drawing crowds to its sales gallery and show flats since the project previewed on Oct 22 and 23. When the project was launched for sale on Nov 5, it moved 242 units by 5pm. Over the weekend of Nov 5 and 6, the developer sold 250 out of a total of 736 units, achieving 34% sales. The average price of units sold was $1,632 psf. One-bedroom units of 431 sq ft are priced from $680,000. Hao Yuan Investment, the developer of Queens Peak, purchased the 99-year leasehold site on Dundee Road in June last year for $483.2 million ($871 psf per plot ratio). The site sits adjacent to the Queenstown MRT station, and the developer will have a direct link from the overhead bridge of the station to Queens Peak, says MCC Land, the project manager. According to property agents, the launch of Queens Peak has stirred interest in neighbouring projects with unsold units, especially the Commonwealth-Alexandra neighbourhood between the Queenstown and Redhill MRT stations.  The crowd at Queens Peak on balloting day on Nov 5  Next door to Queens Peak is Commonwealth Towers, an 845-unit, 43-storey twin tower project by Hong Leong Holdings. Launched in May 2014, the 99-year leasehold private condo saw 175 units snapped up on the first day of sales, at prices ranging from $1,635 to $1,690 psf. As at end-September, the project had sold 428 units (50.7%). Having sold just two units in September, Commonwealth Towers saw at least 13 units sold in October, based on caveats lodged. Prices of units sold in October ranged from $1,530 to $1,806 psf. Units sold ranged from one-bedders of 441 sq ft priced at $788,200 ($1,786 psf) to three-bedders of 904 sq ft, for $1.47 million ($1,621 psf). Commonwealth Towers was not the only one to benefit from the launch of Queens Peak. Principal Garden, located on Prince Charles Crescent, off Alexandra Road, was another beneficiary. Having sold 14 units in September at a median price of $1,651 psf, it moved a similar number of units in October, based on caveats lodged. Units at Principal Garden sold in October ranged from $1,574 psf for a four-bedroom fourth-floor unit to $1,730 psf for a 797 sq ft, two-bedroom unit. Based on caveats lodged as at Nov 1, 326 units, or 49% out of a total of 663, had been sold. The project is jointly developed by UOL Group and Kheng Leong Co. Across the road from Principal Garden is Wing Tai Holdings 373-unit Ascentia Sky, completed in 2013. The 99-year leasehold condo comprises a single 45-storey tower. The latest transaction at Ascentia Sky was of a 1,475 sq ft, three-bedroom unit sold for $2.15 million ($1,458 psf), according to a caveat lodged on Oct 27. The unit was first purchased by the buyer for $2.14 million ($1,453 psf) in April 2011. Both the buyer and seller are HDB upgraders. Besides Principal Garden and Ascentia Sky, the Alexandra neighbourhood also saw the recent completion of the 508-unit Echelon. Next door to Echelon is the 429-unit Alex Residences by United Industrial Corp, which is over 65% sold and expected to be completed next year. The most recent transaction at the 45-storey tower was for a 657 sq ft, two-bedroom unit on the 33rd floor for $1.37 million ($2,079 psf), according to a caveat lodged in October. Next to Principal Garden is also the 469-unit The Crest by Wing Tai Holdings. The 99-year leasehold private condo is expected to be completed sometime next year. The project has sold about 145 units to date, with the latest transaction prices ranging from $1,726 to $1,775 psf, based on caveats lodged as at end-October.  This article appeared in The Edge Property Pullout, Issue 754 (Nov 14, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/condos-1-mil-15-mil-price-range</t>
+          <t>https://www.edgeprop.sg/property-news/ioi-offers-257-billion-central-boulevard-white-site</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Private homes priced between $1 million and $1.5 million were the most sought-after among the respondents polled in a home ownership aspiration survey conducted jointly by Knight Frank andThe Edge Propertyrecently. An analysis of URA caveats for private non-landed homes also confirms the trend. Condominium units and apartments priced between $1 million and &lt;$1.5 million accounted for 37% of the caveats lodged so far this year, followed by those in the $500,000 to &lt;$1 million price range. Respondents also expressed a preference for new homes. Thirty per cent preferred to purchase uncompleted homes, while 28% would go for completed homes that are less than five years old. Respondents ranked proximity to the city centre and a good range of facilities as the two most important criteria in selecting a home. The Edge Propertyhas compiled a list of condos that match respondents criteria. These condos  shoebox units were excluded  have average transacted prices so far this year that fall within the sweet spot of $1 million to $1.5 million. Moreover, the list comprises condos with at least 150 units to ensure the developments are of substantial enough size to offer a good range of facilities. The condos are located in the cityfringe area, which offers a good balance between proximity to the city centre and affordability.  Sims Urban Oasisby GuocoLand is located one stop away from the Paya Lebar MRT station and five stops away from the Raffles Place MRT station  Sims Urban Oasisis a 1,024-unit condominium by GuocoLand. The development sits on a 2.4ha site located about 400m from the Aljunied MRT station and in the vicinity of the upcoming Mattar MRT station of the Downtown line. Sims Urban Oasis was launched in February 2015, when 112 units were sold at a median price of $1,397 psf. The strong sales momentum has continued, with an average of 31 units sold monthly since the launch. Based on URA caveat data as at Oct 10, 180 units have been sold so far this year at an average price of $1,365 psf. Transacted prices so far in 2016 have ranged from $666,660 to $733,000 for one-bedroom units, $840,000 to $1.12 million for two-bedroom units, $1.19 million to $1.38 million for three-bedroom units and $1.32 million to $1.6 million for four-bedroom units. A total of 227 units were sold at a median price of $1,440 psf whenThe Poiz Residenceswas launched in November 2015  The Poiz Residencesis a mixed-use development by MCC Land. It is adjacent to the Potong Pasir MRT station and comprises 731 residential units and 84 shops. A total of 227 residential units were sold at a median $1,440 psf when it was launched in November 2015. The average transacted price so far in 2016 is $1.3 million, or $1,346 psf. Based on the latest URA developer sales data, there are still 189 units available for sale.  Thomson Impressionsis located near Ai Tong School and comprises 288 units  At Thomson Impressions, 80 units were sold at a median price of $1,399 psf when it was launched in October 2015. The 288-unit development is located near a popular primary school, Ai Tong School, and surrounded by three parks  Bishan Park, Lower Peirce Reservoir Park and MacRitchie Reservoir Park. Units sold so far this year have averaged $1.33 million, or $1,411 psf. Some 115 units are still available for sale, according to the latest URA developer sales data.  WhenGem Residenceswas launched in May, 312 units were sold at a median price of $1,431 psf  Located about 500m from the Braddell MRT station,Gem Residencesis a 578-unit condo jointly developed by Gamuda, Evia Real Estate and Maxdin. When it was launched in May, 312 units were sold at a median price of $1,431 psf. The average transacted price so far this year is $1.02 million, or $1,420 psf. A total of 256 units are still available for sale at the development, based on the latest data from URA. The average price for units sold atSturdee Residencesso far this year is $1.17 million, or $1,539 psf  Sturdee Residencesis located in the vicinity of the Farrer Park MRT station and City Square Mall. The 305-unit condo is developed by Sustained Land. A total of 126 units were sold at a median price of $1,620 psf when the condo was launched in April. The average price for units sold so far this year is $1.17 million, or $1,539 psf. Based on the latest developer sales data released by URA, the developer has 120 remaining units available for sale.  The average transacted price atThe Venue Residencesso far this year is $1.36 million, or $1,401 psf  The Venue Residencesis a mixed-use project by City Developments and Hong Leong Holdings. The 266-unit development is located about 300m from the Potong Pasir MRT station. The average transacted price so far this year is $1.36 million, or $1,401 psf. Based on URA developer sales data, the developer has 121 remaining units available for sale.  Monthly rents atEight Riversuitesso far this year have averaged $2,199 for one-bedroom units and $2,652 for two-bedroom units  AtEight Riversuites, located about 500m from the Boon Keng MRT station, 192 units were sold at a median psf price of $1,340 when it was launched in May 2012. Developed by United Engineers Developments, Eight Riversuites comprises 843 non-landed and 19 strata landed homes. Prices have averaged $1.41 million, or $1,272 psf, so far this year. According to the developer, there are 15 strata landed units between 2,800 and 3,000 sq ft available for sale. Monthly rents at Eight Riversuites so far this year have averaged $2,199 for one-bedroom units and $2,652 for two-bedroom units. The Shore Residenceswas completed in 2014 and comprises 408 units  The Shore Residencesis a 408-unit condo located 500m from the upcoming Marine Parade MRT station. The development by Far East Organization was completed in 2014. Prices have averaged $1.46 million, or $1,498 psf, so far this year. Average monthly rents at The Shore Residences so far this year are $2,932 for one-bedroom units and $3,978 for two-bedroom units.  Prices atRegent Residenceshave averaged $1.06 million, or $1,355 psf, so far this year  Completed in 2015,Regent Residencesis a 180- unit freehold development located about 600m from the Boon Keng MRT station. Prices have averaged $1.06 million, or $1,355 psf, so far this year. Monthly rents so far this year have averaged $1,987 for one-bedroom units and $2,580 for two-bedroom units.  Completed in 2014,Nin Residenceis located across the road from the Potong Pasir MRT station  Nin Residenceis a 219-unit development by Qingjian Realty. It is located across the road from the Potong Pasir MRT station and was completed in 2014. Based on transactions so far this year, the average price is $1.48 million, or $1,288 psf. Monthly rents so far this year have averaged $2,223 for one-bedroom units and $2,905 for two-bedroom units. All the units at Alexis were snapped up in less than a fortnight when it was launched in 2009  Completed in 2012, Alexis is a freehold mixed-use development comprising 293 residential units and 21 shop units. The development, jointly developed by Fission Group and Yi Kai Group, is located about 500m from the Queenstown MRT station. All the units at Alexis were snapped up in less than a fortnight when it was launched in February 2009. Prices have averaged $1.1 million, or $1,268 psf, so far this year. Average monthly rents so far this year are $2,637 for one-bedroom units and $3,343 for two-bedroom units.  Average monthly rents at 8@Woodleigh are $1,968 for one-bedroom units and $3,050 for two-bedroom units  8@Woodleigh is located within walking distance of the Woodleigh MRT station. The 330-unit development by Frasers Centrepoint was completed in 2012. Based on transactions so far this year, the average price is $1.22 million, or $1,247 psf. Monthly rents so far this year have averaged $1,968 for one-bedroom units and $3,050 for two-bedroom units.  A 1,109 sq ft unit at Beacon Heights changed hands at $1 million, or $902 psf, in September  Located on Mar Thoma Road near Whampoa, Beacon Heights is a 999-year leasehold development completed in 2012. Prices have averaged $1.1 million, or $1,024 psf, so far this year. Monthly rents so far this year have averaged $2,123 for one-bedroom units and $2,658 for two-bedroom units. Read more aboutSims Urban Oasis. This article appeared inThe EdgeProp PulloutIssue 750 (Oct 17, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/conservation-shophouse-market-abuzz-again</t>
+          <t>https://www.edgeprop.sg/property-news/iwg-banks-multi-brand-strategy-growth</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Over the past year, the conservation shophouse segment has seen a flurry of activity. The total sales value of conservation shophouses that changed hands tripled from $59.92 million in 1Q2016 to $182.54 million in 2Q2016, and rose a further 14.7% to $209.32 million in 3Q2016. Driving this demand were boutique funds, family offices and foreign high-net-worth individuals looking for alternative investment asset classes that are safe havens amid global economic uncertainty. The biggest deal in 2016 so far was the $81.4 million purchase of a portfolio of seven shophouses by boutique property fund 8M Real Estate from veteran international property investor Stanley Quek. The deal was conducted in April and comprised five shophouses at 15-23 Tanjong Pagar Road for $57.40 million; the shophouse at 18 Genmill Lane for $11 million; and 71 Neil Road for $13 million. This row of shophouses on Tanjong Pagar Road changed hands for $57.40 million  Who are the buyers? Set up in 2014,8M Real Estateis said to have acquired 15 shophouses worth $200 million over the past two years. These include 37 Craig Road, which it acquired in April for $6.5 million; 31 Hong Kong Street, purchased in July for $14.45 million; and 22 Genmill Lane, which it picked up for $14.25 million in October 2014. Its maiden acquisition was a row of five shophouses at 112 to 116 Amoy Street, for which it paid $50 million two years ago. In addition to boutique property funds, shophouses have attracted even foreign billionaires such as Ricardo Portabella Peralta, CEO of Luxembourg-based Ventos, which invests in companies involved in the real estate, food processing, venture capital, financial holdings, energy and environment industries. Ventos has operations in Europe, North America and Asia. Peralta is said to have purchased five shophouses in a period of just 12 months. The spending spree started with the acquisition of two adjoining shophouses at 120 and 122 Telok Ayer Street for $18.2 million in October 2015, followed by two more shophouses at 20 and 37 Duxton Road for $13.7 million a month later, and a shophouse at 7 Craig Road for $12.5 million last December. In March this year, he paid $20.25 million for a three-storey shophouse at 83 Amoy Street. The Leong family that started the Axe Brand medicated oil is said to have paid $25 million for two shophouses on Bukit Pasoh Road in Chinatown in September. And the family that owns Hong Kong-based developer Wincome Group is said to have acquired three adjacent shophouses in Joo Chiat for $23 million last December. Heritage value Conservationshophousesare attractive investments, owing to their heritage value. Built from the early 1800s to early 1900s, these shophouses are generally two to three storeys high and formed much of the pre-war urban fabric of Singapores old city centre and other parts of the island. Rapid urbanisation has resulted in many of these shophouses being torn down to make way for skyscrapers. Today, only 6,500 have survived, and they have been gazetted for conservation by URA. Owing to the limited supply, conservation shophouss offer good capital appreciation potential over the long term. This has resulted in some extraordinary gains for investors. For instance, the five conservation shophouses on Amoy Street that were purchased for $34.43 million in June 2011 changed hands for $50 million in 2014 when 8M purchased them. This means a capital appreciation of 45.2% over a three-year period. Likewise, 7 Craig Road was purchased for $12.5 million in December last year by Peralta. Prior to that, the unit traded for $7.88 million in May 2013. Investors can further unlock the value of their shophouses by repositioning the asset, changing the trade mix or refurbishing the interiors. Some shophouses also offer development opportunity via a multi-storey extension in the rear. Steady income stream Conservation shophouses have the potential to generate a steady income stream for investors as they are supported by healthy leasing demand. Ground-floor shophouses that have prominent frontage are sought after by niche retailers and F&amp;B operators. The upper floors of these shophouses tend to attract people in the creative industries, such as architectural firms and interior design and startup companies. In recent years, conservation shophouses have also drawn buyers as they are not subject to additional buyers and sellers stamp duties. This year saw more owners willing to put their properties on the market, which contributed to the flurry of activity. However, before buying a conservation shophouse, investors should do their homework and study the conservation, planning and development guidelines of the area in which the property is located. Tay Huey Ying is head of research at JLL Singapore. This article appeared in The Edge Property Pullout, Issue 752 (Oct 31, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/conservation-shophouses-geylang-and-joo-chiat-sale</t>
+          <t>https://www.edgeprop.sg/property-news/just-sold-caribbean-keppel-bay-unit-sold-145-mil-profit</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SINGAPORE (EDGEPROP) - Two sets of conservation shophouses in Geylang and Joo Chiat are up for sale. They are a row of seven freehold adjoining conservation shophouses in Geylang, and two freehold adjoining shophouses at Joo Chiat Road. Both sets of shophouses are up for sale via expression of interest (EOI). The guide price for the seven shophouses is about $40 million to $42 million, while the guide price for the two tenanted shophouses is at $7 million to $7.5 million. Located at the corner of Geylang Road and Lorong 14 Geylang, the row of seven shophouses is close to Aljunied MRT Station. They have a total land area of 10,520 sq ft and gross floor area (GFA) of about 18,000 sq ft. There will be no additional buyers stamp duty and sellers stamp duty payable. Foreigners and companies are also eligible to purchase. The guide price for the seven shophouses in Geylang is about $40 million to $42 million (Credit: Knight Frank Singapore)  The shophouses are currently fully tenanted and comprise a corner coffeeshop, mobile phone retailer, massage parlour and other retail trades. The properties are suitable for F&amp;B outlets and retail uses on the ground floor, while the upper floors can be designated for office use. Meanwhile, near the junction of Joo Chiat Road and Koon Seng Road, the two adjoining shophouses have a land area of 2,393 sq ft and a GFA of about 4,600 sq ft. The properties are near Parkway Parade, 112 Katong, Kinex, Paya Lebar Square and SingPost Centre. For price trends, recent transactions, other project info, check out theGeylang RoadandJoo Chiat Roadproject research page  The guide price for the two tenanted shophouses at Joo Chiat is at $7 million to $7.5 million. (Credit: Knight Frank Singapore)  Both sets of shophouses are zoned for commercial use with a plot ratio of 3 under the 2014 Master Plan. The EOI for the two sets of shophouses  both marketed by Knight Frank Singapore  will close at 3pm on Oct 3, 2019. Check out the latest listings nearGeylang Road,Joo Chiat RoadandMRT Stations Read also: Three-storey conservation shophouse in Chinatown for sale at $8.5 milSix shophouses on Kampong Bahru Road for sale from $39.6 milSix freehold shophouses in Joo Chiat priced from $32 mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/consider-these-when-buying-shoebox-units</t>
+          <t>https://www.edgeprop.sg/property-news/karamjit-singh-leave-jlls-residential-team</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Using new sales caveats from 2012 onwards as a proxy, there are at least 9,600 shoebox units island-wide that have recently been, or will soon be, completed. Geylang has the highest supply pipeline with at least 1,200 units. However, its proximity to the CBD, Paya Lebar growth corridor and industrial areas in the East mitigates the risk of severe rental downside. However, shoebox rents in the North-East Region will be under pressure given at least 2,000 shoebox units have recently been, or will soon be, completed. While the development of the Punggol Creative Cluster and Learning Corridor will boost rental demand, competition for tenants will be stiff. In addition, there will a bumper supply of new HDB flats that will soon fulfil their five-year Minimum Occupation Period, which will compete in the rental market. The full impact on shoebox rents, as a result, has yet to be felt.  Estimated number of shoebox units that have recently been, or will soon be, completed Graphic by Kim SY  Projects in the pipeline with a substantial number of shoebox units include Midtown Residences, Parc Centros, Riversails, The Promenade @ Pelikat and Vibes@ Upper Serangoon. The vacancy rate for apartments and condominiums in the North-East Region stood at 12.3% and 11.9% respectively as at 1Q2016. The East Region trailed closely with at least 1,500 shoebox units that have recently been, or will soon be, completed. The bulk of these are located in Pasir Ris from projects such as DNest, Ripple Bay and The Inflora. The vacancy rates for apartments and condominiums in the East Region stood at 8.7% and 10.4% respectively as at 1Q2016.  Shoebox rents have fallen by more than 20% since their peak Landlords of shoebox units have lost about $600 per month, or a quarter of their rental income, as rents plunged from their peak in 3Q2013. Monthly rents for shoebox homes, defined here as those measuring 500 sq ft or less, dived 23% from $2,792 in 3Q2013 to $2,139 on average in 1Q2016. The analysis is based on rental data mined by the URA. In contrast, the average rent for all private, non-landed homes has fallen by a slower 12% over the same period. Shoebox rents have also performed worse than large units with four bedrooms and above. The average rent for the latter has fallen by a slower rate of 15%. Meanwhile, the average rent for two-bedroom units has declined by around 13%. For investors, this means having 1.6 percentage points shaved off their rental yields. Assuming they purchased the units direct from the developer at $1,327 psf, which was the median price for shoebox homes in 2010, they would have enjoyed 6.2% gross rental yields when the units were completed and rented out in 2013. However, todays rent would knock the yields down to 4.6%.   Mass-market segment led rental fall Although a 4.6% gross rental yield is mouth-watering, potential investors should note that the performance is not uniform across market segments. The mass-market segment, or Outside Central Region, has performed the worst by far. Shoebox rents in this segment tumbled 24% from $2,502 per month in 3Q2013s peak to $1,906 psf in 1Q2016. The most compelling reason for this is competition from HDB flats. For the same rent, or around $1,900 per month, tenants have the option of renting three-room HDB flats in mature estates, which include Ang Mo Kio, Bishan, Bukit Merah, Clementi, Kallang/Whampoa, Marine Parade, Queenstown, Serangoon and Toa Payoh. The other option is a four-room HDB flat in non-mature estates.  In the high-end segment, or Core Central Region, shoebox rents declined by a smaller percentage of 17%, from $3,269 per month in 1Q2013 to $2,698 in 1Q2016. Those in the city fringe, or Rest of Central Region, fell 21% from $2,675 to $2,103 per month over the same period. On a y-o-y basis, the high-end segment performed the worst, with shoebox rents falling 8% compared with 4% in the city fringe and 5% in the mass market. This is likely due to a temporary spike in the supply of shoebox units in recent years. The steep rental fall was confined to just a few projects. Shoebox rents at Illuminaire on Devonshire and Robertson Edge fell by a double-digit percentage owing to competition from newer projects in their vicinity including Espada, RV Edge and Vivace. In the CBD, shoebox rents at The Clift also fell steeply, presumably because of competition from Skysuites @ Anson, which was completed in 2014. Owing to a limited supply pipeline, we expect this trend to reverse, with the high-end segment outperforming other segments in the coming years. Q-o-q, shoebox rents held firm in 1Q2016 with a 0.1% increase in the high-end segment, but dipped 1.1% in the city fringe and 3.4% in the mass market. For tenants, this poses an opportunity to live in the prime districts. In 2013, a $2,300 rental budget afforded them shoebox units in Telok Kurau or Kovan areas. Today, it is possible to rent units atLoft @ Stevens,RV EdgeorWilkie 80at similar or slightly higher rents.  This article appeared in The Edge Property Pullout, Issue 725 (April 25, 2016) of The Edge Singapore. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/contrasting-fortunes-punggol</t>
+          <t>https://www.edgeprop.sg/property-news/kingsford-bets-riverfront-location-upper-serangoon-view</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Three sellers in Punggol experienced contrasting fortunes recently. At Watertown, a 1,216 sq ft, three-bedroom unit was sold in a sub-sale on June 8 for $1.39 million, or $1,141 psf. The price was lower than what the seller had paid the developer in 2012  $1.41 million, or $1,157 psf. The transaction, therefore, resulted in a loss of about $19,000. The sellers stamp duty (SSD) was not applicable in this case as the holding period had just crossed four years. There have been 16 sub-sale caveats at the 992- unit project so far, but we can only trace the previous caveats for 10 of them. Including SSD, six of the 10 sellers incurred losses ranging from $19,000 to $246,000. On the other hand, four sellers reaped profits ranging from $34,000 to $191,000. In contrast, two sellers at nearby A Treasure Trove made profits exceeding $100,000 in June. The two units sold had been held for less than five years. They fetched $1,020 and $1,081 psf respectively, a tad lower than the Watertown unit. However, the sellers had paid $876 and $920 psf for their units, which they bought direct from the developer in October 2011.  Two sellers at A Treasure Trove reaped profits while a seller at Watertown incurred a loss in June  There have been 67 sub-sale transactions at the 882-unit A Treasure Trove, but we can only trace the previous caveats for 61 of them. All 61 subsale transactions were profitable, with the gains averaging $146,000. If SSD is included, one deal was in the red. A Treasure Trove was launched in September 2011 and 683 units were sold at a median price of $915 psf. Watertown was launched in January 2012 and 770 units were sold at a median price of $1,169 psf. Watertown is part of a mixed development comprising Waterway Point, a suburban mall with a net lettable area of 370,824 sq ft. It is connected to the Punggol MRT station. A Treasure Trove is located within walking distance of the Punggol MRT station. In another part of District 19, a 1,496 sq ft low-floor unit at Kovan Residences was sold at 2011 prices, or $989 psf. Kovan Residences is a 99- year leasehold 521-unit condominium located beside the Kovan MRT station. In the Core Central Region, an 861 sq ft high-floor unit at The Sail @ Marina Bay was sold for a price that is on a par with 2008 levels, or $1,661 psf. In July 2008, an 861 sq ft unit directly two floors below found a buyer at $1,626 psf. According to Daphne Lean, ERAs district division director, interest in the development comes mainly from investors.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/cushman-wakefield%E2%80%99s-dennis-yeo-set-play-%E2%80%98premier-league%E2%80%99</t>
+          <t>https://www.edgeprop.sg/property-news/kingsford-waterbay-sells-140-units-launch-weekend</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Having joined Cushman &amp; Wakefield (C&amp;W) in mid-December last year as chief executive for Singapore and Southeast Asia, Dennis Yeo believes the firm is ready to compete in the premier league and become the top real estate services firm in the region. For now, C&amp;W ranks third among the global real estate advisory firms. Listed on the New York Stock Exchange (NYSE) in August 2018, it had a market capitalisation of US$3.86 billion ($5.27 billion) as at June 11, with FY2018 annual revenue of US$8.22 billion. The worlds biggest and second biggest corporate real estate advisory firms today are CBRE and JLL respectively. The NYSE-listed CBRE had a market cap of US$16.71 billion at June 11, with annual revenue of US$21.34 billion as at end-FY2018. The NYSE-listed JLL, on the other hand, had a market cap of US$6.10 billion at June 11, with annual revenue of US$16.32 billion as at end-FY2018.  Yeo: We are ready to compete in the premier league and become the top real estate services firm in the region (Credit: Albert Chua/EdgeProp Singapore)  In 1Q2019, CBREs total fee revenue made up US$2.43 billion. Meanwhile, at JLL, fee revenue for 1Q2019 was US$1.32 billion. Over the same three-month period from January to March, C&amp;Ws total fee revenue was US$1.37 billion. The biggest contributor to fee revenue for C&amp;W in 1Q2019 was property and facility management at US$707 million or 51.5% of the total. Leasing contributed US$373 million (27.2%), followed by capital markets with US$191 million (13.9%). The Asia-Pacific region accounted for US$251 million (18.3%) of C&amp;Ws fee revenue in 1Q2019, and was second only to the Americas, which contributed US$937 million (68.3%). EMEA (Europe, the Middle East and Africa) generated US$184 million or 13.4% of total fees in 1Q2019.  Untapped potential At C&amp;W, Yeos focus is on growing the transactional business, namely leasing and capital markets, both in Singapore and Southeast Asia. He intends to position Singapore as the centre of excellence for the region in terms of leasing, sales and capital markets. He is also looking at extending the scope and strengths of C&amp;W Services integrated facility services, engineering solutions and energy management to a wider client base across multiple sectors. Prior to joining C&amp;W, Yeo was the managing director for industrial and logistics at CBRE since September 2015. Before that, he had spent 22 years at Colliers International, where he occupied a number of key positions, from country head for Singapore to executive committee member of Colliers Asia leadership and head of Asia for capital markets, investment services and industrial services. I thought I would probably retire in Colliers as I had spent 22 years there, says Yeo, who is in his mid-50s. But I found my way to CBRE, where I was looking after the industrial and logistics business for Asia. At C&amp;W, what excites him is the untapped potential. Says Yeo: As a full-service real estate company with a regional and global platform, we are well-positioned to offer services and solutions at every point of the real estate cycle. He sees opportunity in competing across the entire real estate services platform  be it in brokerage, project and development services or facilities management. The growth trajectory for our business is strong, adds Yeo.   Significant capital market deals brokered by C&amp;W included the sale of Ascott Raffles Place Singapore for $353.3 million in January 2019  Capital market deals In Singapore, significant capital market deals brokered by C&amp;W included the sale of Ascott Raffles Place Singapore for $353.3 million in January 2019. C&amp;Ws capital markets team led by executive director Shaun Poh acted on behalf of the seller, Ascott Residence Trust Management. The buyer of Ascott Raffles Place was Cheong Sim Lam or SL Cheong, the developer of several residential projects, including Robinson Suites on Robinson Road. He previously owned 137 and 139 Cecil Street. C&amp;W also brokered the sale of the office development at 7 and 9 Tampines Grande to a joint venture between Evia Real Estate and Metro Holdings for $395 million in mid-April, followed by the sale of Realty Centre for $148 million a few days later. Realty Centre marked the first commercial collective sale in 2019, and the property was sold to Singapore-listed The Place Holdings. If we can harness the capabilities of our Singapore capital markets team with our regional and global infrastructure, it will be very powerful because Singapore is a huge base for outbound capital, says Yeo. He points to the likes of ARA Asset Management, Ascendas-Singbridge and CapitaLand, Frasers Property, GIC and Temasek Holdings as Singapore-based entities which have been aggressively acquiring real estate assets and portfolios around the world. These are some of our clients and its a great opportunity for our capital markets team, Yeo adds.  Market consolidation Consolidation has been taking place in the real estate services industry, with 12 major merger and acquisition (M&amp;A) deals across the globe in the span of 16 years from 2002 to 2018. (See chart below.)  M&amp;A deals over the years: 2002-2018 Credit: 2019 CBRE Investor Day Presentation, April 2019  Even the C&amp;W of today is the result of an M&amp;A between the firm and DTZ in a deal completed in September 2015. With consolidation, movement of top executives among the real estate advisory firms has been rampant. Yeo, for instance, replaced former C&amp;W managing director for Singapore, Stephen Saul, who left in 2018 and has since retired. He assumed the position in February 2016. Saul is said to have over 30 years experience in the real estate industry, and was previously with JLL, where he was managing director for Korea and New Zealand. Saul in turn had replaced Toby Dodd, the previous managing director for C&amp;W Singapore, following the latters appointment as C&amp;Ws executive managing director of account management for the Tri-State and East Regions in the Americas for Global Occupier Services (GOS). The GOS business at C&amp;W, whose Asia-Pacific team is based in Singapore, provides advice and solutions to global and regional MNCs across the entire real estate spectrum including transaction management, facilities management and workplace strategy. In May, C&amp;W announced the appointment of Cameron Ahrens as head of integrated facilities management (IFM) for Asia-Pacific. Prior to joining C&amp;W, Ahrens was with Brookfield Global Integrated Services (BGIS) where he was head of facilities management for Asia. Before that, Ahrens had held senior positions in the occupier business at CBRE and JLL respectively. Our regional GOS team partners with MNC occupier clients where C&amp;W is the preferred or sole provider for their real estate needs across multiple markets, whether its integrated portfolio management or providing advice on their relocation or expansion on a regional or global platform, says Yeo. These global and regional accounts provide downstream business for C&amp;Ws local offices, such as the leasing of commercial or industrial space as well as sale of these spaces.  Realty Centre marked the first commercial collective sale in 2019, and the property was sold to Singapore-listed The Place Holdings (Credit: C&amp;W)  Developing the hunter instinct Beyond relying on GOS to push business to the Singapore and other regional offices, Yeo believes it is important to hunt for business ourselves in order to grow the transaction business. He is interested in growing the cross-border business, particularly from Chinese manufacturing companies looking to relocate their factories in Vietnam or other markets in Southeast Asia. Thats my passion, says Yeo. During his tenure at Colliers, he turned the international firm into a leading consultancy in the industrial sector in Singapore. In July 2015, CBRE recruited five of Colliers industrial services team, including Brenda Ong who is now CBREs executive director for advisory and transaction services  industrial and logistics. In February 2015, a group of three from Colliers office tenant representation team led by Marcus Loo left for Savills. Loo was appointed CEO of Savills Singapore in January this year. Yeo is proud of the talent that he has groomed during his career as a real estate professional. The business is all about hunting, pitching and winning, and ensuring our clients receive the best service and solution, he says. He wants to develop and sharpen that hunter instinct in the transaction business teams in C&amp;W in Singapore and the region. Research and analysis have also become an important competitive tool in the industry. C&amp;W beefed up its Asia-Pacific research team with two new appointments announced on June 11. James Shepherd, previously C&amp;Ws managing director  research, for Greater China, will take on the role of head of research for Asia-Pacific. Meanwhile, Dominic Brown will assume the role of head of insight and analysis for Asia-Pacific. Having been in the industry for close to 30 years, Yeo believes in looking after our people - the key pillars of our business. He adds: We are a service business and it is critical that we continue to provide a conducive and engaging environment so our people stay passionate and committed to delivering their best, which then translates into better outcomes for them, our clients and our business. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/data-centres-alternative-investment</t>
+          <t>https://www.edgeprop.sg/property-news/landed-homes-below-2-million</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The proliferation of mobile devices and cloud-based e-commerce, as well as social media platforms such as WhatsApp, Facebook and Instagram, has led to a surge in demand for data storage space. And it is not just technology companies that are jumping on the bandwagon, but also property developers who see the opportunity in providing the properties to host these data centres. Keppel launched the first data centre real estate investment trust in the country called Keppel DC REIT, which was listed on the Singapore Exchange in December 2014. US-based data centre REIT Digital Realty may be listed on the New York Stock Exchange, but it also owns three properties in Singapore that will house data centres. Other players are also getting into the act. For example, Ho Lee Construction, Evia Real Estate and their partners entered the data centre hosting business five years ago when they jointly purchased the former Seagate Technology building at 7000 Ang Mo Kio Avenue 5 for $91.5 million. They spent another $10 million retrofitting the one million sq ft building to turn it into an ideal environment for hosting data centres. The property has another 41 years left on its original 60-year lease. Michael Tan, executive director of Ho Lee Construction, realises the potential for hosting data centres. In the past, we used to share one photo, but now with WhatsApp, Viber and Instagram, we can share photos and videos hundred times over, he explains. This means there is a need for more remote data storage space.  Ho Lee Construction and its partners bought the former Seagate factory for $91 million   Opportunity The first data centre operator to enter the newly refurbished space at the premises on Ang Mo Kio Avenue 5 was US-based data centre co-location operator IO, which took up 177,000 sq ft. IO started operations in Singapore in 2013 after it invested more than $30 million in the 177,000 sq ft data centre facility, and spent another $5 million to enhance the security around the building premises. Security is an important issue as IOs clients include MNCs such as Allianz, Goldman Sachs and LexisNexis. The clients of data centre operators, especially MNCs, will want to lock in their leases with the operator for at least five to 10 years, with some even up to 15 years, says Tom Duncan, CBREs executive director on data centres. Meanwhile, the data centre operators, such as IO, tend to lock in their leases for at least 30 years, says Tan. Therefore, this makes data centre hosting facilities attractive as an investment, given the stability of rental income. Gross rental yields tend to be lower at 5% to 6%, compared with the 7% to 8% yield for warehouse or factory space. However, the catch is that leases for warehouse and factory space tend to be shorter, with a typical warehouse lease averaging two to three years, and factory space five to seven years, he adds. Besides IO, other companies that have located their data centres within the building on Ang Mo Kio Avenue 5 include Singapore Power and listed property group Wing Tai Holdings. Wing Tai has even taken up some space in the building to store its retail merchandise. Only 20% of the one million sq ft space in the building is dedicated to hosting data centres. Another 60% of the space has been leased to other tenants such as Seagate, which continues to have a presence there; mobile phone camera lens maker Heptogen; and Evias Business Continuity Planning, a disaster recovery business. So far, the building has an occupancy rate of 80%, with annual rents of $20 million, of which data centre hosting constitutes 20% to 25%, or $4 million to $5 million. Based on the purchase price and renovations, the total cost of the building amounted to about $100 million. This means that net yield on the investment is about 15%, reckons Tan.  Tan: We are hoping to sell the building to someone who has the expertise, track record and capability to
-attract more data centre operators to locate their facilities here   Market size Total data centre co-location market revenue in Singapore is said to have grown 13% from US$963 million in 2014 to US$1.09 billion in 2015. It is projected to grow another 16% to US$1.26 billion ($1.69 billion) in 2016, according to the latest annual report on data centre supply released by Canada-based Structure Research in October 2015. According to Structured Research, there are 36 data centres in the East, with the two largest clusters in the Tai Seng/Ubi area comprising 11 facilities and the Chai Chee area with another six. In the West, there are 18 facilities, with the two largest clusters of seven data centres each at the International Business Park and in the Ayer Rajah/Science Park area. There are another three in Woodlands and one in the Yishun area. Combined, these co-location data centres occupy about two million sq ft of industrial space in 2014. According to CBRE Research, co-location data centres in Singapore increased from two million sq ft to three million sq ft in 2015. It is projected to grow to 4.8 million sq ft this year, and six million sq ft by 2017.  Are data centres the answer to oversupply in industrial space? The departure of some of the more labour-intensive manufacturing companies to lower-cost locations such as Malaysia, Indonesia and China has left an increasing number of industrial buildings and warehouses either unused or underutilised. The question is whether some of these industrial buildings and warehouses can be converted into data centres to meet the growing demand. According to Christine Li, head of research at Cushman &amp; Wakefield, not all factory or warehouse buildings can be converted for use by data centres. She sees a mismatch in terms of the quality of the buildings, such as the floor-to-ceiling height, floor loading factors and even floor layout. Some of these buildings are located in heavy industrial areas, which may not be ideal for data centre use, she adds. It worked five years ago when data centres were first set up in Singapore because they needed to start operations in the shortest possible time. Most of the older buildings do not have efficient space use, and it may be too costly for the owners to demolish and rebuild, observes Li. This does not preclude some data centre operators from setting up shop in refurbished old warehouses or industrial buildings. For example, Digital Realtys latest 177,000 sq ft, four-storey co-location data centre in the Loyang area used to be a warehouse. Digital Realty spent $200 million to rebuild half the building to maximise the gross floor area and install high-power cables, chilling units, unlimited power supply (UPS) backup power, standby generators, internet connection and security features.  Digital Realtys latest 177,000 sq ft, four-storey co-location data centre in the Loyang area used to be a warehouse Source: Digital Realty  An unoccupied 7,000 sq ft suite at Digital Realtys existing data centre building in Loyang  Blast-proof walls and standby power generators on Level 4 of Digital Realtys data centre in Loyang  The facility opened in June. It took us about 12 months to rebuild and refurbish this building compared to between 18 and 24 months to construct our facility in Jurong from ground up, says Omer Wilson, Digital Realtys marketing director for Asia-Pacific. Digital Realtys first facility, in Jurong, is a 370,000 sq ft building, while its third and upcoming facility is in Loyang. The new facility will also be a 370,000 sq ft, purpose-built data centre facility. Land cost is obviously at a premium here, says Wilson. It is getting harder to find land that is cost-effective to build on. We will be increasingly moving towards building conversions or buying existing data centre operators that own their premises to gain access to their assets.  Wilson: It took us about 12 months to rebuild and refurbish this building compared to between 18 and 24
-months to construct our facility in Jurong from ground up  In fact, Ho Lee and its consortium partners now see this as an opportune time to cash out. The group has already put their building on Ang Mo Kio Avenue 5 on the market. The indicative price tag is upwards of $250 million, or $300 psf of net lettable area. Why are they divesting now? We are hoping to sell the building to someone who has the expertise, track record and capability to attract more data centre operators to locate their facilities in the building in order to realise the buildings potential over the long term, says Ho Lees Tan.  This article appeared in The Edge Property pullout, Issue 741 (Aug 15, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/deal-watch-unit-aalto-market-1600-psf</t>
+          <t>https://www.edgeprop.sg/property-news/landed-houses-flipped-million-dollar-profits</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">A 1,550 sq ft, three-bedroom unit at Aalto has been listed for sale at $2.48 million ($1,600 psf) on TheEdgeProperty.com. The unit is said to be facing the greenery and landed area of Amber Road and Meyer Road, according to Jamie Goh, a property agent with PropNex Realty who is marketing the unit. The apartment is said to be currently tenanted at a monthly rent of $5,500 with the lease expiring in July 2018. This translates into a gross rental yield of 2.7%. Buyers have the option to purchase the unit with tenant in place or with vacant possession, says Goh. There is an early termination clause in the lease in the event that the buyer decides to purchase with vacant possession. Monthly rents for three-bedroom units of 1,500 to 1,600 sq ft are generally hovering around $5,455, according to leasing contracts on URA for the past six months (see table).   Aalto is a freehold high-end condominium on Meyer Road that was developed by Hong Leong Holdings  Aalto is a freehold high-end condominium on Meyer Road that was developed by Hong Leong Holdings and completed in 2010. The project is a redevelopment of the former Eastern Mansion, which was purchased en bloc, and an adjacent site. Aalto has twin 27-storey towers and a total of 196 units. The units are three- and four-bedroom apartments sized between 1,442 sq ft and 1,959 sq ft, respectively. There are also two penthouses in the development, the larger of which is a 6,168 sq ft unit on the 26th floor that was sold for $16.8 million ($2,724 psf) in February 2011. The other penthouse of 5,608 sq ft, also on the 26th floor, fetched $16.275 million ($2,902 psf) in March 2008 at the previous peak just before the global financial crisis. The highest psf price achieved at Aalto was for one of the sub-penthouses on the 25th floor. The 3,940 sq ft unit changed hands for $11.5 million ($2,919 psf) at the last peak in February 2013. The three most recent transactions at Aalto were for four-bedroom units of 1,959 to 2,024 sq ft, which were sold at $2.9 million ($1,480 psf) to $3.4 million ($1,735 psf) in the months of July to September, according to caveats lodged with URA Realis. The latest transaction of a three-bedroom unit at Aalto was for a 1,528 sq ft, mid-floor unit, which changed hands for $2.55 million ($1,668 psf) in July. The other three transactions of three-bedroom apartments at Aalto earlier this year were also of similar-sized units. They were sold at prices ranging from $2.3 million ($1,505 psf) to $2.57 million ($1,681 psf). The last time a bigger three-bedroom unit (1,550 sq ft) changed hands was in November last year, when a unit on the 20th floor was sold for $2.73 million ($1,761 psf), according to a caveat lodged then. In the future, homebuyers can look forward to the Tanjong Katong MRT station on the Thomson-East Coast Line that is expected to open in 2023. For more information, call marketing agentJamie Gohat9025 6772.   This article appeared in The Edge Property Pullout, Issue 750 (Oct 17, 2016) of The Edge Singapore. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/developer-slashes-prices-kingsford-hillview-peak</t>
+          <t>https://www.edgeprop.sg/property-news/lawrence-wong-urges-prudence-buyers-and-developers</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Following a three-month lull,Kingsford Hillview Peaksuddenly saw a spike in transactions. A 527 sq ft, one-bedroom unit and three 775 sq ft, two-bedroom units were sold. Prices of the units sold ranged from $682,000 ($1,293 psf) to$1.122 million ($1,448 psf), according to caveats lodged from July 5 to 12.  The developer of Kingsford Hillview Peak is offering discounts of 20% to 22% off the list price  To spur transactions in the development, the developer is offering a discount of 20% to 22% off the list price, starting from this month. Prior to that, units were sold at $1,300 to $1,400 psf. However, post-discount, the new selling price is around $1,200 psf, according to ERA real-estate agents who are marketing the project. The 512-unit private condominium by mainland Chinese developer Kingsford Development was launched in 2013. As at end-June, 172 units had been sold, according to URA data. The developer purchased the 99-year leasehold site in January 2012 for$243.22 million, or $638 psf per plot ratio (psf ppr), which is comparable to the $673 psf ppr paid by Far East Organization for an adjacent 99-yearleasehold site in 2011. The project has since been developed intoThe Hillier. Kingsford Development had snapped up the site at Hillview Rise, following the success of the launch of The Hillier in January 2012. Within a few weeks, 210 out of 333 units released were snapped up, at an average price of $1,174 psf. The Hillier, which was completed last year, consists of 520 units of SOHO-style residences sitting atop a double-storey retail and lifestyle mall called HillV2. The project is fully sold, and was completed last year. The last recorded transaction was in March last year, when an 818 sq ft unit on the seventh floor was sold for just over$1 million ($1,229 psf). One of the main draws of The Hillier and Kingsford Hillview Peak is the upcoming Hillview MRT station, which is scheduled to be completed by year-end, says Daniel Liew, an associate director at ERA Realty. HillV2is also a draw for those living in the neighbourhood and residents of Kingsford Hillview Peak will likewise benefit from the projects proximity to the shopping mall, which contains F&amp;B outlets, clinics and a childcare centre, Liew adds. Some of the tenants include New York gourmet grocers Dean &amp; DeLuca and premium confectioners Cold Stone Creamery. The pricing of the one- and two-bedroom units at Kingsford Hillview Peak, which is just above $600,000 to over$1 million, has also attracted investors, notes Liew. The project comprises win 12-storey blocks, which are currently under construction and expected to be completed by end-2016 or early 2017.   This article appeared in the City &amp; Country of Issue 687 (July 27) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/developers-play-game-one-upmanship</t>
+          <t>https://www.edgeprop.sg/property-news/lian-beng-oxley-launch-strata-titled-industrial-building-tampines</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Much like competitors in a beauty pageant, city-fringe projects being launched around the same time are vying for attention. All eyes are now on Gem Residences as it unveils its showflats and releases its unit prices on the weekend of May 20. The project previewed on Labour Day weekend (April 30 to May 2) with the opening of just the sales gallery. At least 1,036 people are said to have registered interest in the 578-unit development located on Toa Payoh Lorong 5 and Lorong 6. The developer is ramping up interest ahead of its VIP and public launch on May 27 and 28. We are trying to hit the magic number of 2,000 because theres always a certain level of attrition at the actual sales, says Vincent Ong, managing partner of Evia Real Estate.   More than 1,000 people are said to have registered their interest in Gem Residences. Source: Gem Residences.  Gem Residences is a joint project by Malaysian developer Gamuda Land with a 50% stake and its two Singapore-based partners, Evia Real Estate (20% stake) and Maxdin (30%), a subsidiary of construction company Greatearth Holdings. Gem Residences marks Gamuda Lands maiden foray into the Singapore property market. The property arm of Malaysia-listed engineering construction and investment firm Gamuda Bhd, Gamuda Land developed projects in Kuala Lumpur before venturing into Iskandar Malaysia eight years ago. Gamuda and its joint venture partner UEM Sunrise developed Horizon Hills, a 1,200- acre freehold township development with an 18-hole championship golf course. The project has been very popular with Singaporeans and expatriates over the years. Singapore is Gamudas latest overseas venture; it entered Vietnam a decade ago and purchased a development site in Melbourne last year, says Chow Chee Wah, Gamuda Lands managing director. We feel its a good time to enter Singapore now, and we were exploring several government land sites with Evia last year. We thought the Toa Payoh site was ideal, as there hasnt been a new private condo launch there in a long time. At the close of the tender, there were 14 bids with Gamuda and its joint venture partners submitting the top bid of $345.86 million ($755 psf per plot ratio) for the 130,832 sq ft site.  Artists impression of the 578-unit Gem Residences with 37- and 38-storey towers   First launch of private condo since 2009The last private condo to be launched in Toa Payoh was the 590-unit Trevista by Choice Homes in 2009. The 99- year leasehold condo project in Toa Payoh Lorong 3 was fully sold and completed in 2011. Prior to that, there were only two other private condos launched in the area, which is predominantly an HDB estate. One was the 384-unit freehold Trellis Towers in Toa Payoh Lorong 1, which was launched in late 1996 by CDL and completed in 2000. The other was the 99-year leasehold Oleander Towers, also located on Lorong 1, which was developed by Wing Tai Holdings. Launched in late 1995, the project was completed in 1998. Resale prices in Toa Payoh have also been resilient. Units at the 99-year leasehold Oleander Towers, which is almost 20 years old, changed hands at $988 to $1,043 psf in 1Q2016. In recent months, units at Trellis Towers have been sold at $1,266 and $1,342 psf. Meanwhile, Trevistas resale prices of mid-floor units ranged from $1,210 to $1,315 psf from February to April, according to caveats lodged with URA Realis. Gem Residences will be the fourth private condo in Toa Payoh in 50 years, says Evias Ong. So, we feel theres a certain level of pent-up demand. Among the more than 1,000 people who have expressed interest in the project, 35% live in Toa Payoh and 30% within a 5km radius, including Ang Mo Kio, Bishan and Balestier. The most-sought-after units are the two- and three-bedroom apartments, which garnered 30% and 25% interest respectively.  Triple-key units a noveltyClose to 60% of the units at Gem Residences are one- and two-bedroom units measuring 452 to 775 sq ft. Another 30% are three-bedroom units of 936 to 1,055 sq ft; and there are 37 each of four- and five-bedroom units measuring 1,249 sq ft and 1,313 sq ft respectively. There are only two penthouses: a 1,636 sq ft, four-bedroom unit; and a 2,045 sq ft, six-bedroom unit. Of the 172 three-bedroom units, 37 have been designed as trio or triple-key units of 936 sq ft each, which is a novelty in the market. The trio unit will have a main entrance and foyer that opens up to three separate suites. Each suite will be a standalone apartment with its own living room and kitchenette, bedroom and en suite bathroom as well as a balcony. The foyer can be a common area for the occupants shoe racks, umbrella stand and washing machine and dryer, says Evias Ong. Each suite will also have its own sub-meter to allow the landlord to monitor the tenants utility usage and bill accordingly. However, its still one property title for one triokey unit, explains Ong. Interest in these 37 trio units have been so overwhelming that they will have to be sold by balloting at launch, reckons Ong. While there is strong investor interest in Gem Residences, Ong says he also detects a nostalgia factor among the buyers because Toa Payoh, being the first HDB town in Singapore, is the most established in terms of amenities. Many of these young families want to move back to Toa Payoh because its where they grew up, and their parents are still living there, he says.  Chow: We thought the Toa Payoh site was ideal, as there hasnt been a new private condo launch in a long time  Ong: We want to differentiate ourselves by focusing on providing services to make things more convenient for our residents  Providing communal servicesThe project is adjacent to the Seu Teck Sean Tong Temple and within walking distance of the Braddell MRT station. Every project has a 50m swimming pool and tennis court, says Ong. So, we want to differentiate ourselves by being buyer-centric and focusing on providing services to make things more convenient for our residents. As part of the governments efforts to make Singapore car-light, the developer of Gem Residences has also tied up with Smove to provide residents with a car-sharing system. There will also be a bicycle rack for 100 bicycles and 30 communal bicycles for residents use, as well as a taxi bay for cab and Uber or Grab drivers. As more than half the units are one- and two-bedroom apartments, Ong foresees that most of the residents will be singles and young couples. The developer will provide dedicated uniformed housekeeping staff for the convenience of residents, who can book the services and pay an hourly rate.  Showflat of a one-bedroom unit at Gem Residences. The fully fitted unit comes with Smeg appliances such as oven, refrigerator and washer-dryer.  Source: Gem Residences  Ong reckons that residents of the four- and five-bedroom units are likely to be multi-generational families, as Toa Payoh is an ageing estate with an ageing population. Units are designed to be wheelchair-friendly and, for the convenience of the elderly or disabled, the developer will provide a mobile medical clinic with a doctor and nurse on duty on weekends. Concierge staff will be on hand to help residents hail a cab and with other needs. Parcel lockers will be provided for registered mail deliveries and the convenience of those who shop online, adds Ong. When Gem Residences is completed in 2020, the developer will present each owner with a compendium of all the available services, including food and grocery delivery, engaging a private chef for parties, and cleaning services. The project comes with a 6,000 sq ft clubhouse with a gym, barbecue and grill areas and fully equipped function rooms for private parties. Beyond the full condominium facilities, there are also dedicated pet amenities for dogs  with a pet run, pet pool and pet shower. Ong estimates that 7% of the residents at Gem Residences are likely to have pets.  Competitive pricingGem Residences has a guide price averaging $1,480 psf. The actual prices of units will be released on May 20, a week before sales begin. We want to give potential buyers enough time to consider their purchase without duress, says Ong. They will have time to consult their bankers and discuss with their family members before committing to their purchases. The developer is offering an early bird discount in the form of a cheque to buyers. The discount is $7,500 for unit purchases below $800,000; and $10,000 for purchases above $800,000. In the current market, property agents continue to collect cheques [as an expression of interest], says Ong. Cheque collection prior to a launch works in a market in which demand outstrips supply, he says. In the current market, where there are more units pursuing buyers, however, it may not be necessary, he adds. The preview of Gem Residences coincided with the public launch of Sturdee Residences, a 99-year leasehold condo located off Jalan Besar. The VIP preview for Sturdee Residences was held on April 23 and 24, and 122 of a total of 305 units were sold. Another 10 units were snapped up at the launch weekend. Thus, the project is 43% sold at an average of $1,550 psf. Boutique developer Techkon held the soft launch of Viio @ Balestier at end-April. Over the past three weeks, 40% of 56 freehold residential units sitting on top of a three-storey retail podium have been sold at an average price of $1,450 psf.  Glitterati at Stars of KovanMay 7 marked the VIP preview of Cheung Kong Property Holdings Stars of Kovan. The Li Ka-shing-controlled property group unveiled its $10 million sales gallery and showflats last weekend, drawing 4,000 visitors. The 99-year leasehold project is located at the junction of Tampines Road and Upper Serangoon Road and within the Kovan residential estate, which comprises mostly houses and private condos. A mixed-use scheme, Stars of Kovan contains 390 private condo units in four 17-storey blocks sitting on top of a retail podium. Adjoining it is a row of five strata terraced houses. One of the main attractions is that the project is mixed-use, says Joseph Tan, executive director of residential services at CBRE. The other attraction is its proximity to the Kovan MRT station just across the road.  A total of 4,000 people visited the Stars of Kovan showflat at the VIP preview on May 7 and 8  The British-style retail podium of Stars of Kovan will have 46 commercial units with a mix of retail and F&amp;B space. It is set to raise the bar on quality mixed developments in Singapore, says Tan. The closest shopping centre is the ageing 32-year-old Heartland Mall adjacent to the Kovan MRT station. Condo units at Stars of Kovan are a mix of one- to three-bedroom apartments measuring 506 to 1,023 sq ft, with absolute prices said to range from $800,000 to $1.5 million. The two-bedroom units measuring 732 to 807 sq ft were the most popular among Singaporean investors, according to Cheung Kong Property. The indicative price range is said to be $1,550 to $1,600 psf. The project is scheduled to be launched on May 21, with CBRE and Huttons Asia as joint marketing agents. The race is on for the two projects  Stars of Kovan and Gem Residences  that are set to be launched over the next fortnight. Developers will therefore have to sharpen their edge in terms of product differentiation, says a veteran property consultant who declined to be named.  This article appeared in the City &amp; Country, Issue 728 (May 16, 2016) of The Edge Singapore. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/eaton-residences-defy-market-forces</t>
+          <t>https://www.edgeprop.sg/property-news/location-scan-shunfu-ville-collective-sale-whats-its-vicinity</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>On the weekend of Nov 19 and 20, GSH Corp launched in Singapore its maiden residential development, Eaton Residences, a high-end condominium on Jalan Kia Peng in Kuala Lumpur City Centre (KLCC). The property exhibition was held at Fairmont Singapore in Raffles City. So far, 180 units have been booked, says GSH. The figure includes the 150 units taken up when the first phase of 280 units was launched in KL on Sept 20, and the units sold subsequently. These days, its hard to achieve double-digit sales in any overseas property launch, observes Donald Han, managing director of Chesterton Singapore. With the Singapore economy in the doldrums, people are conserving cash. Meanwhile, companies are trying to cut costs. So, in the current environment, if you can achieve such sales at an overseas project launch, thats excellent. Over the weekend, more than 20 groups were said to have visited the exhibition. For a standalone overseas project exhibition, its quite a good turnout, says Sunny Wong, division director at ERA Realty, the exclusive marketing agent for the project. These are serious buyers. Some are interested in buying a unit as a second home and others are looking at an investment opportunity. Riding on the momentum, Eaton Residences will be showcased for a second consecutive weekend in Singapore at ERAs office and sales gallery in Mountbatten Square on Nov 26 and 27.  Petronas Twin Towers  the landmark of Kuala Lumpur City Centre  Palatable absolute prices With the Malaysian ringgit tumbling to a new low of 3.1 against the Singapore dollar, the exchange rate is looking favourable for Singaporeans, and in terms of absolute prices, its equivalent to a 30% to 40% discount, says Gilbert Ee, CEO of GSH. To make absolute prices palatable to price-sensitive buyers, one-bedroom and one-bedroom- plus-study units make up 394 (62%) of a total of 632 units at Eaton Residences. These are sized from 635 to 872 sq ft. Two-bedroom-plus-study units measuring 1,098 to 1,464 sq ft and three- and four-bedroom-plus-study units measuring 1,550 to 2,874 sq ft account for 36% of the units. There are also 12 penthouses of 2,271 to 2,982 sq ft. The one-bedroom units at Eaton Residences are priced from RM1.14 million ($365,000) and one-bedroom-plus-study units start from RM1.45 million ($465,000). Therefore, these units have been the most appealing to investors because of the affordability of their absolute prices. For $365,000 to $465,000, you cannot even buy a shoebox apartment in Singapore today, says a property agent. At that price range, you can probably buy a brand-new BMW 6 Series convertible, a Jaguar F-Type, a Mercedes CLS-Class or a Porsche Boxster in Singapore. But if you buy a property, you can rent it out and earn a return, says Ee.   Ee: The [SGD/RM] exchange rate at this point is looking favourable for Singaporeans, and in terms of absolute prices, its equivalent to a 30% to 40% discount  Rental yields Contrary to popular belief, it is easier to find tenants in KL than in Singapore, says Bruce Lye, managing partner of realtor SRI. Lye, a Singaporean, has been marketing projects in KL and investing there for the past six years. Today, he and his wife jointly own seven condo units in KL  three in the MontKiara area, a popular suburb with expatriates; two at Sentral Residences near the KL Sentral train station, which is due for completion within the next few months; one in KLCC; and one in Bukit Bintang. Based on my experience with the properties that I own there, I realise that the big units in the KLCC area do not perform as well in terms of rentability compared with those in MontKiara, says Lye. The big units in MontKiara tend to be rented out quickly because they are popular with families, as there are international schools in the neighbourhood. In the KLCC area, one- and two-bedroom units are sought after because of the profile of the tenants, says Lye. They tend to be young singles or couples with no children. In fact, rents of the larger units are quite close to the one- and two-bedroom units in the KLCC area. According to Lye, gross rental yields in the MontKiara and KLCC area are about 6%. If one were to take financing cost into consideration, however, then net yield would be 2% to 3%, which is on a par with yields in Singapore, he says. Without a mortgage, however, yields will be around 6%. Reinvesting, dollar cost averaging While Lyes portfolio of properties have seen capital gains, he will incur a loss based on the current exchange rate. This is because many of his purchases were made five to six years ago when the ringgit was 2.2 against the Singapore dollar, says Lye. One way to avoid a currency exchange loss is to reinvest his gains in Malaysia, he says. Thus, he intends to buy another small one- or two-bedroom unit in the KLCC area within the next six months. Another bonus of having multiple properties in KL is that it can also be a second or holiday home. I travel up to KL at least once a month, says Lye. If one of my properties is available between tenants, I will stay in it. While Singaporeans account for about 20% of buyers at Eaton Residences, mainland Chinese form the majority. Other international buyers include those from Hong Kong, Indonesia and Taiwan, says GSHs Ee.  Model of the 632-unit Eaton Residences on Jalan Kia Peng in KLCC  In early November, the Hong Kong government doubled stamp duty for foreign buyers from 15% to 30%, and for second and subsequent Hong Kong resident buyers from 8.5% to 15%. Anticipating that property investors will now look elsewhere, Singapore developers have been quick to seize the opportunity by bringing their projects to Hong Kong on roadshows. Like the other Singapore developers, GSH is also launching Eaton Residences at a weekend roadshow in Hong Kong on Nov 26 and 27. If the overseas and local investors in Hong Kong are deterred by the higher stamp duty, money will flow out and look to invest elsewhere, says Ee. KL may be at the receiving end of some of that outflow. The downward trend of the ringgit is a double-edged sword for many overseas investors. I remember 25 years ago when the exchange rate between the ringgit and Singapore dollar was 1.5 to 1, recounts Chestertons Han. And now its hovering at 3.1 to 1. So, its been on a downward trend. And in the short term and even the medium term, its hard to foresee the ringgit strengthening, especially with oil prices still depressed and the current political uncertainty in Malaysia. Priced at RM1,550 to RM1,800 psf, Eaton Residences looks particularly compelling, especially in the face of a falling ringgit, concedes Han. In the KLCC area, ultra-luxury condos priced at RM2,500 to RM3,000 psf are finding it difficult to move units, especially if they are large and the absolute prices are high. He reckons that GSHs Eaton Residences could have hit the sweet spot with foreign buyers with the exclusivity of the project, and by capitalising on its location and the views.  Every room in every unit  from the kitchen and living area to the master bedroom  has a view Capitalising on views, location Eaton Residences is located within KLs Embassy Row and near the Petronas Twin Towers and Jalan Bukit Bintang shopping belt. It is within walking distance of the KLCC LRT station and within 150m of a future MRT station at Jalan Conlay. The project is also near the Prince Court Medical Centre. The 51-storey tower offers unobstructed panoramic views of the Petronas Twin Towers on one side and the Royal Selangor Golf Club on the other. GSH had purchased the prime 62,726.4 sq ft site from Tropicana Kia Peng for RM132.4 million in December 2013. The 99-year lease on the project is not a concern, says Ee. Unlike in Singapore, owners of private property in Malaysia are able to renew their 99-year lease at a prescribed amount. And buyers only need to pay to renew the lease when there are only 30 years left, he says. GSH has appointed Singapores most established architectural firm, Swan &amp; Maclaren, to design Eaton Residences in collaboration with Patty Mak (formerly of Suying Metropolitan Studio) as interior design consultant. Eaton Residences will have an entrance driveway and lobby designed with the grandeur of a luxury hotel, says Lim Chai Boon, Swan &amp; Maclarens group director. There are three levels of basement parking below an eight-storey car-park podium. Ample parking is provided, as the one-bedroom units are designated one parking space each, but most of the other units have two parking spaces each and the penthouses have up to four. On the rooftop of the car-park podium, there is a facilities deck with a childrens playground, barbeque pods, fitness stations and multi-use spaces. The 33rd level has a sky garden and lounge. The 51st level has a 40m cantilevered infinity swimming pool that allows residents to enjoy the view, says Lim. There are also spa pools and a leisure pool on this level. The view from the 51st floor will be as spectacular as being at the SkyPark of Marina Bay Sands, says GSHs Ee. This is whats going to set the project apart from the rest. And there are many upcoming developments in the vicinity. According to Property Talk &amp; Lifestyle Malaysias PTML Research in a September 2015 report, more than 120 sites in the KL city area are under construction, being proposed for development or being planned for future development. KL is a city of skyscrapers, and thats no different from other cities such as Shanghai or Manhattan, notes interior designer Doyenne Mak. I felt it was important to create an identity for Eaton Residences. We wanted to create city living, and that means embracing the skyline  so, every room in every unit must have a view. All units have an open-concept kitchen, says Mak. This allows residents to interact with other members of the family even while cooking, and enjoy the view at the same time. At Eaton Residences, Mak also chose a muted palette for the units, with the same white marble carried throughout the unit and in the bathrooms, and white timber flooring for the bedrooms. Kitchen cabinets and wardrobes, which are custom-designed, are also in white or grey tones. The idea is to create a canvas for the owner to fill in the colours to complete their dream home against the backdrop of a blue sky, she says.  Every unit at Eaton Residences comes with an open-kitchen concept with a view of the city skyline  Luxury quality for a steal The quality of the materials used at Eaton Residences is equivalent to those of luxury condos in the prime districts of Singapore. Mak has designed the interiors of many high-end condos in Singapore, including the 462-unit OUE Twin Peaks on Leonie Hill Road, where she even handpicked the furniture for each unit; Allgreen Properties 360-unit SkySuites @ Anson on Enggor Street; Sing Holdings 134-unit Robin Residences; and the 97-unit Centennia Suites, where action star Jackie Chan is said to have purchased three units. With Swan &amp; Maclaren and Mak behind the design of Eaton Residences, the response to our project has been very good, says Ee. Despite the challenging environment, we swung quite a few buyers from neighbouring projects because of our price point, product quality and uniqueness. The construction cost of Eaton Residences is estimated at RM450 million, and the condo is expected to be completed in 2020. I dont think I can construct a 51-storey condo project of this quality in Singapore for $150 million, says Ee. Even if the ringgit collapses further, property prices in Malaysia will have to go up because developers can no longer build properties at these prices, he adds. The cost of labour and construction materials will only go up, and that means property prices will also rise. So, if youre buying a unit at below RM2,000 psf in KLCC today, there will be upside potential.  This article appeared in The Edge Property Pullout, Issue 756 (Nov 28, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/economic-headwinds-may-moderate-industrial-rents-2020</t>
+          <t>https://www.edgeprop.sg/property-news/location-scan-sit%E2%80%99s-new-campus-punggol</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SINGAPORE (EDGEPROP) - Industrial real estate rents in Singapore were generally stable in 2019, although the sector was weighed down by oversupply from preceding years, says Christine Li, head of research, Singapore and Southeast Asia, at Cushman &amp; Wakefield (C&amp;W). Tricia Song, head of research for Singapore at Colliers International, agrees. She says that compared to 2018, the overall industrial property market has shown clearer signs of stabilisation, with both rents and vacancy rates remaining relatively stable in the year to September. Both net demand and net supply are expected to have increased in 2019.  But looking ahead, Li says the industrial outlook for 2020 could be gloomier compared to this year. She says global macroeconomic factors, such as slowing economic growth in the US, the EU and China, is likely to have a negative impact on Singapores economy in 2020. The subdued global economy is expected to moderate industrial rents next year, she adds.  Newly completed industrial space doubles in 2019 This year, close to 12.5 million sq ft of net new industrial space is expected to have been completed, which is more than twice the 5.84 million sq ft of net new completions in 2018, says Song. Net new demand is also expected to have increased by 50% y-o-y to 11.0 million sq ft in 2019, she adds. For 2020, the largest new industrial development that will be completed is the Defu Industrial City at Defu Street 1. JTCs flagship stackup complex at Defu Industrial Park will have a total gross floor area (GFA) of 3.52 million sq ft. Other sizeable new industrial developments in 2020 include JTCs TimMac @ Kranji boasting 1.54 million sq ft in GFA, and JTC Bedok Food City with 1.13 million sq ft in GFA.  Over in the one-north business park district, homegrown gaming hardware company Razer is expected to open its purpose-built, 207,743 sq ft headquarters building next year, while ride-hailing giant Grab is due to move into its 387,000 sq ft purpose-built headquarters building by 4Q2020. Two-tier leasing performance in factory segment  Based on CBRE Researchs basket of industrial properties, factory and warehouse rents remained steady at $1.57 psf per month (pm) and $1.58 psf pm respectively in 4Q2019. Looking ahead, warehouse rents are expected to be more resilient, supported by a tight supply pipeline, says Desmond Sim, head of research, Southeast Asia, at CBRE. But he adds that industrial occupiers were looking for premises with higher specifications and better efficiency. This contributed to a two-tier leasing performance by the factory segment in 2019, as industrial developments with higher specifications outperformed older, conventional industrial buildings. The 10.5% vacancy [in the factory segment] in 3Q2019 included a growing pool of vacant, ageing industrial stock of about 53.85 million sq ft. This spurred several landlords to undertake asset enhancement initiatives on older industrial stock in a bid to unlock value by repositioning and redeveloping assets with under- utilised gross floor area, he says. According to Colliers, these enhancements include increased power capacities, high-floor loading capability, modern ventilation and cooling systems, higher ceilings and better loading bay facilities. Redevelopment could also enhance connectivity between adjacent buildings and to transportation nodes. According to Song, landlords feel it is the right time to adopt smart features such as automation and artificial intelligence to improve productivity and space efficiency, and reduce operating costs. In general, leasing demand in 2019 was driven by renewals and relocations of companies in the third-party logistics, high-tech manufacturing, and chemicals sectors. The electronics sector took a backseat in 2019 when the US-China trade war escalated, and the sector was also hit by an economic dispute between Japan and Korea, CBREs Sim says, adding that some industrialists are taking a cautionary stance and limiting expansion plans. According to Colliers, third-party logistics companies, transport agencies, e-commerce, and manufacturing companies were the top occupiers of warehouse logistic spaces this year. Companies in these sectors accounted for close to 74% of occupied islandwide warehouse space.   as well as business parks segment High-spec premises such as business parks also recorded a two-tiered leasing performance in 2019 as the market split between city-fringe and suburban submarkets. City-fringe business park rents climbed 0.9% y-o-y to $5.85 psf pm, but suburban rents fell by 1.3% y-o-y to $3.75 psf pm, based on JTC statistics. We continue to see a flight to quality in the business parks sector, says Colliers Song. We observe that new business park spaces near MRT stations in the city fringe continued to attract healthy demand, while those older and further away from MRT stations located in the suburbs faced more difficulty in finding tenants, despite lower rents. The biggest deal of the year was Mapletree Commercial Trust acquisition of Mapletree Business City II from its sponsor Mapletree Investments for $1.55 billion. (Picture: Samuel Isaac Chua/The Edge Singapore)  She adds that the rent disparity could widen going forward, as centrally-located business parks with good amenities are expected to record rental growth, while rents in older business park spaces could remain flat over the next few years. C&amp;Ws Li says that with office rents near the peak, cost-conscious occupiers are choosing to locate at business parks as an alternative to the CBD. The segment saw improved absorption of 452,000 sq ft during the first three quarters this year, she says. The specs of newly completed business parks are almost no different from that of Grade-A offices which can compete for the same tenant pool if such tenants qualify for both business park and office spaces. That could help to put a lid on the rental upside should there be more decentralised office supply in the pipeline, Li adds. However, decentralised office supply does not necessarily cannibalise the business park demand, as they offer different specifications, eco-systems and different value propositions for different types of tenants, says Colliers Song.  Reits dive into specialised assets Industrial investment activity has been relatively healthy in 2019, clocking in deals worth about $2.99 billion. The biggest deal of the year, in terms of transacted prices, occurred in November when Mapletree Commercial Trust acquired Mapletree Business City II, a premium campus-style business park development, from its sponsor Mapletree Investments for $1.55 billion. The second largest deal was in September, when Keppel DC Reit acquired a 99% stake in Keppel DC Singapore 4 for $381.1 million. The Reit also acquired a second data centre, 1-Net North DC, for $201.8 million. In November, Ascendas Reit acquired two business-park properties, Nucleos and FM Global Centre, from its sponsor CapitaLand for a combined value of $380 million. In April this year, CapitaLand sold the group of companies that own and manage the self- storage business StorHub, for $179.5 million. This comprises StorHubs portfolio of 12 self-storage properties with a total lettable area of about 800,000 sq ft. The largest industrial leasing deal in 2019 was Googles expansion into Alexandra Technopark, taking up 344,100 sq ft (Picture: Samuel Isaac Chua/The Edge Singapore)  Meanwhile, the largest industrial leasing deal in 2019 was Googles expansion into Alexandra Technopark, taking up close to 344,100 sq ft of industrial space. The development is adjacent to Googles Asia-Pacific headquarters in Mapletree Business City II. Another notable leasing deal occurred in January when e-commerce firm Shopee leased all 240,000 sq ft at 5 Science Park Drive, a redevelopment of the former Fleming and Faraday buildings by Ascendas-Singbridge, for its expansion needs.  Read also: Real estate investment activity in Asia-Pacific to outperform Europe and Americas in 2020-2021: JLLCushman &amp; Wakefield appoints industrial and logistics team leaderWoodlands Industrial Park site launched under IGLS programme</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/edge-property-turns-one</t>
+          <t>https://www.edgeprop.sg/property-news/logistics-building-spacetampines-market-170-mil</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The Edge Property celebrated its first birthday with a party on June 16, during which managing director Bernard Tong presented a short video chronicling the successes achieved. The Edge Property is the fastest growing property platform, with 700% growth in number of visitors per month  from 50,000 a year ago to 350,000 today and 1.5 million page views. Tong also announced new initiatives to better serve clients, users and stakeholders. These include the merging of theCity &amp; CountryandThe Edge Propertypullouts into a single property section, and the launch of a mobile app that halves the time taken by agents to post listings, in addition to enabling posting on the go. Thirdly, TheEdgeProperty.com has been revamped for even greater ease of use. Among the 140 VIPs at the party were industry leaders such as Real Estate Developers Association of Singapore (Redas) CEO Joseph Tan Tai Chiew; CapitaLand senior vice-president, marketing and sales Colin Wong; GuocoLand (Singapore) property sales general manager Dora Chng; Kylou Properties managing director Daven Wong; Oxley Holdings director, market ing and sales Eugene Lim; and Teambuild Land executive director Richie Chew. Congratulatory messages The Edge Property in just one year has grown to become quite indispensable. With such a good start, I look forward to it being entrenched as a must-visit portal for all real estate stakeholders. Congratulations to the team at The Edge Property; its a well-deserved first birthday! RedasJoseph Tan Keep scaling new heights of success and setting new standards. Happy birthday and congratulations to The Edge Property! GuocoLandsDora Chng The Edge Property was instrumental in helping us achieve 50% sales during our recent launch of VIIO @ Balestier. The Edge Propertys enthusiastic, dedicated, genuine and energetic team is bound for great success. Happy anniversary! Kylou PropertiesDaven Wong Theres an African proverb that says, If you want to go quickly, go alone. If you want to go far, go together. We have always appreciated a good business partner. The professionalism, enthusiasm and creativity exhibited by the dynamic team at The Edge Property Singapore were exactly what we needed. Its comprehensive property platform, coupled with the teams ability to deliver quality work, have helped us meet our business needs. My heartiest congratulations to The Edge Property Singapore on their first anniversary!  CapitaLandsColin Wong From creating a life-size monopoly one year ago to having 350,000 visitors per month, The Edge Property has certainly created another significant milestone. Heartfelt congratulations to everyone in The Edge Property. OxleysEugene Lim We value our partnership with The Edge Property, which is professional, enthusiastic and thorough. We look forward to many more fruitful years with The Edge Property. Happy Birthday! Teambuild LandsRichie Chew  Real estate salespersons and leaders from ERA Realty Network at the party  Teambuild Land executive director Richie Chew (left) and The Edge Property advertising sales account manager Priscilla Wong  Wing Tai marketing executive Tan Sze Gee, Priscilla Wong, Wing Tai assistant marketing manager Linette Tan, Wing Tai Malaysia marketing and sales manager Calvin Kwet and The Edge Property advertising and sales director Cowie Tan  GuocoLand general manager Dora Chng, GuocoLand senior manager, marketing Corinne Tsang and JTResi founder Jerry Tan  Cowie Tan, The Edge Property associate account director Diana Lim, The Edge Singapore director Anne Tong, Far East Organization director &amp; COO, corporate real estate business group Cheryl Huan; Far East Organization marketing executive, corporate real estate business group Cherylynn Koh, The Edge Property executive director Ian Tong and The Edge Property advertising sales account manager Ken Tan  S P Setia Internationals general manager Neo Keng Hoe, The Edge Propertys Diana Lim, and other S P Setia personnel  senior executives for sales and marketing Koh Kai Ling and Rachel Ong, and interns Dominic Chng and Elson Lee  Ian Tong, Bernard Tong, Kylou Properties managing director Daven Wong, InspireOn Real Estate key executive officer Phyllis Yap, and Diana Lim and Cowie Tan  M+S head of marketing communications Lester Lim; Formul8 account director Nicholas Tan; CapitaLand senior vice-president, marketing and sales Colin Wong; Formul8 managing director Fiona Bartholomeusz; Oxley Holdings director of marketing and sales Eugene Lim; and Bernard Tong, The Edge Property managing director  Real estate salespersons and leaders from PropNex Power of CLOSING Division  Joey Yap Consulting Group founder and chief consultant Joey Yap, Bernard Tong, Redas CEO Joseph Tan, Anne Tong, and The Edge Property Malaysia managing director Au Foong Yee  This article appeared in the The Edge Property pullout of Issue 734 (June 27) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/edmund-tie%E2%80%99s-ceo-putting-people-first</t>
+          <t>https://www.edgeprop.sg/property-news/lost-decade-sentosa-cove-singapores-billionaire-haven</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SINGAPORE (EDGEPROP) - Not only is real estate industry veteran Ong Choon Fah the CEO and head of research and consulting at property consulting firm Edmund Tie, she has also been active in championing the responsible use of land over the years. In July, she was appointed the Singapore Chair for the Urban Land Institute (ULI). The global, independent non-profit has the oldest and largest network of cross-disciplinary real estate and land use experts in the world. The mission of ULI is to provide leadership for the responsible use of land and to create thriving and sustainable communities worldwide. So that really resonates with me, Ong says. Ong: Ultimately, real estate is about people and we are in an amazing industry where we can make a difference, one step at a time (Credit: Albert Chua/EdgeProp Singapore)  With a real estate career spanning more than 25 years, she has advised on the master planning of land parcels in Medini, Iskandar Malaysia (930ha); Vientiane, Laos (44ha) and Mauritius Airport City (17ha). At home, she was involved in the Gardens by the Bay project (101ha). Recalling her experience, Ong says in the early 2000s when Gardens by the Bay was still just an idea, there were not many places in the Central Area where Singaporeans could be close to nature besides the Singapore Botanic Gardens. We want our children to not just go to malls, but also to have places that let them run about and be close to nature, she says. In land-scarce Singapore, Ong notes, it can be difficult to justify allocating land use to a park versus selling it off in the Government Land Sales (GLS) programme. She says: At the end of the day, sustainability is also about economic sustainability. You cant just build a park that is not economically sustainable. This means you have to come up with taxpayers money. To ensure economic sustainability, the planning committee decided to price admission to Gardens by the Bay at $12 for Singaporeans or roughly around the same price as a movie ticket, she says. This ensures that the attraction remains accessible to the public.  Focus on wellness Central to her ethos, Ong believes that when thinking about real estate, one should first consider the people they are catering for. This belief is manifested in Edmund Ties office at UIC Building on Shenton Way. The firm was previously located at Shaw Tower for more than 20 years. In the 1970s, [Shaw Tower] was an amazing building, but now its like a grand old dame, she says. Over time, Ong noticed that the aircon ducts required more frequent cleaning and many of the firms staff were falling ill. She also felt guilty that only her office had windows with views of the outside, and made it a point to leave her door open and shades raised so her staff can enjoy the views too. In 2017, the firm shifted to its current premises. There, everyone in the open-plan office can benefit from the unobstructed sea view. Each employee has a 1.5m-long desk; for those who prefer standing while they work, adjustable desks are also an option. The floor-to-ceiling windows allow all Edmund Tie employees to enjoy an unobstructed sea view (Credit: Samuel Isaac Chua/ EdgeProp Singapore)  The company has also done away with personal wastepaper baskets, opting instead for common recycling bins and paper shredders in designated areas around the office. The idea is to get employees out of their seats to walk to the bins, which keeps them active and fosters interaction among staff, says Ong. The office is also wired for hot-desking so staff can work from anywhere. These design elements have paid off. Ong recalls that when the company was at Shaw Tower, during exit interviews, the physical work environment was always cited as a reason for leaving. [At the new office], my staff feel happier so our retention rate is a lot higher, she says. The Edmund Tie office has adjustable desks for those who prefer standing while they work (Credit: Samuel Isaac Chua/EdgeProp Singapore)  Apart from Edmund Tie, Ong highlights, developers are also looking at how they can promote wellness within their spaces. At the same time, buyers are also becoming more discerning. As a result, developers are now fitting out commercial and residential projects outside the Central Area with features that one would typically find only in the prime areas. Thats become the new normal, she says. Developers actually think about how the occupiers use that space. In particular, this is a common theme in this years project submissions for EdgeProp Singapore Excellence Awards, Ong notes. Into its third year, the Awards benchmarks outstanding quality in property development. This is the second year that Ong is serving as a judge on the panel.  Learning through mistakes Whether it is sustainable land use or designing for wellness, Ong observes that the common denominator is putting people first: When it comes to real estate, not everything can be directly translated into dollars and cents. If you do good, youre actually brand-building. People trust your brand, that you are client-focused and that you are aligned with them, she explains. In addition to providing a better work environment, Ong hopes to strengthen Edmund Tie by nurturing the companys next generation of leaders. To do this, she fosters a safe environment for staff to innovate by giving them opportunities to try new ideas and accepting that people make mistakes. If you dont make mistakes, youll never have the courage to innovate. Of course, this is a calculated risk, she says. Sometimes its very painful when you know that it is not quite the right thing to do, but you have to let people experiment and come to their own conclusions. To her, learning is not restricted to a top-down approach. Instead, Ong is always happy to learn from her staff. Its not just the older people mentoring their juniors, but it is also the juniors and young people mentoring me, she observes.  Giving back Ong reveals that she owes much of her career success to mentors who took a chance on her. She vividly remembers her first job as a valuer, when she was tasked to assess the value of a cold store in Pasir Panjang. She was stumped. As part of her studies, she had learned that there are three methods of valuation  comparable, income and cost. However, she could not apply any of these methods as there was not enough information and data. She then turned to her mentor and industry expert, MH Goh of MH Goh, Tan &amp; Partners (now Colliers International), who gave her the guidance she needed to complete the valuation. Ong also remembers Douglas Hiorns, the late general manager of Bukit Sembawang, who granted her an interview when she was researching her dissertation for graduate school. She had written letters to developers requesting interviews with them but only Hiorns responded. I was a nobodyand he granted me the interview, she says. I will never forget his kindness to me. Now, Ong wants to pay it forward. Theres always an opportunity to give back, and you must not be afraid to share with people, she says. Real estate is not about bricks and mortar. Ultimately, real estate is about people and we are in an amazing industry where we can make a difference, one step at a time.  Read also: ET&amp;Co rebrands as Edmund TieSales of private non-landed housing units to foreigners rise to 6% in 2Q2019: Edmund TieOng Choon Fah appointed as Singapore chair of Urban Land Institute</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/era-revives-coldwell-banker</t>
+          <t>https://www.edgeprop.sg/property-news/malls-revitalise-amid-retail-woes</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>US real estate franchise Coldwell Banker has had a presence in Singapore since 2000, but it has been dormant for the past eight years. The company that held the franchise in Singapore, Hersing Corp, sold the franchise together with Asia-Pacific brokerage firm ERA Real Estate for over $100 million in 2013. The buyer is Singapore-based private equity firm Northstar Group. While ERA has grown to become the biggest real estate agency in Singapore with 6,375 agents and over 40% market share in terms of new project launches, Coldwell Banker has remained dormant since 2008 until now. We have to revive and grow the Coldwell Banker brand within the next five years, says Jack Chua, CEO of ERA and Coldwell Banker. Coldwell Banker and ERA, along with Century 21 and Sothebys International Realty, are owned by New York Stock Exchange-listed real estate services company Realogy. In Singapore, Coldwell Banker and ERA are under Northstar.  Chua (left) and Goh  Consolidation With eight consecutive rounds of property cooling measures culminating in the total debt servicing ratio loan framework in June 2013, residential transaction volume has halved to between 7,000 and 7,500 units over the last two years. Likewise, the number of new agents fell to 1,299 last year  less than half the 3,006 new entrants in 2014, according to the Council for Estate Agencies. There has been a wave of consolidation in the real estate industry, with franchises changing hands. In Singapore, Century 21 is owned by Asia-Pacific Strategic Investments, a former Malaysian bereavement services company that transformed itself into a real estate services firm last year. APSI acquired Century 21 Hong Kong and Asia-Pacific, which includes the Singapore franchise, followed by Global Alliance Property in Singapore in 2015. Sothebys debuted in Singapore in 2007, when it was brought in by a group of high-net-worth investors. However, it subsequently closed. The luxury brand returned to Singapore in March this year. This time, it is operated by List Holdings Singapore, the entity that also operates List Sothebys International Realty in Japan and Honolulu, Hawaii. The Singapore business is headed by Hisashi Kitami, owner and CEO of List Sothebys. There is an urgency to grow the Coldwell Banker franchise in Singapore, concedes Chua. When Coldwell Banker first started in Singapore 16 years ago, it operated as a division of ERA. The real estate services offered by both entities were similar. People started asking why we have ERA and Coldwell Banker. It was like we were cannibalising our own business, he says. That led to the decision to combine the two under ERA eight years ago.  Franchise model This time around, Chua is taking a different tack to grow Coldwell Banker as a separate entity. He is using the franchise model, which is similar to that of Century 21. Chua is making an effort to target small- and medium- sized real estate agencies to bring them under the umbrella brand of Coldwell Banker. At the same time, the individual companies can keep their respective brands, he says. For example, the first company to sign up as a franchisee was Elitehill Real Estate. That was in January. By February, its owner Martin Goh had convinced three more agencies to sign up. So far, there are 11 Coldwell Banker franchisees with a salesforce of 80. The agencies range from sole entrepreneurs to firms with 30 salespersons. Another handful of agencies are coming on board, says Goh. Goh has become more than just a poster child for Coldwell Banker. He was appointed general manager of Coldwell Banker in Singapore and will oversee the expansion of the franchise. However, he will continue to manage his firm, now renamed Coldwell Banker Elitehill Real Estate. The main attraction for most small- and medium-sized agencies is that they will become part of an international brand and will be able to tap both local deals from ERA and overseas deals from other Coldwell Banker franchisees around the world, says Goh. They will also be able to leverage ERAs training programmes for their salespersons and technology platforms that small firms are unable to provide. Coldwell Banker will have its own corporate office within the 7,000 sq ft space at SLF Building. There will be meeting rooms and desks for agents to use, like a co-working space. According to Chua, the target is to have at least 20 franchisees in Singapore by the end of the year. To attract new franchisees, the fee has also been kept at an attractive level. Its in the range of $1,500 to $3,000 for three years, he says.  This article appeared in The Edge Property pullout, Issue 742 (Aug 22, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/evia-real-estate-and-metro-jointly-acquire-7-9-tampines-grande-395-mil</t>
+          <t>https://www.edgeprop.sg/property-news/manhattan-house-collective-sale-300-mil</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Two adjoining eight-storey Grade-A office buildings at 7 and 9 Tampines Grande were sold to a joint venture between Evia Real Estate and Metro Holdings on April 18 for $395 million. Evia is a privately-held property developer, while Metro is a Singapore-listed department store operator-turned-property developer. The deal was brokered on behalf of the sellers, a fund under Alpha Investment Partners and Singapore-listed property group City Developments Ltd (CDL), by Cushman &amp; Wakefield (C&amp;W). Located in Tampines Regional Centre, Singapores first and most established regional centre, the two properties at 7 and 9 Tampines Grande have a combined net lettable area (NLA) of 287,596 sq ft.  The two adjoining, eight-storey buildings at 7 and 9 Tampines Grande have tenants such as AIA, Hitachi Asia and BNP Paribas (Credit: Cushman &amp; Wakefield)  The purchase price therefore translates to $1,373.45 psf based on NLA. The buildings have a balance lease of 87 years, and tenants include AIA, Hitachi Asia and BNP Paribas. The latest sale of 7 &amp; 9 Tampines Grande demonstrates investor confidence in this tightly-held Grade A micro-market, says Shaun Poh, executive director of C&amp;W Capital Markets Group, who led the negotiations. The pair of buildings at Tampines was part of a portfolio of three office assets owned by CDL. The other two assets were the office tower at Central Mall on Magazine Road, off Havelock Road; and Manulife Centre at the corner of Bras Basah Road and Bencoolen Street. CDL and Alpha Investment Partners Alpha Asia Macro Trends Fund II had co-invested in the portfolio, valued at $1.1 billion, through a profit participation securities (PPS) deal in 2015. In January 2019, Manulife Centre was sold to a joint venture between ARA Asset Management and British property group Chesterfield for $555.5 million or $2,305 psf based on NLA. The 11-storey commercial building has a total NLA of about 241,000 sq ft.    </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/far-east-organization-%E2%80%94-first-mover-woodlands-regional-centre</t>
+          <t>https://www.edgeprop.sg/property-news/martin-place-residential-site-fetched-1239-psf-ppr</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>A consortium led by Far East Organization (FEO) has sold about half of the 124 strata offices released at Woods Square in private previews since end-July. Woods Square is the first mixed-use commercial development with strata offices for sale in Woodlands Central. When completed at end-2021, Woods Square will be linked to the neighbouring Woodlands Civic Centre and Causeway Point shopping mall and the Woodlands MRT station. The commercial project comprises two office towers, a pair of SOLO (small office, loft office) blocks and a retail podium with 39 shops and a 5,000 sq ft childcare centre. The entire project has a total gross floor area of 700,000 sq ft. Tower 1 has 16 floors and houses 365 strata offices for sale. A key feature of these strata offices, which measure 549 to 5,339 sq ft, is their ceiling height of 4.2m. Most of the units released for sale are from this tower.  Showflat of a typical office at a Woods Square unit with 4.2m ceiling height  Showflat of a 500 sq ft SOLO unit with 5m ceiling height  The 12-storey Tower 2 features large floor plates of 23,000 sq ft, and will be available only for lease. The tower has already secured its first anchor tenant  FEO, which will be relocating its satellite offices from across Singapore to Woods Square when the mixed-use commercial project is completed. FEO will occupy 70,000 sq ft spanning 3 floors of Tower 2. It demonstrates confidence in both the location and project, says Shaw Lay See, FEOs chief operating officer for the property sales business group. The company will maintain its headquarters at Far East Plaza on Scotts Road, a mixed-use development built in 1983 by the groups founder, the late Ng Teng Fong. The fourth floor of Tower 2 will have shared amenities for office users, such as meeting and conference rooms, an auditorium, a gym and swimming pool. Meanwhile, the two SOLO blocks at Woods Square comprise a total of 101 units measuring 495 to 1,808 sq ft: SOLO 1 has 49 units and SOLO 2 has 52. The main attraction of the SOLOs is that they have a 5m ceiling height and come with a built-in raised platform. Part of SOLO 1 has been released. FEO will be holding the retail units for lease so that it can better manage the tenant mix. It will also engage a reputable operator for the childcare centre. Designed by DP Architects, Woods Square occupies two adjacent sites with a total land area of 199,873 sq ft. The sites were purchased by a joint venture between the privately held FEO, its listed entity Far East Orchard and Japanese developer Sekisui House when they won the government land tender with a top bid of $634 million, or $906 psf per plot ratio (psf ppr) in April 2014. The partners have also received approval from the government to offer strata offices for sale. Prices range from $1,700 to $2,300 psf, or start from $970,000 for a 506 sq ft unit. Shaw says the prices of offices sold at Woods Square averaged $1,800 psf, with SOLO units at an average of $1,950 psf.  Woods Square is the first mixed-use commercial development in Woodlands Central offering strata and loft offices for sale Early buyers Property analysts have pointed out that the price paid for the Woods Square site is 10% less than the $1,009 psf ppr that Sim Lian paid for its Vision Exchange site at Jurong Gateway in December 2012. Vision Exchange features a 25-storey office tower with a retail podium. It has a total of 740 units of offices, medical suites and F&amp;B spaces. Strata offices measure 441 to 1,938 sq ft. Since the strata offices at Vision Exchange were launched for sale in April 2014, they have fetched prices of $1,907 to $2,503 psf. The two most recent transactions were those of two adjacent units on the 16th floor: A 764 sq ft unit was sold for $1.79 million ($2,346 psf) in June and a 840 sq ft unit fetched $1.95 million ($2,323 psf) in April. Vision Exchange is the only office building with strata units for sale in Jurong Gateway, just like Woods Square in Woodlands Central, says Eugene Lim, key executive officer of ERA Realty. One can see the potential that premium strata offices in Woodlands Central can achieve as more plans unfold.  Lim: One can see the potential that premium strata
-offices in Woodlands Central can command as moreplans unfold  The idea of turning Jurong East into a second CBD the size of Marina Bay (360ha) was mooted in 2008. Besides being turned into a business district, it will feature the Jurong Innovation District and terminus for the high-speed rail connecting Singapore to Kuala Lumpur. When it was first announced that Jurong would be the next CBD, the most common comment was, But Jurong is so far away, recounts Lim. But look at it today. Its completely transformed. The same thing will happen in Woodlands. It is clear that businesses that have seen how the government has transformed Tampines and Jurong are also willing to take a bet on Woodlands as the third regional centre. According to FEOs Shaw, about 60% of the buyers are Singaporeans buying under their company names. She adds that many of these companies have their factories or warehouses in the Woodlands industrial estates and are looking to have an office where they can meet clients or open a showroom or sales gallery. ERAs Lim says the Woods Square offices also appeal to family-owned companies that are now in the hands of the second- or third-generation who tend to be more educated and more conscious about branding and image. Most of them are buying for their own use, with some considering an investment play in addition to own use, adds Shaw. The SOLOs in particular appeal to lifestyle companies and the younger set. For instance, one of the units was sold to a wine importer who likes the high ceiling, as he intends to use the unit to display his collection and host events, she says. Plans to extend the Thomson-East Coast Line from Woodlands North MRT station to Johor Baru has also generated keen interest among companies looking to set up their head office in Singapore, while their factories are located in Johor. Therefore, Woods Square has drawn another group of buyers  Malaysian business owners with operations in Johor. They are already familiar with Woodlands and want to have an office in Singapore, says Shaw. They are our second-biggest group of buyers.  Shaw: Malaysian business owners with operations
-in Johor are the second-biggest group of buyers ofWoods Square units Betting on transformation Plans for the Woodlands Regional Centre were announced in 2013. The regional centre contains two precincts: the commercial components that make up Woodlands Central and Woodlands North Coast, a mixed-use business cluster. Woods Square in Woodlands Central is the first sale of site by the government since the announcement of Woodlands Regional Centre. The second site in Woodlands Central was put up for sale last year and sits on the Reserved List of the government land sales programme, waiting to be triggered by a developer. The 99-year leasehold site has a land area of about 240,950 sq ft and maximum gross floor area of 843,327 sq ft. Sixty per cent of the GFA has to be allocated for office use, and 86,000 sq ft for retail and F&amp;B outlets. The remaining GFA can be used to develop more office space, residential units or even serviced apartments. More than 100ha  slightly smaller than the size of Sentosa Cove  will be made available for sale in the coming years. The land can yield 700,000 sq m (more than 7.5 million sq ft) of commercial space and generate 100,000 new jobs over the next 10 to 15 years. The governments intention is for the Woodlands Regional Centre to be the gateway in the northern region and anchor the development of the North Coast Innovation Corridor, which will include the future Punggol Creative Cluster and Learning Corridor and upcoming redevelopment of the Sembawang Shipyard area. It will also be linked to Seletar Aerospace Park in the future. The idea is to bring jobs closer to home, as more than half a million residents are already living in the northern region of Woodlands, Yishun and Sembawang. ERAs Lim says, The potential increase in population, new jobs created, park connectors and improvement in transport network  with the North-South Corridor and the new MRT station in Woodlands North to JB, and direct connection to the CBD and even Changi Airport  will make Woodlands a more exciting place to work and live in. Over time, more MNCs will move to Woodlands, like what we saw in Tampines 20 years ago, when banks and insurance companies set up offices there, and what weve seen in Jurong in recent years.  First-mover advantage Therefore, FEO has first-mover advantage in Woodlands, says Shaw. Woods Square may be its maiden office development in Woodlands Regional Centre, but it is not the developers first project in the area. When the Singapore American School moved to its new and expanded campus in Woodlands in 1996, FEO developed a collection of 33 New England-style mansions called Woodgrove Estate, adjacent to the campus. The houses were completed in 1997 and FEO still holds many of them for lease, as they are popular with American expatriates whose children attend the school, she adds. Asking rents for six-bedroom detached houses with a built-up area of 7,599 sq ft and occupying a 7,589 sq ft site in Woodgrove Estate are listed at $9,500 a month. Meanwhile, seven- bedroom detached houses with a built-up area of 8,547 sq ft and land area of 8,547 sq ft are available for lease at $13,000 a month. Based on the historical price of a detached house sitting on a land area of 7,459 sq ft that was sold for $3.22 million in 1997, and rental rate of about $9,500 a month today, the gross rental yield translates to about 3.5%.  In 1997, FEO developed Woodgrove Estate with its New England-style mansions, popular with American
-expatriates whose children attend the Singapore American School next door  FEO also developed the 478-unit Casablanca, a condominium located off Woodlands Avenue 1 that was completed in 2005. The 99- year leasehold project was launched for sale in July 2002, and units were sold at an average of $450 psf at the time. The sole transaction this year was that of a 1,184 sq ft unit on the eighth floor that changed hands for $936,000 ($791 psf) in April. The private condo is popular with upgraders because it is just a five-minute walk from the Woodlands MRT station, according to property agents. Adjacent to Casablanca is Woodhaven, a 337-unit residential development occupying a 225,600 sq ft site. The 99-year leasehold development offered a mix of condo units, small office, home office (SOHO) and townhouses, and saw strong sales when it was launched in mid-2011. Sale prices for the condos averaged $1,000 psf; the SOHO units were about $1,030 psf and the townhouses, $800 psf. The project was completed just last year. In Woodlands, FEO also developed executive condo La Casa, located off Woodlands Avenue 5. When the 444-unit EC was launched in 2005, average prices of units sold were $382 psf. The project was completed in 2008. According to a caveat lodged on Aug 15, a 904 sq ft unit changed hands for $734,000 ($812 psf). The seller had purchased it in December 2005 for $379,130 ($419 psf), thus enjoying an almost doubling in value of the property over the past decade. FEO also developed Nordcom 1 and Nordcom 2  two light industrial (Business 1) complexes  on Gambas Avenue. The industrial sites were purchased from JTC on 30-year leases. Nordcom 1 has a total of 131 strata industrial units, of which 50% have been sold; Nordcom 2 has 347 strata industrial units, of which 40% have been sold. While Nordcom 1 is targeted for completion later this year, Nordcom 2 is projected to be completed by 2018. In the latest transaction at Nordcom 2, a 1,668 sq ft unit on the fourth floor was sold for $475,000 ($285 psf) in June, based on caveats lodged. At Nordcom 1, the last transaction saw a 1,690 sq ft unit sold for $508,000 ($301 psf) in June last year. Woodlands is not the only area in which FEO has been a market pioneer. In 2012, we were a first mover in Punggol with the launch of Water town  a mixed-use complex with residential units and a shopping mall. We were also the first to introduce innercity living in Tanjong Pagar with the preview of Icon 13 years ago, she adds.  This article appeared in The Edge Property pullout, Issue 743 (Aug 29, 2016) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/fb-spaces-jurong-and-bedok-sale-30-mil</t>
+          <t>https://www.edgeprop.sg/property-news/mcc-land-hao-yuan-launched-highest-number-projects-2016</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Two F&amp;B spaces have been put up for sale by expression of interest (EOI). The indicative price for both is $30 million. Interested buyers could either buy them collectively or individually. The F&amp;B space located at 134 Jurong Gateway is being operated as an air-conditioned coffee shop and food court with an annex outdoor refreshment area. The indicative price for the coffee shop is $18 million. The other F&amp;B space is located at 744 Bedok Reservoir Road, next to Bedok Reservoir Park, and is currently leased to McDonalds Restaurant with an outdoor refreshment area. The subject property also comes with living quarters or a three-room flat on the second storey that is accessible separately. The indicative price for this F&amp;B unit is $12 million. Savills is the appointed sole marketing agent and the EOI closes on Nov 30.  134 Jurong Gateway  744 Bedok Reservoir Road Source: Savills</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/finance-broker-ultra-rich</t>
+          <t>https://www.edgeprop.sg/property-news/mcl-land-sells-329-units-parc-esta-average-price-1680-psf</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Three years ago, Masood Rashid, founding partner of London-based boutique financial brokerage firm Opes Financial Partners, thought it was a great opportunity when he was invited by a top UK law firm to provide financing for potential buyers at a weekend property exhibition in Hong Kong and Singapore. The project showcased was located in the exclusive neighbourhood of St Johns Wood, with prices starting from over 2 million. There was a lot of activity, and people were busy buying and signing contracts to purchase, recounts Rashid, 40. His business partner and director, Matthew Davies, who had attended the weekend exhibitions told him, Wow, its like a new gold rush. However, it was soon clear that many of the buyers had no intention of securing a mortgage as they had started to flip their properties. I saw it as a massive headache, says Rashid. That was the first and last time Opes took part in such an exhibition. Instead, he decided to focus on offering bespoke financing solutions to managers in Geneva, Switzerland and other major wealth hubs, including Singapore and Dubai. They found that many of the wealth man- agers do not provide lending services to clients  and Rashid saw an opportunity to plug that gap. The firm saw a lot of Russian clients and has since expanded its business to Asia and the Middle East. Given Rashids financing repertoire, he was able to provide an attractive financing deal for a Malaysian high-net-worth investor recently. The businessman had purchased a 3 mil- lion property in London. A Malaysian bank was only willing to finance up to 65% of the purchase price, or about 2 million. As the maximum loan repayment period was 65 years, and the client was already 60, the loan term was very short and his monthly mortgage, based on capital and interest repayment, would have been around 40,000. It was very high because they were looking at his age, says Rashid. When the investor was introduced to him, Rashid contacted a Swiss bank he had been dealing with. Within days, the bank agreed to finance the businessman. Based on an interest-only mortgage repayment, his monthly debt payment the ultra-rich for their purchases  from luxury London pads to private jets and yachts. Beyond the UK, Opes also provides financing for luxury home purchases in other key jurisdictions in Europe, for example Southern France, Marbella and Barcelona, as well as Dubai. Among the worlds top 5% His clients rank among the worlds top 5%, he says, and include the super rich from around the world, particularly the Middle East, India, Pakistan, Russia, Ukraine, the Commonwealth of Independent States (CIS) and China. My specialisation is in someone whos big, who could possibly be a PEP [politically exposed person], he adds. [The term] refers to any- one who is politically connected. As long as youre related to a politician  it could be a former or a current minister  youre a PEP. With London being a global financial hub, almost every bank in the world has a presence there. Regulated banks include overseas banks that are licensed to operate in the UK, but have to comply with the regulations of the UK regulatory body, the Financial Conduct Authority. Non-regulated banks are those that do not have a presence in the UK, but could still provide lending for UK property purchases. As they are not governed by the FCA, they are considered non-regulated. London property is considered a safe bet, and prices have a close correlation with gold prices But that doesnt mean they are dodgy, says Rashid. They have to comply with the regulations in their own jurisdictions. Opes works with both FCA-regulated and non-regulated banks to give clients greater access to financing solutions. Were at the top of the game, we know whos in and whos out of the market, he adds. Opes does its own due diligence on clients, and so do the banks it works with. Generally, if a client is on FCAs high risk list, the banks will have to do enhanced due diligence, basically a more stringent process. Recently, some of the major UK banks were reprimanded by the various regulatory authorities for being lax in their due diligence. The FCA used to post the list of 95 high- risk countries on its website. It includes almost every country outside the UK, North America and Australia, with the exception of Hong Kong and Singapore, says Rashid. The list was removed from the website late last year after Cayman Islands objected to being included for money laundering activities. Many of Rashids clients are referrals from major banks. He cites the example of a businessman from a former CIS state referred to him by a bank. The businessman wanted to purchase a home in London, and was looking for financing. Rashid secured a 10 million ($20.38 million) loan at a very low interest rate. As he had a US$50 million ($68.5 million) deposit with an offshore bank that was paying him an interest rate of 15%, he was able to use the interest earned to pay his mortgage, and still earn 1.5 million a year in interest. Its called arbitrage, says Rashid. People are hungry to borrow money. We can provide solutions [for them]. Naturally, Rashid has provided financing for some of the biggest residential deals in the UK, from a 50 million mansion to a 120 million property, as well as luxury apartments at One Hyde Park where prices are north of 6,000 psf. In our line of work, discretion is paramount, he says. Were dealing with private high-net-worth clients who want to stay private.  London property prices comparable to gold prices Typically, when theres an issue or a crisis in a country, there will be an influx of capital into London real estate, observes Rashid. For example, the problems in Ukraine last year saw an exodus of money. The Arab Spring conflict in 2012 saw money flooding in from Egypt and the Middle East. When France introduced the 75% tax on the rich, many moved to London, and purchased homes. People perceive London property as a safe bet, he says. Theres actually a close correlation between prices of London property and gold. Rashids entire business revolves around the premise of this continuous flood of foreign wealth into London. Our business has gone through the roof. As long as London continues to be a global city, we will continue to do good business. Rashid: My specialisation is in someone whos big, who could possibly be a PEP [politically exposed person] Having spent about a decade working for big mortgage brokerage firms in the UK such as Mortgage Matters Direct and John Charcol, as well as real estate equity firm Cobalt Capital Partners, Rashid started Opes together with Davies in 2011. Initially, the duo visited wealth was 2,500, less than 10% of what he would have paid had he signed on with the Malaysian bank. The Swiss bank assessed him based on his overall wealth, and not just his age and income, says Rashid. He was a wealthy, self-made man with a lot of property.  The quick flip Among Asians, buyers of big-ticket homes in London tend to be Chinese, Indonesians and Malaysians, says Rashid. However, Hong Kong and Singapore investors tend to have a trading mentality. A bubble has been created over the last four years, with people buying and selling upon completion, says Rashid. Many of the units are completing in the next two years. And if lending dries up, and the owner can- not secure a buyer or complete the purchase, he will be forced to sell at distressed prices. So, this is going to be a problem. Those buying a flipped contract (or UK properties in a sub-sale) tend to find difficulty in securing financing. There may have been one or two banks in the UK that had initially allowed it, but now they are saying no to reassigned contracts, he adds. So, a lot of these buyers whose game plan is short-term  buying and flip- ping the contract before, or at, completion  are going to struggle as there wont be much of a market. Rashid was recently referred to a Singaporean investor who had bought a UK property on a reassigned con- tract. He helped him secure a bridge loan until completion. Upon completion of the property, the owner will exit the bridge loan and secure a long-term mortgage at a lower interest rate. Its a complicated structure, admits Rashid. But it has to be structured in a way that doesnt kill the deal for the buyer. This article appeared in the City &amp; Country of Issue 670 (Mar 30) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/first-time-hdb-flat-buyers-get-enhanced-grant-income-ceiling-raised</t>
+          <t>https://www.edgeprop.sg/property-news/merchants-building-south-bridge-road-collective-sale</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">SINGAPORE (EDGEPROP) - From Sept 11, first-time HDB homebuyers will receive an enhanced housing grant that provides flexibility on flat type and location. The income ceiling for eligible buyers has also been raised for the first time since 2015. The new Enhanced CPF Housing Grant (EHG) simplifies the existing Additional CPF Housing Grant (AHG) and the Special CPF Housing Grant (SHG) of up to $40,000 respectively. The maximum grant under the EHG will be $80,000, with the income ceiling set at $9,000. This is higher than the AHGs cap of $5,000 and the SHGs cap of $8,500. The new grant applies to both new and resale flat purchases. Unlike the SHG, the EHG has no restrictions on flat type and location. This may help to boost demand for older flats as many of them are in mature estates and stabilise the resale market. Previously, the SHG is for non-mature estates, says Lee Sze Teck, Huttons Asias Director of Research. This year, HDB is on track to supply 15,000 units (Picture Credit: Albert Chua/EdgeProp Singapore) To be eligible for the EHG, first-time families have to purchase a flat with a remaining lease that covers them and their spouse until at least the age of 95. According to HDB, families who buy flats with leases that do not cover them until the age of 95 will still receive grants. However, this will be on a pro-rated basis. Meanwhile, eligible first-timer singles aged 35 and above who are earning not more than $4,500 a month can receive up to $40,000 under the EHG. Both families and singles who purchase resale flats within 4km to their parents homes can still receive the Proximity Housing Grant on top of the EHG. In addition, the monthly household income ceiling will increase from $12,000 to $14,000. This applies to eligible families purchasing a flat from the HDB, buying a resale flat with the CPF Housing Grant, or getting a HDB housing loan to buy a new or resale flat. The monthly household income ceiling for first-time single buyers will also increase from $6,000 to $7,000. Meanwhile, the monthly household income ceiling for households to purchase an executive condominium (EC) will be raised to $16,000 from $14,000 previously. With these enhancements, more young couples may want to buy BTO flats. To support this additional demand, we will increase our build-to-order (BTO) flat supply, said Minister Lawrence Wong at the HDB Awards 2019 on Sept 10. This year, HDB is on track to supply 15,000 units. Huttons Asias Lee observes that the private residential market is unlikely to be affected by these announcements as units in this segment are not subject to the five-year minimum occupation period (MOP). Additionally, homeowners are not restricted to who they can sell their units to. Check out the latest listing ofHDBnow  Read also: HDB resale price index falls 0.2%, transactions up 29.8%BTO or resale flat?HDB launches 6,753 flats for sale under May 2019 exercise </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/five-adjoining-conservation-shophouses-geylang-sale</t>
+          <t>https://www.edgeprop.sg/property-news/mg-real-estate-unveils-revamped-compass-one</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Five adjoining 3-storey conservation shophouses from 236 to 244 Geylang Road have been put up for sale via Expression of Interest at an indicative price of $28.8 million or $1,350 psf on total built-up area of 21,349 sq ft. The shophouses sit on freehold land approximately 7,411 sq ft in size. Located within Geylang Conservation Area, the site is zoned for Commercial usage under the 2014 Master Plan. The property is currently multi-tenanted with an eating house, a Chinese restaurant and a provision shop on the ground floor, and office and association on the upper floors. With the announcement of the rezoning of area bounded by Geylang Road, Lorong 22 Geylang, Guillemard Road and Lorong 4 Geylang, we have started to see an increase in interest and buying momentum for shophouses in the Geylang area, with 11 transactions this year to date in comparison to seven in 2014, says Clemence Lee, JLL Capital Markets Manager. This offering provides an opportunity for both investors and owner-occupiers to acquire a freehold commercial asset located in an area slated for commercial transformation. The expression of interest exercise will close on November 4, 2015 at 3pm. JLL is the exclusive marketing agent.  The subject property Source: JLL </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/five-adjoining-freehold-shophouses-kampong-glam-sale</t>
+          <t>https://www.edgeprop.sg/property-news/mix-heritage-and-luxury</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A row of five adjoining freehold shophouses in Kampong Glam is up for sale at $23.8 million, which translates to $2,970 psf. Located at 17, 19, 21, 23 and 25 Baghdad Street in the Kampong Glam Conservation Area, the five shophouses have areas each ranging from 1,375 sq ft to 2,416 sq ft. They make up a total floor area of about 8,013 sq ft, and occupy a combined land area of about 4,892 sq ft. The five adjoining shophouses at Baghdad Street (Credit: CBRE)  They come with a 60m triple-road frontage onto Baghdad Street, Bussorah Street and one side lane. The shophouses are currently fully tenanted and come with existing F&amp;B approvals. As they are zoned as commercial under the 2019 Draft Master Plan, there will be no additional buyers stamp duty or sellers stamp duty. They are open to both local and foreign buyers. The shophouses will garner keen interest from savvy investors with a medium- to long-term investment horizon who are seeking to benefit from future rental upside and capital appreciation, in addition to enjoying immediate rental income, says Yap Hui Yee, associate director, capital markets, CBRE. The latter is the sole marketing agent for the shophouses. The shophouses are held by a single owner, but each of the shophouses has its individual land title. The five land titles will provide the successful buyer the additional option to keep some of the units or sell them independently in the future, says Yap. The expression of interest exercise will close on July 16, 3pm.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/food-factories-offer-higher-yields-compared-office-retail-colliers</t>
+          <t>https://www.edgeprop.sg/property-news/mixed-prospects-singapore-property-market</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>In line with rising demand for food factories and central kitchens in Singapore, real estate consultancy Colliers expects such facilities to offer more attractive yields compared to office and retail, it highlighted in a report released on May 29. Colliers forecasts that food factories with 30-year land tenures are able to offer yields of about 6-7%, compared to 3.25-3.65% for office properties, and 4.4-4.9% for retail properties. Demand for food factories and central kitchens in the country has risen over the years, with a focus on major food zones in the east, north-east and central regions, the report states. A total of 637,115 sq ft of food factory space (equivalent to 1-2% of current food factory stock) has come into supply in 2019 to date, a surge from the 31,431 sq ft completed in the whole of 2018. Source: Colliers Factory rents and prices in major food zones in the east, north-east and central regions have outperformed the west and north regions, based on JTC data, according to the report. Colliers believes that this is due to their close proximity to the city centre or residential estates, which facilitates food catering and delivery services. However, in established food zones in the west region (Pandan Loop, Jalan Tepong) monthly rents can range from $1.50-2.40 psf, while those in the north region (Senoko Avenue, Mandai Link) can fetch $1.80-2.40 psf. Mature food manufacturing areas such as MacPherson, Pandan Loop and Bedok North are able to maintain occupancy between 80% and 100%, reveals the report. Meanwhile, those in newer and further-off locations, such as Tuas and Senoko, tend to have occupancies of around 60%. Colliers also found that well-located food factories with better facilities such as freezers can fetch about 25-35% higher prices than others. In March 2017, US-based PGIM Real Estate acquired 1 Buroh Lane, a cold store food distribution centre, at $300 psf, Collier highlights. In March 2019, WTT Trading divested its food factory with a cold store at 3 Mandai Link for $325 psf. The increased demand and rents in the F&amp;B industry reflect the Singapore governments push to raise productivity and cut reliance on manpower, as outlined in the Food Manufacturing Industry Transformation Map rolled out in November 2016. The plan includes developing quick models like ready-to-eat meals, promoting adoption of manpower-lean tech, equipping employees with new skills, and expanding the reach of Singapores F&amp;B companies globally. Source: Colliers Upcoming supply An upcoming 3.68 million sq ft of food factory space (9-10% of current food factory stock) is expected to come into supply, concentrated in the north, east and west regions. Of that, 80% is scheduled to be completed in 2019-2020. The largest upcoming project, JTC Bedok Food City, has a total gross floor area of more than 1 million sq ft, and is slated for completion in early 2020, notes Colliers. An integrated Halal Food Hub of 600,000 sq ft is also expected to be completed in two years, at a cost of $80 million-100 million. This was proposed this May by Elite Partners Capital and the Singapore Malay Chamber of Commerce and Industry to position Singapore at the forefront of innovation in the regions halal industry. Overall, Colliers forecasts demand to lag behind supply in 2019-2020. Demand, however, will be sustained by the rise of popularity of food delivery services and e-commerce  Foodpanda and Deliveroo started their central kitchens in the last two years; the need of F&amp;B operators to streamline retail spaces; and the governments push for greater productivity and innovation in F&amp;B, it says. Meanwhile, rents and prices of food factories are expected to remain largely stable over the next three to five years, it adds.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/food-factory-sale-boon-lay-18-million</t>
+          <t>https://www.edgeprop.sg/property-news/mnd-and-hdb-introduced-new-2-room-flexi-scheme</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve">A single-storey detached food factory at 2 Enterprise Road is up for sale at $18 million. The property is within the JTC Chin Bee Food Zone, and surrounded by food suppliers and manufacturers such as Neo Garden, Khong Guan, GSK, Unilever, Olam and Meiji. Located at the corner of Jalan Boon Lay and Enterprise Road, the factory occupies a land of 174,743 sq ft and a gross floor area (GFA) of 151,606 sq ft. Under URAs Master Plan 2014, it is zoned as Business 2 with a plot ratio of 2.5. It has a leasehold tenure of 60 years from JTC, with about 14 years left. Currently, the property is approved for warehousing and distribution of food and related products as well as meat processing. Facilities include a warehouse, production area, chiller and freezer rooms as well as loading bays. The future Enterprise MRT Station at the doorstep of the property will make it even more appealing. We envisage that this sale opportunity is likely to attract strong interest from a diverse mix of users from the food and beverage industry, says Shaun Poh, executive director of capital markets at Cushman &amp; Wakefield. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/forest-woods-sells-337-units-launch-day</t>
+          <t>https://www.edgeprop.sg/property-news/next-stage-co-working</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>On Saturday morning of Oct 8, crowds flooded into a tent adjacent to Nex shopping mall where balloting for units at the 519-unit Forest Woods private condo started at 10am. Excitement was high as more than 800 cheques had been collected during the fortnight of previews prior to the launch on Oct 8. By 5pm that day, 337 units or 65% of the total project had been sold at an average price of $1,400 psf. Were very encouraged by the strong response and demand for Forest Woods, said Chia Ngiang Hong, CDL group general manager. He attributes the overwhelming response to the right mix of prime location, unique features, attractive pricing and great value. According to CDL, all the unit types enjoyed a strong take-up, although the one-bedroom-plus-study and two-bedroom units were all sold. The two-bedroom units were popular because owners have the flexibility of turning the study into an en suite for the second bedroom, or an open study. Alternatively, it can also be converted into a walk-in wardrobe for the second bedroom. Prices of the units started from $688,000 for a one-bedroom-with-study, $830,000 for a two-bedroom, $1.1 million for a three-bedroom and $1.65 million for a four-bedroom unit. There were buyers of multiple units, including a family that was said to have snapped up four units. Even one of the three penthouses priced at $2.85 million was taken up that day.  Showflat of a three-bedroom unit Source: CDL  While many of the buyers were owner occupiers, the project also found favour with investors, especially the one- and two-bedroom units. Due to the limited supply of new projects in this prime location, investors also bought Forest Woods in anticipation of good rental demand, said Chia. 88% of the buyers were said to be Singaporeans, with permanent residents and foreigners making up the remaining 12%. Forest Woods is located within a five-minute walk of the Nex shopping mall, which is integrated with the Serangoon MRT Interchange station which connects the North-East and Circle Lines as well as the Serangoon bus interchange. The project is jointly marketed by ERA Realty, Huttons Asia and PropNex Realty.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/four-freehold-geylang-shophouses-market-14-mil</t>
+          <t>https://www.edgeprop.sg/property-news/no-lack-space-10-million-population</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Knight Frank Singapore is marketing the sale of four shophouses at the junction of Geylang Road and Lorong 33 Geylang. The properties have a guide price of $14 million. The adjoining two-storey conservation shophouses were affected by a fire in March this year. Before the fire, the shophouses used to house a tyre business, furniture retailer, and electrical shop. The properties have since been cleared out and will be sold with vacant possession. The four shophouses are at the junction of Geylang Road and Lorong 33 Geylang (Picture: Knight Frank Singapore)  The properties sit on a freehold land-plot of 5,113 sq ft with a plot ratio of 3.0 under the 2014 Master Plan. Prospective buyers can redevelop the land based on conservation guidelines set out by URA. As this is a secondary settlement area, there is potential for a rear extension, subject to approval, says Mary Sai, executive director, investment and capital markets, of Knight Frank Singapore. There is no additional buyers stamp duty and sellers stamp duty payable, and foreigners and companies are eligible to purchase the properties. As the owners are not GST-registered, no GST will be payable. The expression of interest for the shophouses closes on Aug 15.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-apartments-joo-chiat-still-road-and-telok-kurau</t>
+          <t>https://www.edgeprop.sg/property-news/north-park-residences-set-benchmark-projects-yishun-19768-0</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Property commentaries and analyses are often on large condominium projects and less on apartments. For those who are less familiar with the local property regulations, condos must have a minimum site area of 0.4ha to ensure sufficient space for facilities and greenery, among other parameters stipulated by URA. They are, therefore, perceived to be a higher-value private housing product, a notch above apartments. District 15 accounted for the bulk of the freehold apartment transactions outside the prime districts. These apartments dot the lanes branching out of Joo Chiat Road, Still Road and Telok Kurau Road. Many of them are low-rise, single-block projects with more basic facilities such as a small pool, gymnasium and clubhouse. Given their lack of facilities and green spaces, have apartments suffered a bigger setback in the ongoing property melee? Demand for freehold apartments is underpinned by their niche positioning. Freehold apartments offer value alternatives for buyers coveting a private address in District 15. In our basket of properties, prices of freehold apartments between 700 and 1,100 sq ft in the district, completed from 2000 onwards, averaged $1,248 psf, a significant discount to their freehold and 99-year leasehold condo counterparts in the area, which traded at $1,603 psf and $1,428 psf respectively. Separately, the average price of these freehold apartments is on par with some 99-year leasehold mass-market projects. It seems there is also limited stock of smaller-sized and affordable condos in District 15. Therefore, apartments in the area fill the gap between public and private homes for buyers with tighter budgets. Based on caveats lodged in 2014 and 2015, the average condo size in the district was 1,383 sq ft, and around 80% of the caveats involved units larger than 1,000 sq ft. On the other hand, the average size of apartments sold in 2014 and 2015  1,096 sq ft  is smaller relative to condos. Freehold apartments also appeal to those willing to trade off full condo facilities for exclusivity and tranquillity. Despite standing on compact land parcels, these apartments are nested among landed homes in a low 1.4 plot ratio neighbourhood, based on Master Plan 2014. A lifestyle retail concept adds character to the neighbourhood, in place of traditional suburban malls.   The average size of apartments in District 15 is smaller than condos in the area, making them more affordable  A lifestyle retail comcept adds character to the neighbourhood, in place of traditional suburban malls   The Edge Property found that prices of freehold apartments in District 15 have stayed relatively resilient against market headwinds. Analyses of a basket of freehold apartments in the area showed that the average price for units between 700 and 1,100 sq ft eased about 2%, from $1,267 psf at its peak in 1H2013 to $1,248 psf today. For comparison, the URA price index for all non-landed homes in the city fringe or Rest of Central Region (RCR) dipped 8% around the same period. Only four of the 29 properties surveyed saw prices falling at a rate close to or faster than 8%. In our analysis, prices in 1H2013 were derived based on actual transactions from caveats lodged with URA, while prices in 2015 were derived using Edge Fair Value, a valuation tool on TheEdgeProperty.com. It allows us to track the price movement of the same units between 1H2013 and today, despite a limited number of transactions. For example, an 850 sq ft low-floor unit at Tivoli Grande apartment was transacted at $1,423 psf in 1H2013. Edge Fair Value puts the price of the unit at $1,424 psf today. The tool utilises a valuation algorithm that takes into account variables, such as recent transactions of comparable properties, level, facing, size and outliers, in formulating the values. Using Edge Fair Value to derive the market rents for the same batch of units put the rental yields of these freehold apartments at 3.3%. In an up market, the prices of freehold apartments in District 15 have appreciated at similar rates as non-landed home prices in the city fringe or RCR. For example, an 872 sq ft low-floor unit at Callidora Ville in Telok Kurau was traded at $786 psf in June 2009. A similar unit in the project changed hands at $1,262 psf in June 2013. In another example, a 1,000-plus sq ft unit at One @ Pulasan was sold at $809 psf in March 2009. In June 2013, a similar unit in the project found a buyer at $1,122 psf.  This article appeared in The Edge Property Pullout of Issue 693 (September 7) of The Edge Singapore.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-b1-redevelopment-site-near-aljunied-mrt-sale-11-mil</t>
+          <t>https://www.edgeprop.sg/property-news/nouvel-18-sells-16-units-90-buyers-are-foreigners</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Freehold sites at Nos 81, 83 and 85 Aljunied Road have been launched for sale by expression of interest. The asking price for the three properties is said to be $11 million, or $760 psf per plot ratio. Three adjoining residential terrace houses are currently sitting on the sites, which have a total land area of 6,047 sq ft. Under the 2014 Master Plan, the property is zoned for Business 1 use with a plot ratio of 2.5. The freehold plots can be redeveloped into a seven-storey light industrial building with a maximum gross floor area of up to 15,118 sq ft, subject to approval from the authorities. The property is sited on Aljunied Road, off Sims Avenue. It is located in the light industrial cluster of Sims Drive/Sims Avenue and surrounded by modern industrial buildings such as Atrix@Aljunied, Victory Centre, Agrow Building and One Sims Lane. The property is about 100m from Aljunied MRT station. Cushman and Wakefield is the exclusive marketing agent for the property. The EOI closes on Oct 26.  Three adjoining residential terrace houses are currently sitting on the sites Souce: Cushman and Wakefield </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-commercial-building-joo-chiat-market-20-mil</t>
+          <t>https://www.edgeprop.sg/property-news/oil-tycoon-shifts-focus-real-estate</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>A freehold commercial building at 118 Joo Chiat Road has been launched for sale at a guide price of $20 million. The price translates to about $1,077 psf on the existing gross floor area (GFA). The four-storey building sits on a 4,686 sq ft site, and has a GFA of 18,571 sq ft. It comes with an attic and a lift. The building is zoned for commercial use under the 2014 Master Plan, and is currently approved for shops on the ground floor and offices on the upper floors. There is also a mechanical car park for nine cars in the building. The freehold commercial building at 118 Joo Chiat Road (picture: JLL) The new owner could have naming and signage rights for the building. The existing tenancies could be terminated for an owner-occupier to move in immediately, or an investor could refurbish the building or change the tenant mix. Alternatively, the driveway could be decanted to make way for additional retail space on the ground floor. Based on a URA reply, up to 40% of the GFA could be considered for residential use, says Clemence Lee, senior director, capital markets, at JLL. The property is a 10-minute walk from Paya Lebar and Eunos MRT stations, and is a 15-minute drive to the CBD. It is also accessible by the Pan-Island and Kallang-Paya Lebar Expressways. The sale is through an expression of interest exercise, which closes on May 14.</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-industrial-building-aljunied-sale-23-mil</t>
+          <t>https://www.edgeprop.sg/property-news/one-10-transactions-3q2015-were-unprofitable</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve">A freehold industrial building at 51 Lorong 21 Geylang is on the market for $23 million, or $599 psf per plot ratio, according to Edmund Tie &amp; Co (ET&amp;Co), the sole marketing agent for the sale. The property is held under a single ownership which is likely to make for a straightforward sale. The relatively palatable quantum of the property presents a rare opportunity for end-users and developers to acquire a rare freehold industrial site at a city-fringe location, says Swee Shou Fern, executive director of investment advisory at ET&amp;Co. Picture: ET&amp;Co The new owner will also have potential signage and naming rights for the property. Located in a mature industrial cluster near Aljunied MRT Station, the property sits on a site of 15,364 sq ft. The land has a gross plot ratio of 2.5, and is zoned for Business 1 use under the 2014 Master Plan. The site may be redeveloped to a maximum allowable gross floor area of 38,410 sq ft, and no development charge is payable, the agent says. The tender exercise will close on May 28. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-industrial-building-macpherson-sale-159-mil</t>
+          <t>https://www.edgeprop.sg/property-news/one-global-%E2%80%98shaking-%E2%80%99-international-property-marketing-business-singapore</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">A freehold industrial building, at 14 Genting Road in MacPherson, is up for sale at $15.9 million ($938.44 psf per plot ratio). The five-storey industrial building occupies a site of 5,758 sq ft, with a gross floor area of around 16,943 sq ft. It houses production areas on levels one to three, and secondary workers dormitories on levels four and five. Under URAs 2014 Master Plan, the site is zoned under Industrial (B1), for clean and light industrial usage. It has a gross plot ratio of 2.5. The site is currently approved for use as a secondary workers dormitory, and may also be used by end-users from clean and light industries requiring production, storage, or ancillary office spaces, according to Knight Frank Singapore, which is marketing the property. 14 Genting Road is close to mature industrial estates such as Aljunied, Kallang, Tai Seng, Kim Chuan and Ubi, highlights Knight Frank. The tender for the property will close on March 13, at 3pm. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-properties-balestier-and-east-coast-sale</t>
+          <t>https://www.edgeprop.sg/property-news/orchard-road-retail-rents-may-inch-08-y-o-y-year</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/freehold-properties-balestier-and-east-coast-sale</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/gcb-dalvey-estate-sale-auction-30-mil</t>
+          <t>https://www.edgeprop.sg/property-news/oue-trendsetter</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/gcb-dalvey-estate-sale-auction-30-mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/glimpse-eden-swire-properties%E2%80%99-first-ultra-luxury-condo-singapore</t>
+          <t>https://www.edgeprop.sg/property-news/paradise-lost</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/glimpse-eden-swire-properties%E2%80%99-first-ultra-luxury-condo-singapore</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/global-citizen-global-investor</t>
+          <t>https://www.edgeprop.sg/property-news/paya-lebar-quarter-%E2%80%94-catalyst-future-commercial-hub</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/global-citizen-global-investor</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/good-value-city-fringe-living</t>
+          <t>https://www.edgeprop.sg/property-news/pm-lee-announces-new-initiatives-amk-and-sengkang-west</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/good-value-city-fringe-living</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/government-raises-development-charge-rates-non-landed-residential-sector</t>
+          <t>https://www.edgeprop.sg/property-news/possible-extension-jurong-region-line-circle-line</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/government-raises-development-charge-rates-non-landed-residential-sector</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/grab%E2%80%99s-new-one-north-hq-house-its-largest-rd-centre</t>
+          <t>https://www.edgeprop.sg/property-news/potential-launches-2h2016</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grab and Ascendas Real Estate Investment Trust broke ground for the formers new headquarters at one-north business park on Friday (March 29) morning. The new building will house Grabs largest R&amp;D centre as well as some 3,000 employees. From left: Tan Hooi Ling (Grab Co-Founder), Manohar Khiatani (Ascendas-Singbridge Deputy Group CEO), Minister Heng Swee Keat and Anthony Tan (Grab CEO &amp; Co-founder) with the 3D model of Grab's future HQ (Credit: Grab) Our new headquarters represents our long-term commitment to Singapore and the region; the new space will cater to our evolving business demands as we continue to innovate and use technology to meet our customers daily needs, says Lim Kell Jay, Grab Singapores country head. Grab also launched its second batch of Grab Ventures Velocity (GVV) programme targeted at post-seed start-ups. Introduced in June 2018, the programme allows start-ups to test and commercialise their solutions with Grabs customer base. Applications are open until May 15 to start-ups across Southeast Asia. </t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ground-floor-strata-fb-space-grand-building-selling-18-mil</t>
+          <t>https://www.edgeprop.sg/property-news/price-war-workers%E2%80%99-dormitories</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/ground-floor-strata-fb-space-grand-building-selling-18-mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ground-floor-unit-bukit-timah-shopping-centre-going-58-mil</t>
+          <t>https://www.edgeprop.sg/property-news/property-auctions-how-low-do-prices-really-go</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/ground-floor-unit-bukit-timah-shopping-centre-going-58-mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/habitap-one-app-rule-them-all</t>
+          <t>https://www.edgeprop.sg/property-news/property-bukit-merah</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/habitap-one-app-rule-them-all</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/hefty-loss-incurred-despite-19-year-holding-period</t>
+          <t>https://www.edgeprop.sg/property-news/property-prices-rise-7-2018</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/hefty-loss-incurred-despite-19-year-holding-period</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/high-park-residences-hits-right-note-buyers</t>
+          <t>https://www.edgeprop.sg/property-news/ready-or-not-short-term-rentals-here-stay</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/high-park-residences-hits-right-note-buyers</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/high-park-residences-rises-amid-uncertainty</t>
+          <t>https://www.edgeprop.sg/property-news/real-life-dos-and-donts-property-investing-2462166-0</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/high-park-residences-rises-amid-uncertainty</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/high-specification-industrial-building-paya-lebar-sale</t>
+          <t>https://www.edgeprop.sg/property-news/rebirth-swan-maclaren</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/high-specification-industrial-building-paya-lebar-sale</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/hilltops-unit-sold-2397-psf</t>
+          <t>https://www.edgeprop.sg/property-news/recent-ec-launches-20-30-cheaper-new-private-condos</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/hilltops-unit-sold-2397-psf</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/house-fortune</t>
+          <t>https://www.edgeprop.sg/property-news/redevelopment-site-cuscaden-road-170-million</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/house-fortune</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/house-tour-jerome-and-sarahs-charming-home-industrial-style-mezzanine</t>
+          <t>https://www.edgeprop.sg/property-news/reinventing-soilbuild-group</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/house-tour-jerome-and-sarahs-charming-home-industrial-style-mezzanine</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/how-do-mrt-stations-affect-property-prices-and-rent</t>
+          <t>https://www.edgeprop.sg/property-news/resale-unit-regency-park-reaps-165-mil-profit</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/how-do-mrt-stations-affect-property-prices-and-rent</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/how-has-singapore%E2%80%99s-first-dbss-project-fared-against-resale-hdbs</t>
+          <t>https://www.edgeprop.sg/property-news/residential-market-see-spike-new-launches</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/how-has-singapore%E2%80%99s-first-dbss-project-fared-against-resale-hdbs</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/how-rents-fared-hdb-flats</t>
+          <t>https://www.edgeprop.sg/property-news/retail-units-holland-road-shopping-centre-and-industrial-unit-211-henderson-sale</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/how-rents-fared-hdb-flats</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/impact-mrt-property-prices</t>
+          <t>https://www.edgeprop.sg/property-news/revitalising-potong-pasir%E2%80%99s-private-property-market</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/impact-mrt-property-prices</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/industrial-building-tai-seng-sale-23-mil</t>
+          <t>https://www.edgeprop.sg/property-news/revival-sales-sentosa-cove-bungalows</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/industrial-building-tai-seng-sale-23-mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/inside-48-mil-copper-house</t>
+          <t>https://www.edgeprop.sg/property-news/richard-jany-weathering-ups-and-downs</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/inside-48-mil-copper-house</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ioi-offers-257-billion-central-boulevard-white-site</t>
+          <t>https://www.edgeprop.sg/property-news/roxy-pacific%E2%80%99s-overseas-gambit</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/ioi-offers-257-billion-central-boulevard-white-site</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/iwg-banks-multi-brand-strategy-growth</t>
+          <t>https://www.edgeprop.sg/property-news/safdie%E2%80%99s-%E2%80%98step-pyramid%E2%80%99-bishan</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/iwg-banks-multi-brand-strategy-growth</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/just-sold-caribbean-keppel-bay-unit-sold-145-mil-profit</t>
+          <t>https://www.edgeprop.sg/property-news/sales-mon-jervois-pick-after-completion</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/just-sold-caribbean-keppel-bay-unit-sold-145-mil-profit</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/karamjit-singh-leave-jlls-residential-team</t>
+          <t>https://www.edgeprop.sg/property-news/savills-singapore-launches-business-valuation-advisory-team</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/karamjit-singh-leave-jlls-residential-team</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/kingsford-bets-riverfront-location-upper-serangoon-view</t>
+          <t>https://www.edgeprop.sg/property-news/sentosa-cove-condo-changed-hands-1368-psf</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/kingsford-bets-riverfront-location-upper-serangoon-view</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/kingsford-waterbay-sells-140-units-launch-weekend</t>
+          <t>https://www.edgeprop.sg/property-news/shophouse-holland-avenue-sale</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/kingsford-waterbay-sells-140-units-launch-weekend</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/landed-homes-below-2-million</t>
+          <t>https://www.edgeprop.sg/property-news/shophouses-kampong-glam-and-little-india-poised-be-next-growth-area</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/landed-homes-below-2-million</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/landed-houses-flipped-million-dollar-profits</t>
+          <t>https://www.edgeprop.sg/property-news/shophouses-ripe-picking</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/landed-houses-flipped-million-dollar-profits</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/lawrence-wong-urges-prudence-buyers-and-developers</t>
+          <t>https://www.edgeprop.sg/property-news/shophouses-upper-east-coast-road-tanjong-katong-road-and-jalan-besar-sale</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/lawrence-wong-urges-prudence-buyers-and-developers</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/lian-beng-oxley-launch-strata-titled-industrial-building-tampines</t>
+          <t>https://www.edgeprop.sg/property-news/signature-yishun-open-applications-polling-day</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/lian-beng-oxley-launch-strata-titled-industrial-building-tampines</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/location-scan-shunfu-ville-collective-sale-whats-its-vicinity</t>
+          <t>https://www.edgeprop.sg/property-news/sim-lian-launch-and-lease-200000-sq-ft-office-space-vision-exchange</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/location-scan-shunfu-ville-collective-sale-whats-its-vicinity</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/location-scan-sit%E2%80%99s-new-campus-punggol</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-evolves-so-does-edgeprop</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/location-scan-sit%E2%80%99s-new-campus-punggol</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/logistics-building-spacetampines-market-170-mil</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-has-best-prospects-investment-asia-pacific</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/logistics-building-spacetampines-market-170-mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/lost-decade-sentosa-cove-singapores-billionaire-haven</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-home-prices-have-bottomed-hong-kongs-are-%E2%80%98crazy%E2%80%99-bnp</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/lost-decade-sentosa-cove-singapores-billionaire-haven</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/malls-revitalise-amid-retail-woes</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-investors-snap-us5-billion-chinas-commercial-properties-brushing-aside-trade-war-concerns</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/malls-revitalise-amid-retail-woes</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/manhattan-house-collective-sale-300-mil</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-shopping-centre-launched-collective-sale-255-mil</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/manhattan-house-collective-sale-300-mil</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/martin-place-residential-site-fetched-1239-psf-ppr</t>
+          <t>https://www.edgeprop.sg/property-news/singaporeans-are-loving-luxury-homes-foreigners-cant-buy</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/martin-place-residential-site-fetched-1239-psf-ppr</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mcc-land-hao-yuan-launched-highest-number-projects-2016</t>
+          <t>https://www.edgeprop.sg/property-news/slb-development-looks-new-horizons</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/mcc-land-hao-yuan-launched-highest-number-projects-2016</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mcl-land-sells-329-units-parc-esta-average-price-1680-psf</t>
+          <t>https://www.edgeprop.sg/property-news/slower-sales-and-launches-due-june-holidays</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/mcl-land-sells-329-units-parc-esta-average-price-1680-psf</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/merchants-building-south-bridge-road-collective-sale</t>
+          <t>https://www.edgeprop.sg/property-news/sri5000-splits-slp-international</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/merchants-building-south-bridge-road-collective-sale</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mg-real-estate-unveils-revamped-compass-one</t>
+          <t>https://www.edgeprop.sg/property-news/stamp-duty-common-mistakes-avoid</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/mg-real-estate-unveils-revamped-compass-one</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mix-heritage-and-luxury</t>
+          <t>https://www.edgeprop.sg/property-news/stars-kovan-star-qualities</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/mix-heritage-and-luxury</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mixed-prospects-singapore-property-market</t>
+          <t>https://www.edgeprop.sg/property-news/stars-kovan-unveiled</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/mixed-prospects-singapore-property-market</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mnd-and-hdb-introduced-new-2-room-flexi-scheme</t>
+          <t>https://www.edgeprop.sg/property-news/steady-stream-well-heeled-visitors-meyer-mansion-preview-weekend</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/mnd-and-hdb-introduced-new-2-room-flexi-scheme</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/next-stage-co-working</t>
+          <t>https://www.edgeprop.sg/property-news/strata-office-space-faces-stiff-competition</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/next-stage-co-working</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/no-lack-space-10-million-population</t>
+          <t>https://www.edgeprop.sg/property-news/sultan-plaza-collective-sale-380-mil</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/no-lack-space-10-million-population</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/north-park-residences-set-benchmark-projects-yishun-19768-0</t>
+          <t>https://www.edgeprop.sg/property-news/superbowl-jurong-sale-20-million</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/north-park-residences-set-benchmark-projects-yishun-19768-0</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/nouvel-18-sells-16-units-90-buyers-are-foreigners</t>
+          <t>https://www.edgeprop.sg/property-news/surge-top-end-prices-2018</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/nouvel-18-sells-16-units-90-buyers-are-foreigners</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/oil-tycoon-shifts-focus-real-estate</t>
+          <t>https://www.edgeprop.sg/property-news/tanjong-pagar-new-waterfront-city</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/oil-tycoon-shifts-focus-real-estate</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/one-10-transactions-3q2015-were-unprofitable</t>
+          <t>https://www.edgeprop.sg/property-news/tanjong-rhu%E2%80%99s-draws-%E2%80%94-city-fringe-location-waterfront-views</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/one-10-transactions-3q2015-were-unprofitable</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/one-global-%E2%80%98shaking-%E2%80%99-international-property-marketing-business-singapore</t>
+          <t>https://www.edgeprop.sg/property-news/teambuild-land-pares-down-property-development-business</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/one-global-%E2%80%98shaking-%E2%80%99-international-property-marketing-business-singapore</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/orchard-road-retail-rents-may-inch-08-y-o-y-year</t>
+          <t>https://www.edgeprop.sg/property-news/teho-backs-out-macpherson-deal</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/orchard-road-retail-rents-may-inch-08-y-o-y-year</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/oue-trendsetter</t>
+          <t>https://www.edgeprop.sg/property-news/thong-sia-building-sold-380-million-largest-ever-mixed-use-collective-sale</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/oue-trendsetter</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/paradise-lost</t>
+          <t>https://www.edgeprop.sg/property-news/three-balestier-road-shophouses-going-95-mil</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/paradise-lost</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/paya-lebar-quarter-%E2%80%94-catalyst-future-commercial-hub</t>
+          <t>https://www.edgeprop.sg/property-news/three-generations-enjoy-privacy-under-one-roo</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/paya-lebar-quarter-%E2%80%94-catalyst-future-commercial-hub</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/pm-lee-announces-new-initiatives-amk-and-sengkang-west</t>
+          <t>https://www.edgeprop.sg/property-news/three-landed-homes-sold-3-mil-profit</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/pm-lee-announces-new-initiatives-amk-and-sengkang-west</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/possible-extension-jurong-region-line-circle-line</t>
+          <t>https://www.edgeprop.sg/property-news/three-office-units-peninsular-plaza-going-929-mil</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/possible-extension-jurong-region-line-circle-line</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/potential-launches-2h2016</t>
+          <t>https://www.edgeprop.sg/property-news/three-storey-conservation-shophouse-chinatown-sale-85-mil</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/potential-launches-2h2016</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/price-war-workers%E2%80%99-dormitories</t>
+          <t>https://www.edgeprop.sg/property-news/top-gainer-makes-record-169-mil-profit-watermark-robertson-quay</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/price-war-workers%E2%80%99-dormitories</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/property-auctions-how-low-do-prices-really-go</t>
+          <t>https://www.edgeprop.sg/property-news/trouble-paradise</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/property-auctions-how-low-do-prices-really-go</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/property-bukit-merah</t>
+          <t>https://www.edgeprop.sg/property-news/two-freehold-commercial-shophouses-sale</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/property-bukit-merah</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/property-prices-rise-7-2018</t>
+          <t>https://www.edgeprop.sg/property-news/under-hammer-unit-coastal-view-residences-going-785000</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/property-prices-rise-7-2018</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ready-or-not-short-term-rentals-here-stay</t>
+          <t>https://www.edgeprop.sg/property-news/unit-nassim-sold-20-mil</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/ready-or-not-short-term-rentals-here-stay</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/real-life-dos-and-donts-property-investing-2462166-0</t>
+          <t>https://www.edgeprop.sg/property-news/unit-price-horizon-towers-falls-below-1000-psf</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/real-life-dos-and-donts-property-investing-2462166-0</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/rebirth-swan-maclaren</t>
+          <t>https://www.edgeprop.sg/property-news/unit-sea-view-fetches-1900-psf</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/rebirth-swan-maclaren</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/recent-ec-launches-20-30-cheaper-new-private-condos</t>
+          <t>https://www.edgeprop.sg/property-news/units-nassim-park-residences-cross-3500-psf</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/recent-ec-launches-20-30-cheaper-new-private-condos</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/redevelopment-site-cuscaden-road-170-million</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/redevelopment-site-cuscaden-road-170-million</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/reinventing-soilbuild-group</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/reinventing-soilbuild-group</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/resale-unit-regency-park-reaps-165-mil-profit</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/resale-unit-regency-park-reaps-165-mil-profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/residential-market-see-spike-new-launches</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/residential-market-see-spike-new-launches</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/retail-units-holland-road-shopping-centre-and-industrial-unit-211-henderson-sale</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/retail-units-holland-road-shopping-centre-and-industrial-unit-211-henderson-sale</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/revitalising-potong-pasir%E2%80%99s-private-property-market</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/revitalising-potong-pasir%E2%80%99s-private-property-market</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/revival-sales-sentosa-cove-bungalows</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/revival-sales-sentosa-cove-bungalows</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/richard-jany-weathering-ups-and-downs</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/richard-jany-weathering-ups-and-downs</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/roxy-pacific%E2%80%99s-overseas-gambit</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/roxy-pacific%E2%80%99s-overseas-gambit</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/safdie%E2%80%99s-%E2%80%98step-pyramid%E2%80%99-bishan</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/safdie%E2%80%99s-%E2%80%98step-pyramid%E2%80%99-bishan</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/sales-mon-jervois-pick-after-completion</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/sales-mon-jervois-pick-after-completion</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/savills-singapore-launches-business-valuation-advisory-team</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/savills-singapore-launches-business-valuation-advisory-team</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/sentosa-cove-condo-changed-hands-1368-psf</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/sentosa-cove-condo-changed-hands-1368-psf</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/severed-garden-eden-hall</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The second floor verandah of the British High Comissioners official residence, Eden Hall at 28 Nassim Road, commands a fine prospect of the front lawn, which is ringed by old trees, with the Union Jack fluttering in the wind. That view and the house itself is still protected, although the rest of the estate is up for grabs. This is because the UK government has carved up two plots (Plots A and B) on the eastern side of Eden Hall for sale by public tender. The sites have a combined land area of 34,254 sq ft, and amounts to 35% of the existing grounds of 97,889 sq ft. Plot A has a site area of 18,620 sq ft, and a 36 m frontage along Nassim Road. It includes a huge part of the garden along the driveway and an open air parking space for about six cars. The other land parcel, Plot B, has a long narrow driveway leading up to an elevated rectangular site adjacent to the house. Plot B has a total area of 15,634 sq ft. Both sites are zoned for residential use under the Good Class Bungalow (GCB) area of Nassim Road, the most prestigious address in Singapore. Given its wider frontage along Nassim Road, Plot A has a price tag of $2,200 psf, with the absolute price amounting to $40.96 million. Plot B is priced lower at $2,000 psf, owing to its long driveway, which translates to an absolute price of $31.27 million. CBRE is the sole marketing agent for both plots.  The front lawn of Eden Hall will be retained by the British government  Why sell now? The sale of Plots A and B will mean not just the loss of the eastern part of the garden but the swimming pool too. In return, the British High Commissioner will gain two new neighbours among Singapores seriously rich. The UK government has a responsibility to the taxpayer to ensure that its owned estate is of the right size necessary to undertake the functions associated with the estate, according to a statement by the British governments Foreign &amp; Commonwealth Office (FCO). The sale was undertaken as part of a regular review by FCO of its overseas estate in order to achieve better value and efficiency, it said. In this instance the garden at Eden Hall is larger than is necessary to accommodate the official functions of the HC Residence. Following the sale of these two garden plots, the total land area will be reduced to 63,893 sq ft, which is the minimum size required to maintain the value of Eden Hall, while allowing the normal residence functions to continue, adds the FCO. The British high commissioners residence will continue at Eden Hall, which is a 14,000 sq ft double storey house. It has three reception rooms on the first level, and another reception room on the second level with a wraparound verandah. There are also six bedrooms on the second level.  Steeped in history The house at Eden Hall has a rich history. Designed by renowned architect R.A.J. Bidwell of Singapores oldest and most prominent architectural firm Swan &amp; McLaren, it was built in 1904. The owner was Jewish merchant Ezekiel Saleh Manasseh, a trader in rice and opium, as well as a co-owner of Goodwood Park Hotel between 1918 and 1945. Bidwell was also the architect of Goodwood Park Hotel, Raffles Hotel and the Victoria Theatre and Concert Hall. The house was initially leased to Elizabeth Campbell, who operated a boarding house, Manasseh purchased the 4.75 acre land which the property sat on from his business partner for $30,000 in 1912. He moved into Eden House four years later with his family, and they lived there until 1942 when Singapore fell to the Japanese. Manasseh was sent to Changi Prison, where he later died in the prison hospital at Sime Road. His stepson, Vivian Bath, was sent to a labour camp on the Japanese island of Hokkaido. During the Japanese Occupation, Eden Hall was used by the Japanese as an officers mess. It was requisitioned for the use by the British forces after the occupation. And when Bath returned to Singapore, he regained possession of Eden Hall When Bath decided to retire in Australia, he sold Eden Hall to the British Government in 1957 for a nominal sum of 56,000, with the stipulation that a plaque be installed at the bottom of the flagpole, which reads, May the Union Jack fly here forever.  The neighbours Prior to 2002, the house sat on a sprawling 207,000 sq ft of freehold land, with tennis courts, stables and a swimming pool. The tennis courts and stables disappeared 13 years ago when the FCO sold half the land on the western side of Eden Hall to two prominent businessmen, namely Sam Goi of Tee Yih Jia Foods aka The Popoah King who has since ventured into property development investment, and Peter Kwee of Group Exklusiv, a renowned European car distributor, owner of Laguna Golf &amp; Country Club, as well as a string of properties and hotels. The duo reportedly paid $50.4 million for the site, and subsequently split up the site between them. Kwee took the larger plot of 63,300 sq ft, which he then carved up into two plots. One plot of 39,383 sq ft was sold to Indonesian businesswoman Sukmawati Widjaja or Oei Siu Hua, the executive chairman of Singapore listed company Top Global. She paid $25.5 million ($647 psf) for the site back in 2003. Sukmawati has made the house at Nassim Road her primary residence and is living there with her family. Kwee sold the second plot of 23,920 sq ft to Tay Liam Wee, the former chairman and managing director of Sincere Watch. The selling price was said to be $47.8 million or $2,000 psf in 2012, in a deal brokered by KH Tan of Newsman Realty. Goi has since built his home on the Nassim Road plot. The triangular plot fronting Nassim Road is still vacant. Word on the street is that Tay had appointed a Japanese architect to design the GCB, but the property has yet to be built. Given the shape of plots A and B, which the UK government has offered for sale by public tender, Newsmans Tan believes that the asking prices are in line with market values. According to Sammi Lim, associate director of investment properties at CBRE, Its a fair guide price in the current market and pegged to the previous price, she adds.  Prices coming off Traditionally, people prefer a site with a wider frontage and therefore the price psf of Plot A is higher at $2,200 psf, acknowledges Sammi Lim, associate director of investment properties at CBRE. However, the fact that Plot B is on an elevated site, and has a long driveway means that it is more exclusive. Lim sees expressions of interest for the separate plots, as well as parties interested in the combined sites. She sees the two plots attracting interest of those seeking an empty plot so they can design and build their own home. At the peak of the market in April 2013, Cheng Wai Keung, the executive chairman of Wing Tai Holdings had launched for sale a two-storey home sitting on an 85,000 sq ft elevated plot at 33 Nassim Road. The asking price for the property was $300 million or $3,529 psf. Had it been sold at that price, it would have shattered all records, both in terms of absolute and price psf. Over the past year, GCB transactions have come off, and so have average prices. Data from CBRE Research showed that in 2014, there were 28 GCB transactions totalling $626.14 million. Average transacted price was $22.36 million or $1,428 psf in 2014. For 2015, there have only been 18 GCB transactions  which is the lowest level seen since 1996, according to CBRE Research. Total transaction value for the year to date rang in at $500.78 million. While the average price per GCB was higher at $27.82 million relative to 2014s $22.36 million, on a price psf basis, it was 18.8% lower at $1,159 psf. For many interested parties looking at the two parcels offered for sale by the UK government, the main attraction is the house address, No. 28, according to a property agent who declined to be named. Being able to call the British High Commissioner ones neighbour may lend a certain measure of prestige and bragging rights. It is definitely a once in a lifetime opportunity to be able to stay in a GCB next to the British High Commissioners home, says CBREs Lim. However, there is no assurance that one will get invited over for tea.  Interested in apartments / condos near Eden Hall? Click here  This article appeared in the City &amp; Country of Issue 705 (Nov 30, 2015) of The Edge Singapore. </t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/shophouse-holland-avenue-sale</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/shophouse-holland-avenue-sale</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/shophouses-kampong-glam-and-little-india-poised-be-next-growth-area</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/shophouses-kampong-glam-and-little-india-poised-be-next-growth-area</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/shophouses-ripe-picking</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/shophouses-ripe-picking</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/shophouses-upper-east-coast-road-tanjong-katong-road-and-jalan-besar-sale</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/shophouses-upper-east-coast-road-tanjong-katong-road-and-jalan-besar-sale</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/signature-yishun-open-applications-polling-day</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/signature-yishun-open-applications-polling-day</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/sim-lian-launch-and-lease-200000-sq-ft-office-space-vision-exchange</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/sim-lian-launch-and-lease-200000-sq-ft-office-space-vision-exchange</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-evolves-so-does-edgeprop</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/singapore-evolves-so-does-edgeprop</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-has-best-prospects-investment-asia-pacific</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/singapore-has-best-prospects-investment-asia-pacific</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-home-prices-have-bottomed-hong-kongs-are-%E2%80%98crazy%E2%80%99-bnp</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/singapore-home-prices-have-bottomed-hong-kongs-are-%E2%80%98crazy%E2%80%99-bnp</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-investors-snap-us5-billion-chinas-commercial-properties-brushing-aside-trade-war-concerns</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/singapore-investors-snap-us5-billion-chinas-commercial-properties-brushing-aside-trade-war-concerns</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-shopping-centre-launched-collective-sale-255-mil</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/singapore-shopping-centre-launched-collective-sale-255-mil</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/singaporeans-are-loving-luxury-homes-foreigners-cant-buy</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/singaporeans-are-loving-luxury-homes-foreigners-cant-buy</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/slb-development-looks-new-horizons</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/slb-development-looks-new-horizons</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/slower-sales-and-launches-due-june-holidays</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/slower-sales-and-launches-due-june-holidays</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/sri5000-splits-slp-international</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/sri5000-splits-slp-international</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/stamp-duty-common-mistakes-avoid</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/stamp-duty-common-mistakes-avoid</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/stars-kovan-star-qualities</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/stars-kovan-star-qualities</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/stars-kovan-unveiled</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/stars-kovan-unveiled</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/steady-stream-well-heeled-visitors-meyer-mansion-preview-weekend</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/steady-stream-well-heeled-visitors-meyer-mansion-preview-weekend</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/strata-office-space-faces-stiff-competition</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/strata-office-space-faces-stiff-competition</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/sultan-plaza-collective-sale-380-mil</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/sultan-plaza-collective-sale-380-mil</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/superbowl-jurong-sale-20-million</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/superbowl-jurong-sale-20-million</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/surge-top-end-prices-2018</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/surge-top-end-prices-2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/tanjong-pagar-new-waterfront-city</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/tanjong-pagar-new-waterfront-city</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/tanjong-rhu%E2%80%99s-draws-%E2%80%94-city-fringe-location-waterfront-views</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/tanjong-rhu%E2%80%99s-draws-%E2%80%94-city-fringe-location-waterfront-views</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/teambuild-land-pares-down-property-development-business</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/teambuild-land-pares-down-property-development-business</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/teho-backs-out-macpherson-deal</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/teho-backs-out-macpherson-deal</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/thong-sia-building-sold-380-million-largest-ever-mixed-use-collective-sale</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/thong-sia-building-sold-380-million-largest-ever-mixed-use-collective-sale</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/three-balestier-road-shophouses-going-95-mil</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/three-balestier-road-shophouses-going-95-mil</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/three-generations-enjoy-privacy-under-one-roo</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/three-generations-enjoy-privacy-under-one-roo</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/three-landed-homes-sold-3-mil-profit</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/three-landed-homes-sold-3-mil-profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/three-office-units-peninsular-plaza-going-929-mil</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/three-office-units-peninsular-plaza-going-929-mil</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/three-storey-conservation-shophouse-chinatown-sale-85-mil</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/three-storey-conservation-shophouse-chinatown-sale-85-mil</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/top-gainer-makes-record-169-mil-profit-watermark-robertson-quay</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/top-gainer-makes-record-169-mil-profit-watermark-robertson-quay</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/trouble-paradise</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/trouble-paradise</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/two-freehold-commercial-shophouses-sale</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/two-freehold-commercial-shophouses-sale</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/under-hammer-unit-coastal-view-residences-going-785000</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/under-hammer-unit-coastal-view-residences-going-785000</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/unit-nassim-sold-20-mil</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/unit-nassim-sold-20-mil</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/unit-price-horizon-towers-falls-below-1000-psf</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/unit-price-horizon-towers-falls-below-1000-psf</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/unit-sea-view-fetches-1900-psf</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/unit-sea-view-fetches-1900-psf</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>https://www.edgeprop.sg/property-news/units-nassim-park-residences-cross-3500-psf</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>HTTP error: 429 Client Error: Too Many Requests for url: https://www.edgeprop.sg/property-news/units-nassim-park-residences-cross-3500-psf</t>
+          <t>failed to retrieve content</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
did batch api for 2020 - 2024
</commit_message>
<xml_diff>
--- a/data_cleaning.xlsx
+++ b/data_cleaning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B123"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/freehold-properties-balestier-and-east-coast-sale</t>
+          <t>https://www.edgeprop.sg/property-news/more-optimistic-asia-pacific-market-outlook-2024-says-knight-frank</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/gcb-dalvey-estate-sale-auction-30-mil</t>
+          <t>https://www.edgeprop.sg/property-news/colliers-builds-its-centre-excellence-singapore</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/glimpse-eden-swire-properties%E2%80%99-first-ultra-luxury-condo-singapore</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-sets-higher-benchmarks-targets-super-rich-investors</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/global-citizen-global-investor</t>
+          <t>https://www.edgeprop.sg/property-news/prime-logistics-outperform-other-real-estate-sectors-cbre</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/good-value-city-fringe-living</t>
+          <t>https://www.edgeprop.sg/property-news/29-mil-sq-ft-new-office-space-enter-market-2024-vacancy-rate-expand</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/government-raises-development-charge-rates-non-landed-residential-sector</t>
+          <t>https://www.edgeprop.sg/property-news/outlook-positive-2021-property-market</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ground-floor-strata-fb-space-grand-building-selling-18-mil</t>
+          <t>https://www.edgeprop.sg/property-news/property-market-should-not-run-ahead-economic-fundamentals-dpm-heng</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ground-floor-unit-bukit-timah-shopping-centre-going-58-mil</t>
+          <t>https://www.edgeprop.sg/property-news/fraxtor-offers-investors-opportunity-co-invest-real-estate-little-20000</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/habitap-one-app-rule-them-all</t>
+          <t>https://www.edgeprop.sg/property-news/growth-private-residential-property-prices-slows-07-q-o-q-1q2022</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/hefty-loss-incurred-despite-19-year-holding-period</t>
+          <t>https://www.edgeprop.sg/property-news/bagnall-court-collective-sale-125-mil</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/high-park-residences-hits-right-note-buyers</t>
+          <t>https://www.edgeprop.sg/property-news/analysis-singapore%E2%80%99s-property-cycles-are-less-volatile-compared-other-major-cities</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/high-park-residences-rises-amid-uncertainty</t>
+          <t>https://www.edgeprop.sg/property-news/navigating-real-estate-market-singapore-bali-dubai-japan-and-uk</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/high-specification-industrial-building-paya-lebar-sale</t>
+          <t>https://www.edgeprop.sg/property-news/tj-choo-navigating-industrial-frontier-property-investment</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/hilltops-unit-sold-2397-psf</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-rents-and-prices-post-12th-consecutive-quarter-growth-3q2023</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/house-fortune</t>
+          <t>https://www.edgeprop.sg/property-news/cbre%E2%80%99s-moray-armstrong-sees-%E2%80%98-raft-opportunities%E2%80%99-post-covid-19</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/house-tour-jerome-and-sarahs-charming-home-industrial-style-mezzanine</t>
+          <t>https://www.edgeprop.sg/property-news/ikea-targets-affordable-interior-design-market-singapore-and-southeast-asia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/how-do-mrt-stations-affect-property-prices-and-rent</t>
+          <t>https://www.edgeprop.sg/property-news/five-industrial-units-kaki-bukit-going-64-mil</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/how-has-singapore%E2%80%99s-first-dbss-project-fared-against-resale-hdbs</t>
+          <t>https://www.edgeprop.sg/property-news/five-hdb-shophouses-market-42-mil</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/how-rents-fared-hdb-flats</t>
+          <t>https://www.edgeprop.sg/property-news/navigating-challenges-and-leveraging-insights-dynamic-cold-chain-industry</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/impact-mrt-property-prices</t>
+          <t>https://www.edgeprop.sg/property-news/nus-real-estate-survey-points-improving-market-sentiment-among-industry-leaders</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/industrial-building-tai-seng-sale-23-mil</t>
+          <t>https://www.edgeprop.sg/property-news/b2-industrial-site-gul-lane-sale-48-mil</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/inside-48-mil-copper-house</t>
+          <t>https://www.edgeprop.sg/property-news/boutique-projects-shoring-quality-prices-and-rents-huttons-asia</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ioi-offers-257-billion-central-boulevard-white-site</t>
+          <t>https://www.edgeprop.sg/property-news/orchard-prime-retail-space-sees-strong-take-1q2024-central-area-rents-02-q-o-q</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/iwg-banks-multi-brand-strategy-growth</t>
+          <t>https://www.edgeprop.sg/property-news/cross-border-sources-account-465-singapore%E2%80%99s-inbound-real-estate-investment-1q2024-highest-apac</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/just-sold-caribbean-keppel-bay-unit-sold-145-mil-profit</t>
+          <t>https://www.edgeprop.sg/property-news/japan-continues-growth-streak-even-rest-apac-commercial-property-sales-contracted-1q2024</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/karamjit-singh-leave-jlls-residential-team</t>
+          <t>https://www.edgeprop.sg/property-news/shophouse-sales-value-62-q-o-q-1q2024-propnex-research</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/kingsford-bets-riverfront-location-upper-serangoon-view</t>
+          <t>https://www.edgeprop.sg/property-news/private-home-prices-14-q-o-q-1q2024-even-sentiment-turns-cautious</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/kingsford-waterbay-sells-140-units-launch-weekend</t>
+          <t>https://www.edgeprop.sg/property-news/flight-quality-continues-industrial-property-tenants-flock-limited-high-spec-space</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/landed-homes-below-2-million</t>
+          <t>https://www.edgeprop.sg/property-news/singapore%E2%80%99s-residential-sector-will-be-buyer%E2%80%99s-market-2020-cbre</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/landed-houses-flipped-million-dollar-profits</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-site-loyang-sale-88-mil</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/lawrence-wong-urges-prudence-buyers-and-developers</t>
+          <t>https://www.edgeprop.sg/property-news/covid-19-may-amplify-attractiveness-singapore%E2%80%99s-real-estate-market</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/lian-beng-oxley-launch-strata-titled-industrial-building-tampines</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-ranked-sixth-globally-data-centre-market-competitiveness</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/location-scan-shunfu-ville-collective-sale-whats-its-vicinity</t>
+          <t>https://www.edgeprop.sg/property-news/jtc-launches-two-industrial-gls-sites-1h2020</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/location-scan-sit%E2%80%99s-new-campus-punggol</t>
+          <t>https://www.edgeprop.sg/property-news/glimmers-hope-retail-sector</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -856,7 +856,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/logistics-building-spacetampines-market-170-mil</t>
+          <t>https://www.edgeprop.sg/property-news/how-resilient-demand-high-end-condos</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/lost-decade-sentosa-cove-singapores-billionaire-haven</t>
+          <t>https://www.edgeprop.sg/property-news/private-property-prices-climb-27-2019</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/malls-revitalise-amid-retail-woes</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-tops-asian-outbound-property-investment-2019</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/manhattan-house-collective-sale-300-mil</t>
+          <t>https://www.edgeprop.sg/property-news/iob-building-cecil-street-sale-1800-psf-ppr</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/martin-place-residential-site-fetched-1239-psf-ppr</t>
+          <t>https://www.edgeprop.sg/property-news/jean-yip%E2%80%99s-hair-raising-foray-property-development</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mcc-land-hao-yuan-launched-highest-number-projects-2016</t>
+          <t>https://www.edgeprop.sg/property-news/two-storey-commercial-podium-rise-oxley-going-625-mil</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mcl-land-sells-329-units-parc-esta-average-price-1680-psf</t>
+          <t>https://www.edgeprop.sg/property-news/eleven-commercial-units-balestier-point-sale-68-mil</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/merchants-building-south-bridge-road-collective-sale</t>
+          <t>https://www.edgeprop.sg/property-news/jll-appoints-stuart-ross-head-industrial-and-logistics</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mg-real-estate-unveils-revamped-compass-one</t>
+          <t>https://www.edgeprop.sg/property-news/holland-village-shophouse-market-138-mil</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mix-heritage-and-luxury</t>
+          <t>https://www.edgeprop.sg/property-news/veerasamy-road-freehold-conservation-shophouse-going-52-mil</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mixed-prospects-singapore-property-market</t>
+          <t>https://www.edgeprop.sg/property-news/unit-village-tower-reaps-187-mil-profit</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -988,7 +988,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/mnd-and-hdb-introduced-new-2-room-flexi-scheme</t>
+          <t>https://www.edgeprop.sg/property-news/new-home-sales-2019-jump-156-developers-sell-10164-new-units</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/next-stage-co-working</t>
+          <t>https://www.edgeprop.sg/property-news/dc-rates-dip-02-non-landed-residential-unchanged-other-sectors</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/no-lack-space-10-million-population</t>
+          <t>https://www.edgeprop.sg/property-news/cairnhill-enclave-where-prices-have-outperformed-general-luxury-segment-0</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/north-park-residences-set-benchmark-projects-yishun-19768-0</t>
+          <t>https://www.edgeprop.sg/property-news/snapshot-singapore%E2%80%99s-property-market-2h2020</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1036,7 +1036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/nouvel-18-sells-16-units-90-buyers-are-foreigners</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-properties-tagore-and-bukit-merah-sale</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/oil-tycoon-shifts-focus-real-estate</t>
+          <t>https://www.edgeprop.sg/property-news/commercial-properties-kallang-and-suntec-city-market</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/one-10-transactions-3q2015-were-unprofitable</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-building-macpherson-road-sale-21-mil</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1072,7 +1072,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/one-global-%E2%80%98shaking-%E2%80%99-international-property-marketing-business-singapore</t>
+          <t>https://www.edgeprop.sg/property-news/adjacent-factory-sites-jalan-lembah-kallang-17-mil</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/orchard-road-retail-rents-may-inch-08-y-o-y-year</t>
+          <t>https://www.edgeprop.sg/property-news/two-storey-industrial-building-near-tuas-second-link-sale-8-mil</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/oue-trendsetter</t>
+          <t>https://www.edgeprop.sg/property-news/mortgagee-sale-three-industrial-units-t99-tuas</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/paradise-lost</t>
+          <t>https://www.edgeprop.sg/property-news/commercial-podium-st-michael%E2%80%99s-place-market-25-mil</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/paya-lebar-quarter-%E2%80%94-catalyst-future-commercial-hub</t>
+          <t>https://www.edgeprop.sg/property-news/mixed-use-development-balestier-market-22-mil</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1132,7 +1132,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/pm-lee-announces-new-initiatives-amk-and-sengkang-west</t>
+          <t>https://www.edgeprop.sg/property-news/dc-rates-dip-most-78-hotelhospitality</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1144,7 +1144,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/possible-extension-jurong-region-line-circle-line</t>
+          <t>https://www.edgeprop.sg/property-news/jtc-launches-tender-two-industrial-sites</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/potential-launches-2h2016</t>
+          <t>https://www.edgeprop.sg/property-news/en-bloc-cycle-may-start-2021-huttons</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/price-war-workers%E2%80%99-dormitories</t>
+          <t>https://www.edgeprop.sg/property-news/portfolio-shophouses-and-retail-units-going-333-mil</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/property-auctions-how-low-do-prices-really-go</t>
+          <t>https://www.edgeprop.sg/property-news/possible-land-supply-crunch-2021-0</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/property-bukit-merah</t>
+          <t>https://www.edgeprop.sg/property-news/ground-floor-commercial-unit-bukit-timah-plaza-sale-30-mil</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/property-prices-rise-7-2018</t>
+          <t>https://www.edgeprop.sg/property-news/recognising-singapore%E2%80%99s-top-real-estate-developments-fast-changing-environment</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1216,7 +1216,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/ready-or-not-short-term-rentals-here-stay</t>
+          <t>https://www.edgeprop.sg/property-news/city-developments-%E2%80%98well-attuned-market-trends%E2%80%99</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/real-life-dos-and-donts-property-investing-2462166-0</t>
+          <t>https://www.edgeprop.sg/property-news/sammi-lim-shape-shifter</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/rebirth-swan-maclaren</t>
+          <t>https://www.edgeprop.sg/property-news/uol-group%E2%80%99s-projects-see-good-sales-despite-covid-19</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/recent-ec-launches-20-30-cheaper-new-private-condos</t>
+          <t>https://www.edgeprop.sg/property-news/freight-forwarding-land-transport-fashion-and-real-estate</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1264,7 +1264,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/redevelopment-site-cuscaden-road-170-million</t>
+          <t>https://www.edgeprop.sg/property-news/asia-pacific-real-estate-may-face-market-correction-2021-uli-pwc</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/reinventing-soilbuild-group</t>
+          <t>https://www.edgeprop.sg/property-news/portfolio-17-strata-commercial-units-market-428-million</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1288,7 +1288,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/resale-unit-regency-park-reaps-165-mil-profit</t>
+          <t>https://www.edgeprop.sg/property-news/roxy-pacific-goes-shopping</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1300,7 +1300,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/residential-market-see-spike-new-launches</t>
+          <t>https://www.edgeprop.sg/property-news/four-high-floor-office-units-suntec-tower-two-market-33-mil</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1312,7 +1312,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/retail-units-holland-road-shopping-centre-and-industrial-unit-211-henderson-sale</t>
+          <t>https://www.edgeprop.sg/property-news/city-developments%E2%80%99-kaleidoscope-projects</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/revitalising-potong-pasir%E2%80%99s-private-property-market</t>
+          <t>https://www.edgeprop.sg/property-news/perennial-real-estate-holdings-acquires-big-box-118-mil</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/revival-sales-sentosa-cove-bungalows</t>
+          <t>https://www.edgeprop.sg/property-news/four-freehold-conservation-shophouses-tiong-bahru-sale-50-mil</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1348,7 +1348,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/richard-jany-weathering-ups-and-downs</t>
+          <t>https://www.edgeprop.sg/property-news/three-conservation-shophouses-jalan-sultan-market-938-mil</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/roxy-pacific%E2%80%99s-overseas-gambit</t>
+          <t>https://www.edgeprop.sg/property-news/corner-shophouse-new-bridge-road-sale-169-mil</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1372,7 +1372,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/safdie%E2%80%99s-%E2%80%98step-pyramid%E2%80%99-bishan</t>
+          <t>https://www.edgeprop.sg/property-news/freehold-strata-titled-development-50-tagore-lane-sale-100-mil</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1384,7 +1384,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/sales-mon-jervois-pick-after-completion</t>
+          <t>https://www.edgeprop.sg/property-news/mirror-city</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1396,7 +1396,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/savills-singapore-launches-business-valuation-advisory-team</t>
+          <t>https://www.edgeprop.sg/property-news/lessons-2-new-condo-launches</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/sentosa-cove-condo-changed-hands-1368-psf</t>
+          <t>https://www.edgeprop.sg/property-news/real-estate-investments-115-q-o-q-1q2021-led-residential</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/shophouse-holland-avenue-sale</t>
+          <t>https://www.edgeprop.sg/property-news/suntec-city-office-floors-sold-197-mil</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1432,7 +1432,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/shophouses-kampong-glam-and-little-india-poised-be-next-growth-area</t>
+          <t>https://www.edgeprop.sg/property-news/297-m-o-m-fall-may-new-home-sales-%E2%80%98temporary-setback%E2%80%99</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1444,7 +1444,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/shophouses-ripe-picking</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-development-loyang-drive-sale-25-mil</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/shophouses-upper-east-coast-road-tanjong-katong-road-and-jalan-besar-sale</t>
+          <t>https://www.edgeprop.sg/property-news/lhn-group-records-net-profit-153-mil-1h2021</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1468,7 +1468,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/signature-yishun-open-applications-polling-day</t>
+          <t>https://www.edgeprop.sg/property-news/four-factories-mandai-sale-72-mil</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/sim-lian-launch-and-lease-200000-sq-ft-office-space-vision-exchange</t>
+          <t>https://www.edgeprop.sg/property-news/projects-completing-between-now-and-2023-what-look-out</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-evolves-so-does-edgeprop</t>
+          <t>https://www.edgeprop.sg/property-news/real-estate-investment-deals-singapore-amount-38-bil-1q2021-knight-frank</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-has-best-prospects-investment-asia-pacific</t>
+          <t>https://www.edgeprop.sg/property-news/high-street-centre-launches-second-collective-sale-tender</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-home-prices-have-bottomed-hong-kongs-are-%E2%80%98crazy%E2%80%99-bnp</t>
+          <t>https://www.edgeprop.sg/property-news/park-nova-tomlinson-road-preview-may-1</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1528,7 +1528,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-investors-snap-us5-billion-chinas-commercial-properties-brushing-aside-trade-war-concerns</t>
+          <t>https://www.edgeprop.sg/property-news/cdl-sells-over-50-units-irwell-hill-residences-launch-weekend</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/singapore-shopping-centre-launched-collective-sale-255-mil</t>
+          <t>https://www.edgeprop.sg/property-news/office-chinatown-point-sale-446-mil</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/singaporeans-are-loving-luxury-homes-foreigners-cant-buy</t>
+          <t>https://www.edgeprop.sg/property-news/gls-sites-lentor-central-and-tampines-street-62-tender</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1564,7 +1564,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/slb-development-looks-new-horizons</t>
+          <t>https://www.edgeprop.sg/property-news/hdb-executive-maisonette-ang-mo-kio-market-999999</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/slower-sales-and-launches-due-june-holidays</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-site-8b-buroh-street-sale-22-mil</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/sri5000-splits-slp-international</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-prime-office-rental-market-bottoms-out-3q2021-rents-climb-02-q-o-q</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1600,7 +1600,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/stamp-duty-common-mistakes-avoid</t>
+          <t>https://www.edgeprop.sg/property-news/cbd-grade-office-vacancy-rate-46-2q2021-highest-1q2018-cw</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1612,7 +1612,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/stars-kovan-star-qualities</t>
+          <t>https://www.edgeprop.sg/property-news/office-rents-breakout-or-rebound</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/stars-kovan-unveiled</t>
+          <t>https://www.edgeprop.sg/property-news/lhn-group-buys-industrial-complex-tuas-21-mil</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/steady-stream-well-heeled-visitors-meyer-mansion-preview-weekend</t>
+          <t>https://www.edgeprop.sg/property-news/value-buys-week-%E2%80%93-july-30-2021</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1648,7 +1648,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/strata-office-space-faces-stiff-competition</t>
+          <t>https://www.edgeprop.sg/property-news/era-launches-app-showcasing-property-market-insights-and-trend</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/sultan-plaza-collective-sale-380-mil</t>
+          <t>https://www.edgeprop.sg/property-news/demand-pushes-occupancy-high-specs-industrial-space-near-full-capacity-2021</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/superbowl-jurong-sale-20-million</t>
+          <t>https://www.edgeprop.sg/property-news/warehouse-rents-17-3q2021-%E2%80%93-highest-quarterly-growth-eight-years</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1684,7 +1684,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/surge-top-end-prices-2018</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-building-changi-south-street-sale-12mil</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1696,7 +1696,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/tanjong-pagar-new-waterfront-city</t>
+          <t>https://www.edgeprop.sg/property-news/stellar-housing-market-ends-year-shadow-cooling-measures-and-omicron</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1708,7 +1708,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/tanjong-rhu%E2%80%99s-draws-%E2%80%94-city-fringe-location-waterfront-views</t>
+          <t>https://www.edgeprop.sg/property-news/nascent-life-sciences-real-estate-market-asia-pacific-needs-more-data-sharing-grow-uli</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1720,7 +1720,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/teambuild-land-pares-down-property-development-business</t>
+          <t>https://www.edgeprop.sg/property-news/freehold-commercial-building-near-farrer-park-market-235-mil</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/teho-backs-out-macpherson-deal</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-rents-increased-sixth-straight-quarter-1q2022</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1744,7 +1744,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/thong-sia-building-sold-380-million-largest-ever-mixed-use-collective-sale</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-sales-and-leasing-activities-rise-49-y-o-y-1q-knight-frank</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/three-balestier-road-shophouses-going-95-mil</t>
+          <t>https://www.edgeprop.sg/property-news/leasehold-industrial-building-ang-mo-kio-sale-27-mil</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1768,7 +1768,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/three-generations-enjoy-privacy-under-one-roo</t>
+          <t>https://www.edgeprop.sg/property-news/singapore-office-market-recovery-well-underway-colliers</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1780,7 +1780,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/three-landed-homes-sold-3-mil-profit</t>
+          <t>https://www.edgeprop.sg/property-news/market-stabilising-four-months-after-property-cooling-measures</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1792,7 +1792,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/three-office-units-peninsular-plaza-going-929-mil</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-building-kung-chong-road-sale-19-mil</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1804,7 +1804,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/three-storey-conservation-shophouse-chinatown-sale-85-mil</t>
+          <t>https://www.edgeprop.sg/property-news/good-time-invest-prime-property-core-central-region</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -1816,7 +1816,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/top-gainer-makes-record-169-mil-profit-watermark-robertson-quay</t>
+          <t>https://www.edgeprop.sg/property-news/private-home-prices-see-sharp-slowdown-growth-04-1q2022-ura-flash-estimates</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1828,7 +1828,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/trouble-paradise</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-rents-15-2q2022-charting-seventh-consecutive-quarter-growth</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/two-freehold-commercial-shophouses-sale</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-property-jalan-lembah-kallang-sale-75-mil</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1852,7 +1852,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/under-hammer-unit-coastal-view-residences-going-785000</t>
+          <t>https://www.edgeprop.sg/property-news/strata-industrial-unit-delta-house-market-sale-and-leaseback-30-mil</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/unit-nassim-sold-20-mil</t>
+          <t>https://www.edgeprop.sg/property-news/strata-office-market-records-3651-mil-sales-1h2022-investors-eye-en-bloc-potential</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1876,7 +1876,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/unit-price-horizon-towers-falls-below-1000-psf</t>
+          <t>https://www.edgeprop.sg/property-news/commercial-siakson-building-market-30-mil</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -1888,7 +1888,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/unit-sea-view-fetches-1900-psf</t>
+          <t>https://www.edgeprop.sg/property-news/industrial-building-tuas-market-68-mil</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -1900,10 +1900,358 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>https://www.edgeprop.sg/property-news/units-nassim-park-residences-cross-3500-psf</t>
+          <t>https://www.edgeprop.sg/property-news/metro-holdings-and-boustead-projects-announce-joint-acquisition-industrial-property-tai-seng-988-mi</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/savills-real-estate-investment-volume-totals-247-bil-2022-down-1-y-o-y</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/singapore-real-estate-market-remain-bright-spot-savills</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/freehold-industrial-building-new-industrial-road-sale</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/2022-apac-real-estate-investments-down-27-y-o-y-rate-hikes-cooling-sentiment-jll</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/am-alpha%E2%80%99s-timing-driven-value-add-real-estate-play</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/shophouse-market-sentiment-turned-cautious-2h2022-knight-frank</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/demand-still-apparent-office-market-despite-global-setbacks-knight-frank</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/industrial-building-yishun-sale-192-mil</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/list-current-en-bloc-developments-and-their-likelihood-success</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/banking-crisis-how-will-real-estate-capital-markets-be-hit</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/singapore-office-rents-see-subdued-growth-1q2023-jll</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/industrial-rents-climb-15-1q2023-new-supply-erodes-occupancy-88</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/higher-supply-industrial-sites-available-under-2h2023-gls-programme</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/supply-driven-office-market-sustain-singapore%E2%80%99s-10-year-usage</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/freehold-industrial-land-kim-chuan-lane-sale-43-mil</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/slow-start-2023-real-estate-investment-sales-amid-market-uncertainties-knight-frank</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/sevens-atelier-purchase-industrial-building-60-bendemeer-road-415-mil</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/real-estate-sector-shows-significant-bounce-back-investment-sales-1q2023-savills</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/servicing-high-net-worth-deep-market-knowledge-key</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/asia-pacific-real-estate-investments-down-30-y-o-y-1q2023-jll</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/climate-controlled-industrial-facility-60-tuas-ave-11-market-50-mil</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/office-rents-grow-sixth-consecutive-quarter-51-1q2023</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/smartisan-development-buys-two-freehold-industrial-sites-mandai-estate-100-million</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/capitaland-ascendas-reit-divests-local-industrial-building-219-premium-2005-purchase-price</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/fewer-commercial-shophouse-sales-1q2023-shophouse-rental-market-remains-brisk-propnex</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/analysis-are-current-asking-prices-unrealistic</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/three-freehold-jalan-besar-shophouses-market-30-mil</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/singapore-property-buying-sentiment-slides-1q2023-amid-high-interest-rates-and-cooling-measures-nus</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>failed to retrieve content</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>https://www.edgeprop.sg/property-news/56-units-sold-ct-foodnex-launch-underscores-demand-food-factories</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
         <is>
           <t>failed to retrieve content</t>
         </is>

</xml_diff>